<commit_message>
Commit merge cho Sáng
</commit_message>
<xml_diff>
--- a/Documents/TaskMember.xlsx
+++ b/Documents/TaskMember.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceGit\BusBooking_Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A6C101-8C19-441E-8B9D-A505F9C4A0B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A210E1-D37E-4B9D-B7CA-12D5AC4A7F67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="394" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="302" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Task Member</t>
   </si>
@@ -173,6 +173,9 @@
   <si>
     <t>Tìm kiếm giao diện(table có phân trang, sort) cho bảng giá. Có thể tham khảo ở Phương Trang mụn lịch trình</t>
   </si>
+  <si>
+    <t>Note: Mọi người code và làm xong Task thì push lúc 20h và nhớ thông báo nha !!!</t>
+  </si>
 </sst>
 </file>
 
@@ -203,9 +206,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -405,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -564,372 +570,261 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -939,59 +834,176 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1253,15 +1265,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>393612</xdr:colOff>
+          <xdr:colOff>396240</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>184194</xdr:rowOff>
+          <xdr:rowOff>182880</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>27852</xdr:colOff>
+          <xdr:colOff>30480</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>22598</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1271,7 +1283,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0700350-208A-4080-AB67-4B083FDB7C11}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1320,15 +1332,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>25</xdr:col>
-          <xdr:colOff>480323</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>194441</xdr:rowOff>
+          <xdr:rowOff>198120</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>114563</xdr:colOff>
+          <xdr:colOff>114300</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>32846</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1338,7 +1350,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A07D0CE-13BF-40AC-9288-E32839FD4CC2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1387,15 +1399,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>517109</xdr:colOff>
+          <xdr:colOff>518160</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>199696</xdr:rowOff>
+          <xdr:rowOff>198120</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>151349</xdr:colOff>
+          <xdr:colOff>152400</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>38101</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1405,7 +1417,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD4CE5F-0F09-445F-867A-D47F9B06A24E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1454,15 +1466,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>390985</xdr:colOff>
+          <xdr:colOff>388620</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>94594</xdr:rowOff>
+          <xdr:rowOff>91440</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>25225</xdr:colOff>
+          <xdr:colOff>22860</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>132693</xdr:rowOff>
+          <xdr:rowOff>129540</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1472,7 +1484,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4C678AF-5EDD-462E-840B-1FEA55158E2A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1521,15 +1533,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>25</xdr:col>
-          <xdr:colOff>474805</xdr:colOff>
+          <xdr:colOff>472440</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>109834</xdr:rowOff>
+          <xdr:rowOff>106680</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>109045</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>140313</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1539,7 +1551,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72A3D8C3-4E18-430D-BEFA-C2616AB212D1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1588,15 +1600,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>512905</xdr:colOff>
+          <xdr:colOff>510540</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>109834</xdr:rowOff>
+          <xdr:rowOff>106680</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>147145</xdr:colOff>
+          <xdr:colOff>144780</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>147933</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1606,7 +1618,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB304168-1633-47A4-9F38-D33F5BF4DC9C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1673,7 +1685,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{565A90A0-30BF-449C-88A5-89ACBAC502E1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1740,7 +1752,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05D62D4A-E0F0-4A1E-9FB8-B409F6211DF1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1807,7 +1819,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31A9FDEB-2761-47EC-AF56-95EA93078E06}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1874,7 +1886,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0545230B-FFFB-48CB-B00B-15589487C32C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1941,7 +1953,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2725FB69-AFBA-4432-8B9E-A3D73AE4F0E4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2008,7 +2020,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D47759F-7DC5-4B3B-85EC-DA6AFE5B4D53}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2059,13 +2071,13 @@
           <xdr:col>23</xdr:col>
           <xdr:colOff>396240</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>35859</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
           <xdr:colOff>30480</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>73959</xdr:rowOff>
+          <xdr:rowOff>76199</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2075,7 +2087,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6B49DF3-8A1A-492A-9446-70F8AE633ECE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2126,13 +2138,13 @@
           <xdr:col>25</xdr:col>
           <xdr:colOff>480060</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>51099</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
           <xdr:colOff>114300</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>81579</xdr:rowOff>
+          <xdr:rowOff>83819</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2142,7 +2154,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F086ABD4-FA2F-4BBF-9546-DC8F5E4704AD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2193,13 +2205,13 @@
           <xdr:col>27</xdr:col>
           <xdr:colOff>518160</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>51099</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>89199</xdr:rowOff>
+          <xdr:rowOff>91439</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2209,7 +2221,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD437B70-EF32-4891-AA19-88960918827F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2260,13 +2272,13 @@
           <xdr:col>23</xdr:col>
           <xdr:colOff>396240</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>35859</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
           <xdr:colOff>30480</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>73958</xdr:rowOff>
+          <xdr:rowOff>76201</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2276,7 +2288,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{580B6AE1-7DBC-40A1-A17A-F0DDDE172C2C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2327,13 +2339,13 @@
           <xdr:col>25</xdr:col>
           <xdr:colOff>480060</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>51099</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
           <xdr:colOff>114300</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>81578</xdr:rowOff>
+          <xdr:rowOff>83821</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2343,7 +2355,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D642C4E-D785-4516-9339-EEF9862A696B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2394,13 +2406,13 @@
           <xdr:col>27</xdr:col>
           <xdr:colOff>518160</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>51099</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>89198</xdr:rowOff>
+          <xdr:rowOff>91441</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2410,7 +2422,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{565BB990-297D-4907-9628-23610029C5E6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2459,15 +2471,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>431650</xdr:colOff>
+          <xdr:colOff>434340</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>62753</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>65890</xdr:colOff>
+          <xdr:colOff>68580</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>100853</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2477,7 +2489,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30D2339B-E5FE-47B8-ACDC-FC6CA948CA65}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2526,15 +2538,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>25</xdr:col>
-          <xdr:colOff>515470</xdr:colOff>
+          <xdr:colOff>518160</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>77993</xdr:rowOff>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>149710</xdr:colOff>
+          <xdr:colOff>152400</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>108473</xdr:rowOff>
+          <xdr:rowOff>106680</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2544,7 +2556,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00BD6ECA-34CC-4A32-B4A1-B6F256D5A0E7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2593,15 +2605,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>553570</xdr:colOff>
+          <xdr:colOff>556260</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>77993</xdr:rowOff>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>187810</xdr:colOff>
+          <xdr:colOff>190500</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>116093</xdr:rowOff>
+          <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2611,7 +2623,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{608C68BF-E7EB-41F2-884E-F014728A3410}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2662,13 +2674,13 @@
           <xdr:col>23</xdr:col>
           <xdr:colOff>449580</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>53788</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>91888</xdr:rowOff>
+          <xdr:rowOff>91440</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2678,7 +2690,7 @@
                   <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10F60E63-9D73-41CE-B1C2-6E734EC16103}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2729,13 +2741,13 @@
           <xdr:col>25</xdr:col>
           <xdr:colOff>533400</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>69028</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
           <xdr:colOff>167640</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>99508</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2745,7 +2757,7 @@
                   <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBF8C4A9-14E2-4E49-9196-5677F521946F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2796,13 +2808,13 @@
           <xdr:col>27</xdr:col>
           <xdr:colOff>571500</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>69028</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
           <xdr:colOff>205740</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>107128</xdr:rowOff>
+          <xdr:rowOff>106680</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2812,7 +2824,7 @@
                   <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61FE1948-ED70-4527-A528-FE5E747FB8D3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2879,7 +2891,7 @@
                   <a14:compatExt spid="_x0000_s1049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8145C35-D925-473F-A856-B05E0F9A25FB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2946,7 +2958,7 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EA9AC5D-C451-4AB8-9CD0-0B789AACD390}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3013,7 +3025,7 @@
                   <a14:compatExt spid="_x0000_s1051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA795F17-ACC8-4E77-A0AF-906D7ADB40FE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3070,7 +3082,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>38101</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3080,7 +3092,7 @@
                   <a14:compatExt spid="_x0000_s1052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9A19D7D-0ED1-485A-B0F4-4368B216D663}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3137,7 +3149,7 @@
           <xdr:col>26</xdr:col>
           <xdr:colOff>167640</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>45720</xdr:rowOff>
+          <xdr:rowOff>45721</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3147,7 +3159,7 @@
                   <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F7A192C-B81B-49E2-8174-CFA7B1C04D2D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3204,7 +3216,7 @@
           <xdr:col>28</xdr:col>
           <xdr:colOff>205740</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>53340</xdr:rowOff>
+          <xdr:rowOff>53341</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3214,7 +3226,7 @@
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{580CC0B8-DAD4-4038-AD39-E0973AA12591}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3281,7 +3293,7 @@
                   <a14:compatExt spid="_x0000_s1055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B947A8B-5136-41D7-A8DA-51CE6D67B094}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3348,7 +3360,7 @@
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9848089-0F6C-413B-85CE-8D0206FF207A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3415,7 +3427,7 @@
                   <a14:compatExt spid="_x0000_s1057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC95344E-5B7A-422A-8DBD-9101969D8114}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3482,7 +3494,7 @@
                   <a14:compatExt spid="_x0000_s1058"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E6347FE-2D12-47C4-BCDB-FFBA0E6332C2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3549,7 +3561,7 @@
                   <a14:compatExt spid="_x0000_s1059"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{699142B5-74D2-4B6B-AFFD-85D186695B7C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3616,7 +3628,7 @@
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3105C08-B9EB-4F14-B711-F8A06E363A2A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3683,7 +3695,7 @@
                   <a14:compatExt spid="_x0000_s1061"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{735FED20-A8C7-41C2-AED7-B32BEBFDFEC7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3750,7 +3762,7 @@
                   <a14:compatExt spid="_x0000_s1062"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B99D4927-075A-48BC-9F90-F217F1B94292}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3817,7 +3829,7 @@
                   <a14:compatExt spid="_x0000_s1063"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09E88598-4747-4FAA-A80C-82B144E52454}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3884,7 +3896,7 @@
                   <a14:compatExt spid="_x0000_s1064"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2AF2192-D251-4C55-A9C4-3AC935DB75B6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3951,7 +3963,7 @@
                   <a14:compatExt spid="_x0000_s1065"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E1BAC7-C9A6-456B-BB69-465FDD1CCAD3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4018,7 +4030,7 @@
                   <a14:compatExt spid="_x0000_s1066"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B883FFF5-FB83-4167-9831-3116200EE138}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4085,7 +4097,7 @@
                   <a14:compatExt spid="_x0000_s1067"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF740F6C-8714-448B-A12B-A53D0B2986B5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4152,7 +4164,7 @@
                   <a14:compatExt spid="_x0000_s1068"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B8C0DD1-8CB4-45D5-8B94-6EA174690B35}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4219,7 +4231,7 @@
                   <a14:compatExt spid="_x0000_s1069"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C86C7207-DF36-4179-A861-73F3EF71D20C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4286,7 +4298,7 @@
                   <a14:compatExt spid="_x0000_s1070"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD228635-7E28-4BB7-8596-D6CF90080E3A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4353,7 +4365,7 @@
                   <a14:compatExt spid="_x0000_s1071"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA7A066-D1A2-4FA8-AA78-EAC233A02E01}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4420,7 +4432,7 @@
                   <a14:compatExt spid="_x0000_s1072"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA5E7A6D-4C53-4359-9334-51AA11E83BAC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4487,7 +4499,7 @@
                   <a14:compatExt spid="_x0000_s1073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5111AD54-F2DE-4860-8EE5-06AC7C60F82A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4554,7 +4566,7 @@
                   <a14:compatExt spid="_x0000_s1074"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F745DED9-4B53-4D2D-A452-6C7EB443BE8C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4621,7 +4633,7 @@
                   <a14:compatExt spid="_x0000_s1075"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75D051A8-7F6C-4747-B03A-B1FDB1CDEB77}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4670,15 +4682,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>458545</xdr:colOff>
+          <xdr:colOff>457200</xdr:colOff>
           <xdr:row>42</xdr:row>
-          <xdr:rowOff>26894</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>92785</xdr:colOff>
+          <xdr:colOff>91440</xdr:colOff>
           <xdr:row>43</xdr:row>
-          <xdr:rowOff>64994</xdr:rowOff>
+          <xdr:rowOff>68581</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4688,7 +4700,7 @@
                   <a14:compatExt spid="_x0000_s1076"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AE153CB-A346-477A-AEEF-2AECAE85A4BA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4737,15 +4749,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>25</xdr:col>
-          <xdr:colOff>542365</xdr:colOff>
+          <xdr:colOff>541020</xdr:colOff>
           <xdr:row>42</xdr:row>
-          <xdr:rowOff>42134</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>176605</xdr:colOff>
+          <xdr:colOff>175260</xdr:colOff>
           <xdr:row>43</xdr:row>
-          <xdr:rowOff>72614</xdr:rowOff>
+          <xdr:rowOff>76201</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4755,7 +4767,7 @@
                   <a14:compatExt spid="_x0000_s1077"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFBDABA7-4EDB-4560-ABEC-248C4992AE3D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4804,15 +4816,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>580465</xdr:colOff>
+          <xdr:colOff>579120</xdr:colOff>
           <xdr:row>42</xdr:row>
-          <xdr:rowOff>42134</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>214705</xdr:colOff>
+          <xdr:colOff>213360</xdr:colOff>
           <xdr:row>43</xdr:row>
-          <xdr:rowOff>80234</xdr:rowOff>
+          <xdr:rowOff>83821</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4822,7 +4834,7 @@
                   <a14:compatExt spid="_x0000_s1078"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80A65728-07C2-46AF-82B4-7E0563FE3D9B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000036040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4873,13 +4885,13 @@
           <xdr:col>23</xdr:col>
           <xdr:colOff>449580</xdr:colOff>
           <xdr:row>45</xdr:row>
-          <xdr:rowOff>71718</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>46</xdr:row>
-          <xdr:rowOff>109818</xdr:rowOff>
+          <xdr:rowOff>106680</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4889,7 +4901,7 @@
                   <a14:compatExt spid="_x0000_s1079"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FEB1FE9-29F3-47C7-B593-397790A5C290}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4940,13 +4952,13 @@
           <xdr:col>25</xdr:col>
           <xdr:colOff>533400</xdr:colOff>
           <xdr:row>45</xdr:row>
-          <xdr:rowOff>86958</xdr:rowOff>
+          <xdr:rowOff>83820</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
           <xdr:colOff>167640</xdr:colOff>
           <xdr:row>46</xdr:row>
-          <xdr:rowOff>117438</xdr:rowOff>
+          <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4956,7 +4968,7 @@
                   <a14:compatExt spid="_x0000_s1080"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{798B8A62-4833-4E77-ADDE-E62257C1586E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5007,13 +5019,13 @@
           <xdr:col>27</xdr:col>
           <xdr:colOff>571500</xdr:colOff>
           <xdr:row>45</xdr:row>
-          <xdr:rowOff>86958</xdr:rowOff>
+          <xdr:rowOff>83820</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
           <xdr:colOff>205740</xdr:colOff>
           <xdr:row>46</xdr:row>
-          <xdr:rowOff>125058</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5023,7 +5035,7 @@
                   <a14:compatExt spid="_x0000_s1081"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{749F3CE8-B875-407E-A982-8C84DC5BF770}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5335,8 +5347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AC60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18:Y19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5344,1233 +5356,1252 @@
     <col min="2" max="2" width="5.21875" customWidth="1"/>
     <col min="3" max="3" width="5.77734375" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
     <col min="15" max="15" width="8.109375" customWidth="1"/>
-    <col min="16" max="19" width="8.88671875" style="214"/>
+    <col min="16" max="19" width="8.88671875" style="77"/>
     <col min="20" max="20" width="11.88671875" customWidth="1"/>
     <col min="25" max="25" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="21" x14ac:dyDescent="0.4">
-      <c r="H2" s="173" t="s">
+      <c r="H2" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="173"/>
-      <c r="J2" s="173"/>
-      <c r="K2" s="173"/>
-      <c r="L2" s="173"/>
-      <c r="M2" s="173"/>
-      <c r="N2" s="173"/>
-      <c r="O2" s="173"/>
-      <c r="P2" s="173"/>
-      <c r="Q2" s="173"/>
-      <c r="R2" s="173"/>
-      <c r="S2" s="173"/>
-      <c r="T2" s="173"/>
-      <c r="U2" s="173"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
+    </row>
+    <row r="4" spans="2:29" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="H4" s="216" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="215"/>
+      <c r="J4" s="215"/>
+      <c r="K4" s="215"/>
+      <c r="L4" s="215"/>
+      <c r="M4" s="215"/>
+      <c r="N4" s="215"/>
+      <c r="O4" s="215"/>
+      <c r="P4" s="215"/>
+      <c r="Q4" s="215"/>
+      <c r="R4" s="215"/>
+      <c r="S4" s="215"/>
+      <c r="T4" s="215"/>
+      <c r="U4" s="215"/>
     </row>
     <row r="5" spans="2:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="154" t="s">
+      <c r="B5" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="155"/>
-      <c r="D5" s="156" t="s">
+      <c r="C5" s="143"/>
+      <c r="D5" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="157"/>
-      <c r="F5" s="157"/>
-      <c r="G5" s="157"/>
-      <c r="H5" s="157"/>
-      <c r="I5" s="158"/>
-      <c r="J5" s="168" t="s">
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="169"/>
-      <c r="L5" s="150" t="s">
+      <c r="K5" s="145"/>
+      <c r="L5" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="151"/>
-      <c r="N5" s="150" t="s">
+      <c r="M5" s="98"/>
+      <c r="N5" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="151"/>
-      <c r="P5" s="205" t="s">
+      <c r="O5" s="98"/>
+      <c r="P5" s="137" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" s="206"/>
-      <c r="R5" s="206"/>
-      <c r="S5" s="207"/>
-      <c r="T5" s="152" t="s">
+      <c r="Q5" s="138"/>
+      <c r="R5" s="138"/>
+      <c r="S5" s="139"/>
+      <c r="T5" s="140" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="153"/>
-      <c r="V5" s="153"/>
-      <c r="W5" s="153"/>
-      <c r="X5" s="175" t="s">
+      <c r="U5" s="141"/>
+      <c r="V5" s="141"/>
+      <c r="W5" s="141"/>
+      <c r="X5" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="Y5" s="176"/>
-      <c r="Z5" s="177" t="s">
+      <c r="Y5" s="96"/>
+      <c r="Z5" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="AA5" s="176"/>
-      <c r="AB5" s="175" t="s">
+      <c r="AA5" s="96"/>
+      <c r="AB5" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="AC5" s="176"/>
+      <c r="AC5" s="96"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="198" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="165" t="s">
+      <c r="C6" s="199"/>
+      <c r="D6" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="166"/>
-      <c r="F6" s="166"/>
-      <c r="G6" s="166"/>
-      <c r="H6" s="166"/>
-      <c r="I6" s="167"/>
-      <c r="J6" s="80" t="s">
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="106"/>
+      <c r="J6" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="81"/>
-      <c r="L6" s="192">
+      <c r="K6" s="101"/>
+      <c r="L6" s="93">
         <v>43981</v>
       </c>
-      <c r="M6" s="174"/>
-      <c r="N6" s="192">
+      <c r="M6" s="94"/>
+      <c r="N6" s="93">
         <v>43981</v>
       </c>
-      <c r="O6" s="174"/>
+      <c r="O6" s="94"/>
       <c r="P6" s="60"/>
       <c r="Q6" s="60"/>
       <c r="R6" s="60"/>
       <c r="S6" s="60"/>
-      <c r="T6" s="113"/>
-      <c r="U6" s="114"/>
-      <c r="V6" s="114"/>
-      <c r="W6" s="115"/>
-      <c r="X6" s="178"/>
-      <c r="Y6" s="179"/>
-      <c r="Z6" s="178"/>
-      <c r="AA6" s="179"/>
-      <c r="AB6" s="178"/>
-      <c r="AC6" s="179"/>
+      <c r="T6" s="160"/>
+      <c r="U6" s="161"/>
+      <c r="V6" s="161"/>
+      <c r="W6" s="162"/>
+      <c r="X6" s="90"/>
+      <c r="Y6" s="91"/>
+      <c r="Z6" s="90"/>
+      <c r="AA6" s="91"/>
+      <c r="AB6" s="90"/>
+      <c r="AC6" s="91"/>
     </row>
     <row r="7" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="70"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="122" t="s">
+      <c r="B7" s="200"/>
+      <c r="C7" s="201"/>
+      <c r="D7" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="193">
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="146">
         <v>43982</v>
       </c>
-      <c r="M7" s="108"/>
-      <c r="N7" s="107"/>
-      <c r="O7" s="108"/>
+      <c r="M7" s="147"/>
+      <c r="N7" s="150"/>
+      <c r="O7" s="147"/>
       <c r="P7" s="62"/>
       <c r="Q7" s="62"/>
       <c r="R7" s="62"/>
       <c r="S7" s="62"/>
-      <c r="T7" s="116"/>
-      <c r="U7" s="117"/>
-      <c r="V7" s="117"/>
-      <c r="W7" s="118"/>
-      <c r="X7" s="186"/>
-      <c r="Y7" s="187"/>
-      <c r="Z7" s="186"/>
-      <c r="AA7" s="187"/>
-      <c r="AB7" s="186"/>
-      <c r="AC7" s="187"/>
+      <c r="T7" s="163"/>
+      <c r="U7" s="164"/>
+      <c r="V7" s="164"/>
+      <c r="W7" s="165"/>
+      <c r="X7" s="78"/>
+      <c r="Y7" s="79"/>
+      <c r="Z7" s="78"/>
+      <c r="AA7" s="79"/>
+      <c r="AB7" s="78"/>
+      <c r="AC7" s="79"/>
     </row>
     <row r="8" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B8" s="70"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="111"/>
-      <c r="M8" s="112"/>
-      <c r="N8" s="111"/>
-      <c r="O8" s="112"/>
+      <c r="B8" s="200"/>
+      <c r="C8" s="201"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="148"/>
+      <c r="M8" s="149"/>
+      <c r="N8" s="148"/>
+      <c r="O8" s="149"/>
       <c r="P8" s="61"/>
       <c r="Q8" s="61"/>
       <c r="R8" s="61"/>
       <c r="S8" s="61"/>
-      <c r="T8" s="119"/>
-      <c r="U8" s="120"/>
-      <c r="V8" s="120"/>
-      <c r="W8" s="121"/>
-      <c r="X8" s="190"/>
-      <c r="Y8" s="191"/>
-      <c r="Z8" s="190"/>
-      <c r="AA8" s="191"/>
-      <c r="AB8" s="190"/>
-      <c r="AC8" s="191"/>
+      <c r="T8" s="166"/>
+      <c r="U8" s="167"/>
+      <c r="V8" s="167"/>
+      <c r="W8" s="168"/>
+      <c r="X8" s="80"/>
+      <c r="Y8" s="81"/>
+      <c r="Z8" s="80"/>
+      <c r="AA8" s="81"/>
+      <c r="AB8" s="80"/>
+      <c r="AC8" s="81"/>
     </row>
     <row r="9" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="70"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="122" t="s">
+      <c r="B9" s="200"/>
+      <c r="C9" s="201"/>
+      <c r="D9" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="80" t="s">
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="108"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="81"/>
+      <c r="K9" s="101"/>
       <c r="L9" s="57"/>
       <c r="M9" s="54"/>
       <c r="N9" s="57"/>
       <c r="O9" s="54"/>
-      <c r="P9" s="141" t="s">
+      <c r="P9" s="169" t="s">
         <v>28</v>
       </c>
-      <c r="Q9" s="142"/>
-      <c r="R9" s="142"/>
-      <c r="S9" s="143"/>
-      <c r="T9" s="113"/>
-      <c r="U9" s="114"/>
-      <c r="V9" s="114"/>
-      <c r="W9" s="115"/>
-      <c r="X9" s="186"/>
-      <c r="Y9" s="187"/>
-      <c r="Z9" s="186"/>
-      <c r="AA9" s="187"/>
-      <c r="AB9" s="186"/>
-      <c r="AC9" s="187"/>
+      <c r="Q9" s="170"/>
+      <c r="R9" s="170"/>
+      <c r="S9" s="171"/>
+      <c r="T9" s="160"/>
+      <c r="U9" s="161"/>
+      <c r="V9" s="161"/>
+      <c r="W9" s="162"/>
+      <c r="X9" s="78"/>
+      <c r="Y9" s="79"/>
+      <c r="Z9" s="78"/>
+      <c r="AA9" s="79"/>
+      <c r="AB9" s="78"/>
+      <c r="AC9" s="79"/>
     </row>
     <row r="10" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="70"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="132"/>
-      <c r="H10" s="132"/>
-      <c r="I10" s="133"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="83"/>
+      <c r="B10" s="200"/>
+      <c r="C10" s="201"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="126"/>
+      <c r="F10" s="126"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="126"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="123"/>
+      <c r="K10" s="124"/>
       <c r="L10" s="58"/>
       <c r="M10" s="59"/>
       <c r="N10" s="58"/>
       <c r="O10" s="59"/>
-      <c r="P10" s="144"/>
-      <c r="Q10" s="145"/>
-      <c r="R10" s="145"/>
-      <c r="S10" s="146"/>
-      <c r="T10" s="116"/>
-      <c r="U10" s="117"/>
-      <c r="V10" s="117"/>
-      <c r="W10" s="118"/>
-      <c r="X10" s="188"/>
-      <c r="Y10" s="189"/>
-      <c r="Z10" s="188"/>
-      <c r="AA10" s="189"/>
-      <c r="AB10" s="188"/>
-      <c r="AC10" s="189"/>
+      <c r="P10" s="172"/>
+      <c r="Q10" s="173"/>
+      <c r="R10" s="173"/>
+      <c r="S10" s="174"/>
+      <c r="T10" s="163"/>
+      <c r="U10" s="164"/>
+      <c r="V10" s="164"/>
+      <c r="W10" s="165"/>
+      <c r="X10" s="82"/>
+      <c r="Y10" s="83"/>
+      <c r="Z10" s="82"/>
+      <c r="AA10" s="83"/>
+      <c r="AB10" s="82"/>
+      <c r="AC10" s="83"/>
     </row>
     <row r="11" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="70"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="132"/>
-      <c r="F11" s="132"/>
-      <c r="G11" s="132"/>
-      <c r="H11" s="132"/>
-      <c r="I11" s="133"/>
-      <c r="J11" s="82"/>
-      <c r="K11" s="83"/>
+      <c r="B11" s="200"/>
+      <c r="C11" s="201"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="126"/>
+      <c r="I11" s="127"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="124"/>
       <c r="L11" s="58"/>
       <c r="M11" s="59"/>
       <c r="N11" s="58"/>
       <c r="O11" s="59"/>
-      <c r="P11" s="144"/>
-      <c r="Q11" s="145"/>
-      <c r="R11" s="145"/>
-      <c r="S11" s="146"/>
-      <c r="T11" s="116"/>
-      <c r="U11" s="117"/>
-      <c r="V11" s="117"/>
-      <c r="W11" s="118"/>
-      <c r="X11" s="188"/>
-      <c r="Y11" s="189"/>
-      <c r="Z11" s="188"/>
-      <c r="AA11" s="189"/>
-      <c r="AB11" s="188"/>
-      <c r="AC11" s="189"/>
+      <c r="P11" s="172"/>
+      <c r="Q11" s="173"/>
+      <c r="R11" s="173"/>
+      <c r="S11" s="174"/>
+      <c r="T11" s="163"/>
+      <c r="U11" s="164"/>
+      <c r="V11" s="164"/>
+      <c r="W11" s="165"/>
+      <c r="X11" s="82"/>
+      <c r="Y11" s="83"/>
+      <c r="Z11" s="82"/>
+      <c r="AA11" s="83"/>
+      <c r="AB11" s="82"/>
+      <c r="AC11" s="83"/>
     </row>
     <row r="12" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B12" s="70"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="126"/>
-      <c r="I12" s="127"/>
-      <c r="J12" s="99"/>
-      <c r="K12" s="100"/>
+      <c r="B12" s="200"/>
+      <c r="C12" s="201"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="102"/>
+      <c r="K12" s="103"/>
       <c r="L12" s="55"/>
       <c r="M12" s="56"/>
       <c r="N12" s="55"/>
       <c r="O12" s="56"/>
-      <c r="P12" s="147"/>
-      <c r="Q12" s="148"/>
-      <c r="R12" s="148"/>
-      <c r="S12" s="149"/>
-      <c r="T12" s="119"/>
-      <c r="U12" s="120"/>
-      <c r="V12" s="120"/>
-      <c r="W12" s="121"/>
-      <c r="X12" s="190"/>
-      <c r="Y12" s="191"/>
-      <c r="Z12" s="190"/>
-      <c r="AA12" s="191"/>
-      <c r="AB12" s="190"/>
-      <c r="AC12" s="191"/>
+      <c r="P12" s="175"/>
+      <c r="Q12" s="176"/>
+      <c r="R12" s="176"/>
+      <c r="S12" s="177"/>
+      <c r="T12" s="166"/>
+      <c r="U12" s="167"/>
+      <c r="V12" s="167"/>
+      <c r="W12" s="168"/>
+      <c r="X12" s="80"/>
+      <c r="Y12" s="81"/>
+      <c r="Z12" s="80"/>
+      <c r="AA12" s="81"/>
+      <c r="AB12" s="80"/>
+      <c r="AC12" s="81"/>
     </row>
     <row r="13" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="70"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="122" t="s">
+      <c r="B13" s="200"/>
+      <c r="C13" s="201"/>
+      <c r="D13" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="124"/>
-      <c r="J13" s="134" t="s">
+      <c r="E13" s="108"/>
+      <c r="F13" s="108"/>
+      <c r="G13" s="108"/>
+      <c r="H13" s="108"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="170"/>
-      <c r="L13" s="107"/>
-      <c r="M13" s="108"/>
-      <c r="N13" s="107"/>
-      <c r="O13" s="108"/>
-      <c r="P13" s="135" t="s">
+      <c r="K13" s="120"/>
+      <c r="L13" s="150"/>
+      <c r="M13" s="147"/>
+      <c r="N13" s="150"/>
+      <c r="O13" s="147"/>
+      <c r="P13" s="151" t="s">
         <v>46</v>
       </c>
-      <c r="Q13" s="136"/>
-      <c r="R13" s="136"/>
-      <c r="S13" s="137"/>
+      <c r="Q13" s="152"/>
+      <c r="R13" s="152"/>
+      <c r="S13" s="153"/>
       <c r="T13" s="26"/>
       <c r="U13" s="27"/>
       <c r="V13" s="27"/>
       <c r="W13" s="28"/>
-      <c r="X13" s="186"/>
-      <c r="Y13" s="187"/>
-      <c r="Z13" s="186"/>
-      <c r="AA13" s="187"/>
-      <c r="AB13" s="186"/>
-      <c r="AC13" s="187"/>
+      <c r="X13" s="78"/>
+      <c r="Y13" s="79"/>
+      <c r="Z13" s="78"/>
+      <c r="AA13" s="79"/>
+      <c r="AB13" s="78"/>
+      <c r="AC13" s="79"/>
     </row>
     <row r="14" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B14" s="70"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="131"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="132"/>
-      <c r="G14" s="132"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="133"/>
-      <c r="J14" s="197"/>
-      <c r="K14" s="198"/>
-      <c r="L14" s="109"/>
-      <c r="M14" s="110"/>
-      <c r="N14" s="109"/>
-      <c r="O14" s="110"/>
-      <c r="P14" s="138"/>
-      <c r="Q14" s="139"/>
-      <c r="R14" s="139"/>
-      <c r="S14" s="140"/>
+      <c r="B14" s="200"/>
+      <c r="C14" s="201"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
+      <c r="H14" s="126"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="213"/>
+      <c r="K14" s="214"/>
+      <c r="L14" s="178"/>
+      <c r="M14" s="179"/>
+      <c r="N14" s="178"/>
+      <c r="O14" s="179"/>
+      <c r="P14" s="154"/>
+      <c r="Q14" s="155"/>
+      <c r="R14" s="155"/>
+      <c r="S14" s="156"/>
       <c r="T14" s="26"/>
       <c r="U14" s="27"/>
       <c r="V14" s="27"/>
       <c r="W14" s="28"/>
-      <c r="X14" s="188"/>
-      <c r="Y14" s="189"/>
-      <c r="Z14" s="188"/>
-      <c r="AA14" s="189"/>
-      <c r="AB14" s="188"/>
-      <c r="AC14" s="189"/>
+      <c r="X14" s="82"/>
+      <c r="Y14" s="83"/>
+      <c r="Z14" s="82"/>
+      <c r="AA14" s="83"/>
+      <c r="AB14" s="82"/>
+      <c r="AC14" s="83"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B15" s="70"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="125"/>
-      <c r="E15" s="126"/>
-      <c r="F15" s="126"/>
-      <c r="G15" s="126"/>
-      <c r="H15" s="126"/>
-      <c r="I15" s="127"/>
-      <c r="J15" s="171"/>
-      <c r="K15" s="172"/>
-      <c r="L15" s="111"/>
-      <c r="M15" s="112"/>
-      <c r="N15" s="111"/>
-      <c r="O15" s="112"/>
-      <c r="P15" s="194"/>
-      <c r="Q15" s="195"/>
-      <c r="R15" s="195"/>
-      <c r="S15" s="196"/>
+      <c r="B15" s="200"/>
+      <c r="C15" s="201"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="111"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="111"/>
+      <c r="H15" s="111"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="121"/>
+      <c r="K15" s="122"/>
+      <c r="L15" s="148"/>
+      <c r="M15" s="149"/>
+      <c r="N15" s="148"/>
+      <c r="O15" s="149"/>
+      <c r="P15" s="157"/>
+      <c r="Q15" s="158"/>
+      <c r="R15" s="158"/>
+      <c r="S15" s="159"/>
       <c r="T15" s="26"/>
       <c r="U15" s="27"/>
       <c r="V15" s="27"/>
       <c r="W15" s="28"/>
-      <c r="X15" s="190"/>
-      <c r="Y15" s="191"/>
-      <c r="Z15" s="190"/>
-      <c r="AA15" s="191"/>
-      <c r="AB15" s="190"/>
-      <c r="AC15" s="191"/>
+      <c r="X15" s="80"/>
+      <c r="Y15" s="81"/>
+      <c r="Z15" s="80"/>
+      <c r="AA15" s="81"/>
+      <c r="AB15" s="80"/>
+      <c r="AC15" s="81"/>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B16" s="70"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="122" t="s">
+      <c r="B16" s="200"/>
+      <c r="C16" s="201"/>
+      <c r="D16" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="123"/>
-      <c r="I16" s="124"/>
-      <c r="J16" s="80" t="s">
+      <c r="E16" s="108"/>
+      <c r="F16" s="108"/>
+      <c r="G16" s="108"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="109"/>
+      <c r="J16" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="81"/>
+      <c r="K16" s="101"/>
       <c r="L16" s="57"/>
       <c r="M16" s="54"/>
       <c r="N16" s="57"/>
       <c r="O16" s="54"/>
-      <c r="P16" s="101" t="s">
+      <c r="P16" s="186" t="s">
         <v>33</v>
       </c>
-      <c r="Q16" s="102"/>
-      <c r="R16" s="102"/>
-      <c r="S16" s="103"/>
+      <c r="Q16" s="187"/>
+      <c r="R16" s="187"/>
+      <c r="S16" s="188"/>
       <c r="T16" s="43"/>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="7"/>
-      <c r="X16" s="186"/>
-      <c r="Y16" s="187"/>
-      <c r="Z16" s="186"/>
-      <c r="AA16" s="187"/>
-      <c r="AB16" s="186"/>
-      <c r="AC16" s="187"/>
+      <c r="X16" s="78"/>
+      <c r="Y16" s="79"/>
+      <c r="Z16" s="78"/>
+      <c r="AA16" s="79"/>
+      <c r="AB16" s="78"/>
+      <c r="AC16" s="79"/>
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B17" s="70"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="125"/>
-      <c r="E17" s="126"/>
-      <c r="F17" s="126"/>
-      <c r="G17" s="126"/>
-      <c r="H17" s="126"/>
-      <c r="I17" s="127"/>
-      <c r="J17" s="99"/>
-      <c r="K17" s="100"/>
+      <c r="B17" s="200"/>
+      <c r="C17" s="201"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="111"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="111"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="102"/>
+      <c r="K17" s="103"/>
       <c r="L17" s="55"/>
       <c r="M17" s="56"/>
       <c r="N17" s="55"/>
       <c r="O17" s="56"/>
-      <c r="P17" s="208"/>
-      <c r="Q17" s="209"/>
-      <c r="R17" s="209"/>
-      <c r="S17" s="210"/>
+      <c r="P17" s="189"/>
+      <c r="Q17" s="190"/>
+      <c r="R17" s="190"/>
+      <c r="S17" s="191"/>
       <c r="T17" s="44"/>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
       <c r="W17" s="9"/>
-      <c r="X17" s="190"/>
-      <c r="Y17" s="191"/>
-      <c r="Z17" s="190"/>
-      <c r="AA17" s="191"/>
-      <c r="AB17" s="190"/>
-      <c r="AC17" s="191"/>
+      <c r="X17" s="80"/>
+      <c r="Y17" s="81"/>
+      <c r="Z17" s="80"/>
+      <c r="AA17" s="81"/>
+      <c r="AB17" s="80"/>
+      <c r="AC17" s="81"/>
     </row>
     <row r="18" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B18" s="70"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="90" t="s">
+      <c r="B18" s="200"/>
+      <c r="C18" s="201"/>
+      <c r="D18" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="91"/>
-      <c r="F18" s="91"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="91"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="80" t="s">
+      <c r="E18" s="114"/>
+      <c r="F18" s="114"/>
+      <c r="G18" s="114"/>
+      <c r="H18" s="114"/>
+      <c r="I18" s="115"/>
+      <c r="J18" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="81"/>
+      <c r="K18" s="101"/>
       <c r="L18" s="58"/>
       <c r="M18" s="59"/>
       <c r="N18" s="58"/>
       <c r="O18" s="59"/>
-      <c r="P18" s="101" t="s">
+      <c r="P18" s="186" t="s">
         <v>35</v>
       </c>
-      <c r="Q18" s="102"/>
-      <c r="R18" s="102"/>
-      <c r="S18" s="103"/>
+      <c r="Q18" s="187"/>
+      <c r="R18" s="187"/>
+      <c r="S18" s="188"/>
       <c r="T18" s="26"/>
       <c r="U18" s="27"/>
       <c r="V18" s="27"/>
       <c r="W18" s="28"/>
-      <c r="X18" s="186"/>
-      <c r="Y18" s="187"/>
-      <c r="Z18" s="186"/>
-      <c r="AA18" s="187"/>
-      <c r="AB18" s="186"/>
-      <c r="AC18" s="187"/>
+      <c r="X18" s="78"/>
+      <c r="Y18" s="79"/>
+      <c r="Z18" s="78"/>
+      <c r="AA18" s="79"/>
+      <c r="AB18" s="78"/>
+      <c r="AC18" s="79"/>
     </row>
     <row r="19" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B19" s="70"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="97"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="97"/>
-      <c r="H19" s="97"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="99"/>
-      <c r="K19" s="100"/>
+      <c r="B19" s="200"/>
+      <c r="C19" s="201"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="102"/>
+      <c r="K19" s="103"/>
       <c r="L19" s="58"/>
       <c r="M19" s="59"/>
       <c r="N19" s="58"/>
       <c r="O19" s="59"/>
-      <c r="P19" s="208"/>
-      <c r="Q19" s="209"/>
-      <c r="R19" s="209"/>
-      <c r="S19" s="210"/>
+      <c r="P19" s="189"/>
+      <c r="Q19" s="190"/>
+      <c r="R19" s="190"/>
+      <c r="S19" s="191"/>
       <c r="T19" s="26"/>
       <c r="U19" s="27"/>
       <c r="V19" s="27"/>
       <c r="W19" s="28"/>
-      <c r="X19" s="190"/>
-      <c r="Y19" s="191"/>
-      <c r="Z19" s="190"/>
-      <c r="AA19" s="191"/>
-      <c r="AB19" s="190"/>
-      <c r="AC19" s="191"/>
+      <c r="X19" s="80"/>
+      <c r="Y19" s="81"/>
+      <c r="Z19" s="80"/>
+      <c r="AA19" s="81"/>
+      <c r="AB19" s="80"/>
+      <c r="AC19" s="81"/>
     </row>
     <row r="20" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B20" s="70"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="90" t="s">
+      <c r="B20" s="200"/>
+      <c r="C20" s="201"/>
+      <c r="D20" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="80" t="s">
+      <c r="E20" s="114"/>
+      <c r="F20" s="114"/>
+      <c r="G20" s="114"/>
+      <c r="H20" s="114"/>
+      <c r="I20" s="115"/>
+      <c r="J20" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="81"/>
+      <c r="K20" s="101"/>
       <c r="L20" s="39"/>
       <c r="M20" s="40"/>
       <c r="N20" s="39"/>
       <c r="O20" s="40"/>
-      <c r="P20" s="84" t="s">
+      <c r="P20" s="180" t="s">
         <v>34</v>
       </c>
-      <c r="Q20" s="85"/>
-      <c r="R20" s="85"/>
-      <c r="S20" s="86"/>
+      <c r="Q20" s="181"/>
+      <c r="R20" s="181"/>
+      <c r="S20" s="182"/>
       <c r="T20" s="43"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="7"/>
-      <c r="X20" s="186"/>
-      <c r="Y20" s="187"/>
-      <c r="Z20" s="186"/>
-      <c r="AA20" s="187"/>
-      <c r="AB20" s="186"/>
-      <c r="AC20" s="187"/>
+      <c r="X20" s="78"/>
+      <c r="Y20" s="79"/>
+      <c r="Z20" s="78"/>
+      <c r="AA20" s="79"/>
+      <c r="AB20" s="78"/>
+      <c r="AC20" s="79"/>
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B21" s="70"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="97"/>
-      <c r="G21" s="97"/>
-      <c r="H21" s="97"/>
-      <c r="I21" s="98"/>
-      <c r="J21" s="99"/>
-      <c r="K21" s="100"/>
+      <c r="B21" s="200"/>
+      <c r="C21" s="201"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="117"/>
+      <c r="H21" s="117"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="102"/>
+      <c r="K21" s="103"/>
       <c r="L21" s="41"/>
       <c r="M21" s="42"/>
       <c r="N21" s="41"/>
       <c r="O21" s="42"/>
-      <c r="P21" s="87"/>
-      <c r="Q21" s="88"/>
-      <c r="R21" s="88"/>
-      <c r="S21" s="89"/>
+      <c r="P21" s="183"/>
+      <c r="Q21" s="184"/>
+      <c r="R21" s="184"/>
+      <c r="S21" s="185"/>
       <c r="T21" s="44"/>
       <c r="U21" s="8"/>
       <c r="V21" s="8"/>
       <c r="W21" s="9"/>
-      <c r="X21" s="190"/>
-      <c r="Y21" s="191"/>
-      <c r="Z21" s="190"/>
-      <c r="AA21" s="191"/>
-      <c r="AB21" s="190"/>
-      <c r="AC21" s="191"/>
+      <c r="X21" s="80"/>
+      <c r="Y21" s="81"/>
+      <c r="Z21" s="80"/>
+      <c r="AA21" s="81"/>
+      <c r="AB21" s="80"/>
+      <c r="AC21" s="81"/>
     </row>
     <row r="22" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B22" s="70"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="90" t="s">
+      <c r="B22" s="200"/>
+      <c r="C22" s="201"/>
+      <c r="D22" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="91"/>
-      <c r="I22" s="92"/>
-      <c r="J22" s="80" t="s">
+      <c r="E22" s="114"/>
+      <c r="F22" s="114"/>
+      <c r="G22" s="114"/>
+      <c r="H22" s="114"/>
+      <c r="I22" s="115"/>
+      <c r="J22" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="K22" s="81"/>
+      <c r="K22" s="101"/>
       <c r="L22" s="14"/>
       <c r="M22" s="15"/>
       <c r="N22" s="14"/>
       <c r="O22" s="15"/>
-      <c r="P22" s="211"/>
-      <c r="Q22" s="211"/>
-      <c r="R22" s="211"/>
-      <c r="S22" s="211"/>
+      <c r="P22" s="74"/>
+      <c r="Q22" s="74"/>
+      <c r="R22" s="74"/>
+      <c r="S22" s="74"/>
       <c r="T22" s="43"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="7"/>
-      <c r="X22" s="186"/>
-      <c r="Y22" s="187"/>
-      <c r="Z22" s="186"/>
-      <c r="AA22" s="187"/>
-      <c r="AB22" s="186"/>
-      <c r="AC22" s="187"/>
+      <c r="X22" s="78"/>
+      <c r="Y22" s="79"/>
+      <c r="Z22" s="78"/>
+      <c r="AA22" s="79"/>
+      <c r="AB22" s="78"/>
+      <c r="AC22" s="79"/>
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B23" s="70"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
-      <c r="G23" s="97"/>
-      <c r="H23" s="97"/>
-      <c r="I23" s="98"/>
-      <c r="J23" s="99"/>
-      <c r="K23" s="100"/>
+      <c r="B23" s="200"/>
+      <c r="C23" s="201"/>
+      <c r="D23" s="116"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="118"/>
+      <c r="J23" s="102"/>
+      <c r="K23" s="103"/>
       <c r="L23" s="18"/>
       <c r="M23" s="19"/>
       <c r="N23" s="18"/>
       <c r="O23" s="19"/>
-      <c r="P23" s="212"/>
-      <c r="Q23" s="212"/>
-      <c r="R23" s="212"/>
-      <c r="S23" s="212"/>
+      <c r="P23" s="75"/>
+      <c r="Q23" s="75"/>
+      <c r="R23" s="75"/>
+      <c r="S23" s="75"/>
       <c r="T23" s="44"/>
       <c r="U23" s="8"/>
       <c r="V23" s="8"/>
       <c r="W23" s="9"/>
-      <c r="X23" s="190"/>
-      <c r="Y23" s="191"/>
-      <c r="Z23" s="190"/>
-      <c r="AA23" s="191"/>
-      <c r="AB23" s="190"/>
-      <c r="AC23" s="191"/>
+      <c r="X23" s="80"/>
+      <c r="Y23" s="81"/>
+      <c r="Z23" s="80"/>
+      <c r="AA23" s="81"/>
+      <c r="AB23" s="80"/>
+      <c r="AC23" s="81"/>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B24" s="70"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="90" t="s">
+      <c r="B24" s="200"/>
+      <c r="C24" s="201"/>
+      <c r="D24" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="91"/>
-      <c r="F24" s="91"/>
-      <c r="G24" s="91"/>
-      <c r="H24" s="91"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="80" t="s">
+      <c r="E24" s="114"/>
+      <c r="F24" s="114"/>
+      <c r="G24" s="114"/>
+      <c r="H24" s="114"/>
+      <c r="I24" s="115"/>
+      <c r="J24" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="81"/>
+      <c r="K24" s="101"/>
       <c r="L24" s="14"/>
       <c r="M24" s="15"/>
       <c r="N24" s="14"/>
       <c r="O24" s="15"/>
-      <c r="P24" s="211"/>
-      <c r="Q24" s="211"/>
-      <c r="R24" s="211"/>
-      <c r="S24" s="211"/>
+      <c r="P24" s="74"/>
+      <c r="Q24" s="74"/>
+      <c r="R24" s="74"/>
+      <c r="S24" s="74"/>
       <c r="T24" s="43"/>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="7"/>
-      <c r="X24" s="186"/>
-      <c r="Y24" s="187"/>
-      <c r="Z24" s="186"/>
-      <c r="AA24" s="187"/>
-      <c r="AB24" s="186"/>
-      <c r="AC24" s="187"/>
+      <c r="X24" s="78"/>
+      <c r="Y24" s="79"/>
+      <c r="Z24" s="78"/>
+      <c r="AA24" s="79"/>
+      <c r="AB24" s="78"/>
+      <c r="AC24" s="79"/>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B25" s="70"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="97"/>
-      <c r="G25" s="97"/>
-      <c r="H25" s="97"/>
-      <c r="I25" s="98"/>
-      <c r="J25" s="99"/>
-      <c r="K25" s="100"/>
+      <c r="B25" s="202"/>
+      <c r="C25" s="203"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="117"/>
+      <c r="F25" s="117"/>
+      <c r="G25" s="117"/>
+      <c r="H25" s="117"/>
+      <c r="I25" s="118"/>
+      <c r="J25" s="102"/>
+      <c r="K25" s="103"/>
       <c r="L25" s="18"/>
       <c r="M25" s="19"/>
       <c r="N25" s="18"/>
       <c r="O25" s="19"/>
-      <c r="P25" s="212"/>
-      <c r="Q25" s="212"/>
-      <c r="R25" s="212"/>
-      <c r="S25" s="212"/>
+      <c r="P25" s="75"/>
+      <c r="Q25" s="75"/>
+      <c r="R25" s="75"/>
+      <c r="S25" s="75"/>
       <c r="T25" s="44"/>
       <c r="U25" s="8"/>
       <c r="V25" s="8"/>
       <c r="W25" s="9"/>
-      <c r="X25" s="190"/>
-      <c r="Y25" s="191"/>
-      <c r="Z25" s="190"/>
-      <c r="AA25" s="191"/>
-      <c r="AB25" s="190"/>
-      <c r="AC25" s="191"/>
+      <c r="X25" s="80"/>
+      <c r="Y25" s="81"/>
+      <c r="Z25" s="80"/>
+      <c r="AA25" s="81"/>
+      <c r="AB25" s="80"/>
+      <c r="AC25" s="81"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B26" s="72"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="90" t="s">
+      <c r="B26" s="204" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="205"/>
+      <c r="D26" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="91"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="91"/>
-      <c r="I26" s="92"/>
-      <c r="J26" s="134" t="s">
+      <c r="E26" s="114"/>
+      <c r="F26" s="114"/>
+      <c r="G26" s="114"/>
+      <c r="H26" s="114"/>
+      <c r="I26" s="115"/>
+      <c r="J26" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="K26" s="81"/>
+      <c r="K26" s="101"/>
       <c r="L26" s="16"/>
       <c r="M26" s="17"/>
       <c r="N26" s="16"/>
       <c r="O26" s="17"/>
-      <c r="P26" s="84" t="s">
+      <c r="P26" s="180" t="s">
         <v>31</v>
       </c>
-      <c r="Q26" s="85"/>
-      <c r="R26" s="85"/>
-      <c r="S26" s="86"/>
+      <c r="Q26" s="181"/>
+      <c r="R26" s="181"/>
+      <c r="S26" s="182"/>
       <c r="T26" s="26"/>
       <c r="U26" s="27"/>
       <c r="V26" s="27"/>
       <c r="W26" s="28"/>
-      <c r="X26" s="186"/>
-      <c r="Y26" s="187"/>
-      <c r="Z26" s="186"/>
-      <c r="AA26" s="187"/>
-      <c r="AB26" s="186"/>
-      <c r="AC26" s="187"/>
+      <c r="X26" s="78"/>
+      <c r="Y26" s="79"/>
+      <c r="Z26" s="78"/>
+      <c r="AA26" s="79"/>
+      <c r="AB26" s="78"/>
+      <c r="AC26" s="79"/>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B27" s="74" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="75"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="97"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="97"/>
-      <c r="I27" s="98"/>
-      <c r="J27" s="99"/>
-      <c r="K27" s="100"/>
+      <c r="B27" s="206"/>
+      <c r="C27" s="207"/>
+      <c r="D27" s="116"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="117"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="118"/>
+      <c r="J27" s="102"/>
+      <c r="K27" s="103"/>
       <c r="L27" s="16"/>
       <c r="M27" s="17"/>
       <c r="N27" s="16"/>
       <c r="O27" s="17"/>
-      <c r="P27" s="87"/>
-      <c r="Q27" s="88"/>
-      <c r="R27" s="88"/>
-      <c r="S27" s="89"/>
+      <c r="P27" s="183"/>
+      <c r="Q27" s="184"/>
+      <c r="R27" s="184"/>
+      <c r="S27" s="185"/>
       <c r="T27" s="26"/>
       <c r="U27" s="27"/>
       <c r="V27" s="27"/>
       <c r="W27" s="28"/>
-      <c r="X27" s="190"/>
-      <c r="Y27" s="191"/>
-      <c r="Z27" s="190"/>
-      <c r="AA27" s="191"/>
-      <c r="AB27" s="190"/>
-      <c r="AC27" s="191"/>
+      <c r="X27" s="80"/>
+      <c r="Y27" s="81"/>
+      <c r="Z27" s="80"/>
+      <c r="AA27" s="81"/>
+      <c r="AB27" s="80"/>
+      <c r="AC27" s="81"/>
     </row>
     <row r="28" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B28" s="76"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="90" t="s">
+      <c r="B28" s="206"/>
+      <c r="C28" s="207"/>
+      <c r="D28" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="91"/>
-      <c r="F28" s="91"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="91"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="80" t="s">
+      <c r="E28" s="114"/>
+      <c r="F28" s="114"/>
+      <c r="G28" s="114"/>
+      <c r="H28" s="114"/>
+      <c r="I28" s="115"/>
+      <c r="J28" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="K28" s="81"/>
+      <c r="K28" s="101"/>
       <c r="L28" s="14"/>
       <c r="M28" s="15"/>
       <c r="N28" s="14"/>
       <c r="O28" s="15"/>
-      <c r="P28" s="211"/>
-      <c r="Q28" s="211"/>
-      <c r="R28" s="211"/>
-      <c r="S28" s="211"/>
+      <c r="P28" s="74"/>
+      <c r="Q28" s="74"/>
+      <c r="R28" s="74"/>
+      <c r="S28" s="74"/>
       <c r="T28" s="43"/>
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
       <c r="W28" s="7"/>
-      <c r="X28" s="186"/>
-      <c r="Y28" s="187"/>
-      <c r="Z28" s="186"/>
-      <c r="AA28" s="187"/>
-      <c r="AB28" s="186"/>
-      <c r="AC28" s="187"/>
+      <c r="X28" s="78"/>
+      <c r="Y28" s="79"/>
+      <c r="Z28" s="78"/>
+      <c r="AA28" s="79"/>
+      <c r="AB28" s="78"/>
+      <c r="AC28" s="79"/>
     </row>
     <row r="29" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="76"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="96"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="97"/>
-      <c r="G29" s="97"/>
-      <c r="H29" s="97"/>
-      <c r="I29" s="98"/>
-      <c r="J29" s="99"/>
-      <c r="K29" s="100"/>
+      <c r="B29" s="206"/>
+      <c r="C29" s="207"/>
+      <c r="D29" s="116"/>
+      <c r="E29" s="117"/>
+      <c r="F29" s="117"/>
+      <c r="G29" s="117"/>
+      <c r="H29" s="117"/>
+      <c r="I29" s="118"/>
+      <c r="J29" s="102"/>
+      <c r="K29" s="103"/>
       <c r="L29" s="18"/>
       <c r="M29" s="19"/>
       <c r="N29" s="18"/>
       <c r="O29" s="19"/>
-      <c r="P29" s="212"/>
-      <c r="Q29" s="212"/>
-      <c r="R29" s="212"/>
-      <c r="S29" s="212"/>
+      <c r="P29" s="75"/>
+      <c r="Q29" s="75"/>
+      <c r="R29" s="75"/>
+      <c r="S29" s="75"/>
       <c r="T29" s="44"/>
       <c r="U29" s="8"/>
       <c r="V29" s="8"/>
       <c r="W29" s="9"/>
-      <c r="X29" s="190"/>
-      <c r="Y29" s="191"/>
-      <c r="Z29" s="190"/>
-      <c r="AA29" s="191"/>
-      <c r="AB29" s="190"/>
-      <c r="AC29" s="191"/>
+      <c r="X29" s="80"/>
+      <c r="Y29" s="81"/>
+      <c r="Z29" s="80"/>
+      <c r="AA29" s="81"/>
+      <c r="AB29" s="80"/>
+      <c r="AC29" s="81"/>
     </row>
     <row r="30" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B30" s="76"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="159" t="s">
+      <c r="B30" s="206"/>
+      <c r="C30" s="207"/>
+      <c r="D30" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
-      <c r="G30" s="160"/>
-      <c r="H30" s="160"/>
-      <c r="I30" s="161"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="81"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="132"/>
+      <c r="G30" s="132"/>
+      <c r="H30" s="132"/>
+      <c r="I30" s="133"/>
+      <c r="J30" s="100"/>
+      <c r="K30" s="101"/>
       <c r="L30" s="14"/>
       <c r="M30" s="15"/>
       <c r="N30" s="14"/>
       <c r="O30" s="15"/>
-      <c r="P30" s="84" t="s">
+      <c r="P30" s="180" t="s">
         <v>32</v>
       </c>
-      <c r="Q30" s="85"/>
-      <c r="R30" s="85"/>
-      <c r="S30" s="86"/>
+      <c r="Q30" s="181"/>
+      <c r="R30" s="181"/>
+      <c r="S30" s="182"/>
       <c r="T30" s="43"/>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
       <c r="W30" s="7"/>
-      <c r="X30" s="186"/>
-      <c r="Y30" s="187"/>
-      <c r="Z30" s="186"/>
-      <c r="AA30" s="187"/>
-      <c r="AB30" s="186"/>
-      <c r="AC30" s="187"/>
+      <c r="X30" s="78"/>
+      <c r="Y30" s="79"/>
+      <c r="Z30" s="78"/>
+      <c r="AA30" s="79"/>
+      <c r="AB30" s="78"/>
+      <c r="AC30" s="79"/>
     </row>
     <row r="31" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B31" s="76"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="162"/>
-      <c r="E31" s="163"/>
-      <c r="F31" s="163"/>
-      <c r="G31" s="163"/>
-      <c r="H31" s="163"/>
-      <c r="I31" s="164"/>
-      <c r="J31" s="99"/>
-      <c r="K31" s="100"/>
+      <c r="B31" s="206"/>
+      <c r="C31" s="207"/>
+      <c r="D31" s="134"/>
+      <c r="E31" s="135"/>
+      <c r="F31" s="135"/>
+      <c r="G31" s="135"/>
+      <c r="H31" s="135"/>
+      <c r="I31" s="136"/>
+      <c r="J31" s="102"/>
+      <c r="K31" s="103"/>
       <c r="L31" s="18"/>
       <c r="M31" s="19"/>
       <c r="N31" s="18"/>
       <c r="O31" s="19"/>
-      <c r="P31" s="87"/>
-      <c r="Q31" s="88"/>
-      <c r="R31" s="88"/>
-      <c r="S31" s="89"/>
+      <c r="P31" s="183"/>
+      <c r="Q31" s="184"/>
+      <c r="R31" s="184"/>
+      <c r="S31" s="185"/>
       <c r="T31" s="44"/>
       <c r="U31" s="8"/>
       <c r="V31" s="8"/>
       <c r="W31" s="9"/>
-      <c r="X31" s="190"/>
-      <c r="Y31" s="191"/>
-      <c r="Z31" s="190"/>
-      <c r="AA31" s="191"/>
-      <c r="AB31" s="190"/>
-      <c r="AC31" s="191"/>
+      <c r="X31" s="80"/>
+      <c r="Y31" s="81"/>
+      <c r="Z31" s="80"/>
+      <c r="AA31" s="81"/>
+      <c r="AB31" s="80"/>
+      <c r="AC31" s="81"/>
     </row>
     <row r="32" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B32" s="76"/>
-      <c r="C32" s="77"/>
-      <c r="D32" s="90" t="s">
+      <c r="B32" s="206"/>
+      <c r="C32" s="207"/>
+      <c r="D32" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="91"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="91"/>
-      <c r="H32" s="91"/>
-      <c r="I32" s="92"/>
-      <c r="J32" s="134" t="s">
+      <c r="E32" s="114"/>
+      <c r="F32" s="114"/>
+      <c r="G32" s="114"/>
+      <c r="H32" s="114"/>
+      <c r="I32" s="115"/>
+      <c r="J32" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="K32" s="170"/>
+      <c r="K32" s="120"/>
       <c r="L32" s="14"/>
       <c r="M32" s="15"/>
       <c r="N32" s="14"/>
       <c r="O32" s="15"/>
-      <c r="P32" s="211"/>
-      <c r="Q32" s="211"/>
-      <c r="R32" s="211"/>
-      <c r="S32" s="211"/>
+      <c r="P32" s="74"/>
+      <c r="Q32" s="74"/>
+      <c r="R32" s="74"/>
+      <c r="S32" s="74"/>
       <c r="T32" s="43"/>
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
       <c r="W32" s="7"/>
-      <c r="X32" s="186"/>
-      <c r="Y32" s="187"/>
-      <c r="Z32" s="186"/>
-      <c r="AA32" s="187"/>
-      <c r="AB32" s="186"/>
-      <c r="AC32" s="187"/>
+      <c r="X32" s="78"/>
+      <c r="Y32" s="79"/>
+      <c r="Z32" s="78"/>
+      <c r="AA32" s="79"/>
+      <c r="AB32" s="78"/>
+      <c r="AC32" s="79"/>
     </row>
     <row r="33" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B33" s="76"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="97"/>
-      <c r="F33" s="97"/>
-      <c r="G33" s="97"/>
-      <c r="H33" s="97"/>
-      <c r="I33" s="98"/>
-      <c r="J33" s="171"/>
-      <c r="K33" s="172"/>
+      <c r="B33" s="206"/>
+      <c r="C33" s="207"/>
+      <c r="D33" s="116"/>
+      <c r="E33" s="117"/>
+      <c r="F33" s="117"/>
+      <c r="G33" s="117"/>
+      <c r="H33" s="117"/>
+      <c r="I33" s="118"/>
+      <c r="J33" s="121"/>
+      <c r="K33" s="122"/>
       <c r="L33" s="18"/>
       <c r="M33" s="19"/>
       <c r="N33" s="18"/>
       <c r="O33" s="19"/>
-      <c r="P33" s="212"/>
-      <c r="Q33" s="212"/>
-      <c r="R33" s="212"/>
-      <c r="S33" s="212"/>
+      <c r="P33" s="75"/>
+      <c r="Q33" s="75"/>
+      <c r="R33" s="75"/>
+      <c r="S33" s="75"/>
       <c r="T33" s="44"/>
       <c r="U33" s="8"/>
       <c r="V33" s="8"/>
       <c r="W33" s="9"/>
-      <c r="X33" s="190"/>
-      <c r="Y33" s="191"/>
-      <c r="Z33" s="190"/>
-      <c r="AA33" s="191"/>
-      <c r="AB33" s="190"/>
-      <c r="AC33" s="191"/>
+      <c r="X33" s="80"/>
+      <c r="Y33" s="81"/>
+      <c r="Z33" s="80"/>
+      <c r="AA33" s="81"/>
+      <c r="AB33" s="80"/>
+      <c r="AC33" s="81"/>
     </row>
     <row r="34" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B34" s="76"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="90" t="s">
+      <c r="B34" s="206"/>
+      <c r="C34" s="207"/>
+      <c r="D34" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="91"/>
-      <c r="H34" s="91"/>
-      <c r="I34" s="92"/>
-      <c r="J34" s="80" t="s">
+      <c r="E34" s="114"/>
+      <c r="F34" s="114"/>
+      <c r="G34" s="114"/>
+      <c r="H34" s="114"/>
+      <c r="I34" s="115"/>
+      <c r="J34" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="K34" s="81"/>
+      <c r="K34" s="101"/>
       <c r="L34" s="14"/>
       <c r="M34" s="15"/>
       <c r="N34" s="14"/>
       <c r="O34" s="15"/>
-      <c r="P34" s="211"/>
-      <c r="Q34" s="211"/>
-      <c r="R34" s="211"/>
-      <c r="S34" s="211"/>
+      <c r="P34" s="74"/>
+      <c r="Q34" s="74"/>
+      <c r="R34" s="74"/>
+      <c r="S34" s="74"/>
       <c r="T34" s="43"/>
       <c r="U34" s="6"/>
       <c r="V34" s="6"/>
       <c r="W34" s="7"/>
-      <c r="X34" s="186"/>
-      <c r="Y34" s="187"/>
-      <c r="Z34" s="186"/>
-      <c r="AA34" s="187"/>
-      <c r="AB34" s="186"/>
-      <c r="AC34" s="187"/>
+      <c r="X34" s="78"/>
+      <c r="Y34" s="79"/>
+      <c r="Z34" s="78"/>
+      <c r="AA34" s="79"/>
+      <c r="AB34" s="78"/>
+      <c r="AC34" s="79"/>
     </row>
     <row r="35" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B35" s="76"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="97"/>
-      <c r="F35" s="97"/>
-      <c r="G35" s="97"/>
-      <c r="H35" s="97"/>
-      <c r="I35" s="98"/>
-      <c r="J35" s="99"/>
-      <c r="K35" s="100"/>
+      <c r="B35" s="206"/>
+      <c r="C35" s="207"/>
+      <c r="D35" s="116"/>
+      <c r="E35" s="117"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="117"/>
+      <c r="H35" s="117"/>
+      <c r="I35" s="118"/>
+      <c r="J35" s="102"/>
+      <c r="K35" s="103"/>
       <c r="L35" s="18"/>
       <c r="M35" s="19"/>
       <c r="N35" s="18"/>
       <c r="O35" s="19"/>
-      <c r="P35" s="212"/>
-      <c r="Q35" s="212"/>
-      <c r="R35" s="212"/>
-      <c r="S35" s="212"/>
+      <c r="P35" s="75"/>
+      <c r="Q35" s="75"/>
+      <c r="R35" s="75"/>
+      <c r="S35" s="75"/>
       <c r="T35" s="44"/>
       <c r="U35" s="8"/>
       <c r="V35" s="8"/>
       <c r="W35" s="9"/>
-      <c r="X35" s="190"/>
-      <c r="Y35" s="191"/>
-      <c r="Z35" s="190"/>
-      <c r="AA35" s="191"/>
-      <c r="AB35" s="190"/>
-      <c r="AC35" s="191"/>
+      <c r="X35" s="80"/>
+      <c r="Y35" s="81"/>
+      <c r="Z35" s="80"/>
+      <c r="AA35" s="81"/>
+      <c r="AB35" s="80"/>
+      <c r="AC35" s="81"/>
     </row>
     <row r="36" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B36" s="76"/>
-      <c r="C36" s="77"/>
-      <c r="D36" s="90" t="s">
+      <c r="B36" s="206"/>
+      <c r="C36" s="207"/>
+      <c r="D36" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="91"/>
-      <c r="F36" s="91"/>
-      <c r="G36" s="91"/>
-      <c r="H36" s="91"/>
-      <c r="I36" s="92"/>
-      <c r="J36" s="80" t="s">
+      <c r="E36" s="114"/>
+      <c r="F36" s="114"/>
+      <c r="G36" s="114"/>
+      <c r="H36" s="114"/>
+      <c r="I36" s="115"/>
+      <c r="J36" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="K36" s="81"/>
+      <c r="K36" s="101"/>
       <c r="L36" s="29"/>
       <c r="M36" s="30"/>
       <c r="N36" s="29"/>
       <c r="O36" s="30"/>
-      <c r="P36" s="84" t="s">
+      <c r="P36" s="180" t="s">
         <v>39</v>
       </c>
-      <c r="Q36" s="85"/>
-      <c r="R36" s="85"/>
-      <c r="S36" s="86"/>
+      <c r="Q36" s="181"/>
+      <c r="R36" s="181"/>
+      <c r="S36" s="182"/>
       <c r="T36" s="45"/>
       <c r="U36" s="46"/>
       <c r="V36" s="46"/>
       <c r="W36" s="47"/>
-      <c r="X36" s="199"/>
-      <c r="Y36" s="200"/>
-      <c r="Z36" s="199"/>
-      <c r="AA36" s="200"/>
-      <c r="AB36" s="199"/>
-      <c r="AC36" s="200"/>
+      <c r="X36" s="84"/>
+      <c r="Y36" s="85"/>
+      <c r="Z36" s="84"/>
+      <c r="AA36" s="85"/>
+      <c r="AB36" s="84"/>
+      <c r="AC36" s="85"/>
     </row>
     <row r="37" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B37" s="76"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="97"/>
-      <c r="F37" s="97"/>
-      <c r="G37" s="97"/>
-      <c r="H37" s="97"/>
-      <c r="I37" s="98"/>
-      <c r="J37" s="82"/>
-      <c r="K37" s="83"/>
+      <c r="B37" s="206"/>
+      <c r="C37" s="207"/>
+      <c r="D37" s="116"/>
+      <c r="E37" s="117"/>
+      <c r="F37" s="117"/>
+      <c r="G37" s="117"/>
+      <c r="H37" s="117"/>
+      <c r="I37" s="118"/>
+      <c r="J37" s="123"/>
+      <c r="K37" s="124"/>
       <c r="L37" s="34"/>
       <c r="M37" s="35"/>
       <c r="N37" s="34"/>
       <c r="O37" s="35"/>
-      <c r="P37" s="87"/>
-      <c r="Q37" s="88"/>
-      <c r="R37" s="88"/>
-      <c r="S37" s="89"/>
+      <c r="P37" s="183"/>
+      <c r="Q37" s="184"/>
+      <c r="R37" s="184"/>
+      <c r="S37" s="185"/>
       <c r="T37" s="48"/>
       <c r="U37" s="49"/>
       <c r="V37" s="49"/>
       <c r="W37" s="50"/>
-      <c r="X37" s="201"/>
-      <c r="Y37" s="202"/>
-      <c r="Z37" s="201"/>
-      <c r="AA37" s="202"/>
-      <c r="AB37" s="201"/>
-      <c r="AC37" s="202"/>
+      <c r="X37" s="88"/>
+      <c r="Y37" s="89"/>
+      <c r="Z37" s="88"/>
+      <c r="AA37" s="89"/>
+      <c r="AB37" s="88"/>
+      <c r="AC37" s="89"/>
     </row>
     <row r="38" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B38" s="76"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="90" t="s">
+      <c r="B38" s="206"/>
+      <c r="C38" s="207"/>
+      <c r="D38" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="91"/>
-      <c r="F38" s="91"/>
-      <c r="G38" s="91"/>
-      <c r="H38" s="91"/>
-      <c r="I38" s="92"/>
-      <c r="J38" s="80" t="s">
+      <c r="E38" s="114"/>
+      <c r="F38" s="114"/>
+      <c r="G38" s="114"/>
+      <c r="H38" s="114"/>
+      <c r="I38" s="115"/>
+      <c r="J38" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="K38" s="81"/>
+      <c r="K38" s="101"/>
       <c r="L38" s="29"/>
       <c r="M38" s="30"/>
       <c r="N38" s="29"/>
       <c r="O38" s="30"/>
-      <c r="P38" s="101" t="s">
+      <c r="P38" s="186" t="s">
         <v>41</v>
       </c>
-      <c r="Q38" s="102"/>
-      <c r="R38" s="102"/>
-      <c r="S38" s="103"/>
+      <c r="Q38" s="187"/>
+      <c r="R38" s="187"/>
+      <c r="S38" s="188"/>
       <c r="T38" s="31"/>
       <c r="U38" s="32"/>
       <c r="V38" s="32"/>
       <c r="W38" s="33"/>
-      <c r="X38" s="199"/>
-      <c r="Y38" s="200"/>
-      <c r="Z38" s="199"/>
-      <c r="AA38" s="200"/>
-      <c r="AB38" s="199"/>
-      <c r="AC38" s="200"/>
+      <c r="X38" s="84"/>
+      <c r="Y38" s="85"/>
+      <c r="Z38" s="84"/>
+      <c r="AA38" s="85"/>
+      <c r="AB38" s="84"/>
+      <c r="AC38" s="85"/>
     </row>
     <row r="39" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="76"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="93"/>
-      <c r="E39" s="94"/>
-      <c r="F39" s="94"/>
-      <c r="G39" s="94"/>
-      <c r="H39" s="94"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="82"/>
-      <c r="K39" s="83"/>
+      <c r="B39" s="206"/>
+      <c r="C39" s="207"/>
+      <c r="D39" s="195"/>
+      <c r="E39" s="196"/>
+      <c r="F39" s="196"/>
+      <c r="G39" s="196"/>
+      <c r="H39" s="196"/>
+      <c r="I39" s="197"/>
+      <c r="J39" s="123"/>
+      <c r="K39" s="124"/>
       <c r="L39" s="63"/>
       <c r="M39" s="64"/>
       <c r="N39" s="63"/>
       <c r="O39" s="64"/>
-      <c r="P39" s="104"/>
-      <c r="Q39" s="105"/>
-      <c r="R39" s="105"/>
-      <c r="S39" s="106"/>
+      <c r="P39" s="210"/>
+      <c r="Q39" s="211"/>
+      <c r="R39" s="211"/>
+      <c r="S39" s="212"/>
       <c r="T39" s="65"/>
       <c r="U39" s="66"/>
       <c r="V39" s="66"/>
       <c r="W39" s="67"/>
-      <c r="X39" s="203"/>
-      <c r="Y39" s="204"/>
-      <c r="Z39" s="203"/>
-      <c r="AA39" s="204"/>
-      <c r="AB39" s="203"/>
-      <c r="AC39" s="204"/>
+      <c r="X39" s="86"/>
+      <c r="Y39" s="87"/>
+      <c r="Z39" s="86"/>
+      <c r="AA39" s="87"/>
+      <c r="AB39" s="86"/>
+      <c r="AC39" s="87"/>
     </row>
     <row r="40" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B40" s="76"/>
-      <c r="C40" s="77"/>
-      <c r="D40" s="96"/>
-      <c r="E40" s="97"/>
-      <c r="F40" s="97"/>
-      <c r="G40" s="97"/>
-      <c r="H40" s="97"/>
-      <c r="I40" s="98"/>
-      <c r="J40" s="99"/>
-      <c r="K40" s="100"/>
+      <c r="B40" s="206"/>
+      <c r="C40" s="207"/>
+      <c r="D40" s="116"/>
+      <c r="E40" s="117"/>
+      <c r="F40" s="117"/>
+      <c r="G40" s="117"/>
+      <c r="H40" s="117"/>
+      <c r="I40" s="118"/>
+      <c r="J40" s="102"/>
+      <c r="K40" s="103"/>
       <c r="L40" s="63"/>
       <c r="M40" s="64"/>
       <c r="N40" s="63"/>
       <c r="O40" s="64"/>
-      <c r="P40" s="104"/>
-      <c r="Q40" s="105"/>
-      <c r="R40" s="105"/>
-      <c r="S40" s="106"/>
+      <c r="P40" s="210"/>
+      <c r="Q40" s="211"/>
+      <c r="R40" s="211"/>
+      <c r="S40" s="212"/>
       <c r="T40" s="36"/>
       <c r="U40" s="37"/>
       <c r="V40" s="37"/>
       <c r="W40" s="38"/>
-      <c r="X40" s="201"/>
-      <c r="Y40" s="202"/>
-      <c r="Z40" s="201"/>
-      <c r="AA40" s="202"/>
-      <c r="AB40" s="201"/>
-      <c r="AC40" s="202"/>
+      <c r="X40" s="88"/>
+      <c r="Y40" s="89"/>
+      <c r="Z40" s="88"/>
+      <c r="AA40" s="89"/>
+      <c r="AB40" s="88"/>
+      <c r="AC40" s="89"/>
     </row>
     <row r="41" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B41" s="76"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="90" t="s">
+      <c r="B41" s="206"/>
+      <c r="C41" s="207"/>
+      <c r="D41" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="91"/>
-      <c r="F41" s="91"/>
-      <c r="G41" s="91"/>
-      <c r="H41" s="91"/>
-      <c r="I41" s="92"/>
-      <c r="J41" s="80" t="s">
+      <c r="E41" s="114"/>
+      <c r="F41" s="114"/>
+      <c r="G41" s="114"/>
+      <c r="H41" s="114"/>
+      <c r="I41" s="115"/>
+      <c r="J41" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="K41" s="81"/>
+      <c r="K41" s="101"/>
       <c r="L41" s="39"/>
       <c r="M41" s="40"/>
       <c r="N41" s="39"/>
@@ -6583,24 +6614,24 @@
       <c r="U41" s="6"/>
       <c r="V41" s="6"/>
       <c r="W41" s="7"/>
-      <c r="X41" s="186"/>
-      <c r="Y41" s="187"/>
-      <c r="Z41" s="186"/>
-      <c r="AA41" s="187"/>
-      <c r="AB41" s="186"/>
-      <c r="AC41" s="187"/>
+      <c r="X41" s="78"/>
+      <c r="Y41" s="79"/>
+      <c r="Z41" s="78"/>
+      <c r="AA41" s="79"/>
+      <c r="AB41" s="78"/>
+      <c r="AC41" s="79"/>
     </row>
     <row r="42" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B42" s="76"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="97"/>
-      <c r="F42" s="97"/>
-      <c r="G42" s="97"/>
-      <c r="H42" s="97"/>
-      <c r="I42" s="98"/>
-      <c r="J42" s="99"/>
-      <c r="K42" s="100"/>
+      <c r="B42" s="208"/>
+      <c r="C42" s="209"/>
+      <c r="D42" s="116"/>
+      <c r="E42" s="117"/>
+      <c r="F42" s="117"/>
+      <c r="G42" s="117"/>
+      <c r="H42" s="117"/>
+      <c r="I42" s="118"/>
+      <c r="J42" s="102"/>
+      <c r="K42" s="103"/>
       <c r="L42" s="41"/>
       <c r="M42" s="42"/>
       <c r="N42" s="41"/>
@@ -6613,194 +6644,192 @@
       <c r="U42" s="8"/>
       <c r="V42" s="8"/>
       <c r="W42" s="9"/>
-      <c r="X42" s="190"/>
-      <c r="Y42" s="191"/>
-      <c r="Z42" s="190"/>
-      <c r="AA42" s="191"/>
-      <c r="AB42" s="190"/>
-      <c r="AC42" s="191"/>
+      <c r="X42" s="80"/>
+      <c r="Y42" s="81"/>
+      <c r="Z42" s="80"/>
+      <c r="AA42" s="81"/>
+      <c r="AB42" s="80"/>
+      <c r="AC42" s="81"/>
     </row>
     <row r="43" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B43" s="78"/>
-      <c r="C43" s="79"/>
-      <c r="D43" s="90" t="s">
+      <c r="D43" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="91"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="91"/>
-      <c r="H43" s="91"/>
-      <c r="I43" s="92"/>
-      <c r="J43" s="80" t="s">
+      <c r="E43" s="114"/>
+      <c r="F43" s="114"/>
+      <c r="G43" s="114"/>
+      <c r="H43" s="114"/>
+      <c r="I43" s="115"/>
+      <c r="J43" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="K43" s="81"/>
+      <c r="K43" s="101"/>
       <c r="L43" s="39"/>
       <c r="M43" s="40"/>
       <c r="N43" s="39"/>
       <c r="O43" s="40"/>
-      <c r="P43" s="84" t="s">
+      <c r="P43" s="180" t="s">
         <v>36</v>
       </c>
-      <c r="Q43" s="85"/>
-      <c r="R43" s="85"/>
-      <c r="S43" s="86"/>
+      <c r="Q43" s="181"/>
+      <c r="R43" s="181"/>
+      <c r="S43" s="182"/>
       <c r="T43" s="43"/>
       <c r="U43" s="6"/>
       <c r="V43" s="6"/>
       <c r="W43" s="7"/>
-      <c r="X43" s="186"/>
-      <c r="Y43" s="187"/>
-      <c r="Z43" s="186"/>
-      <c r="AA43" s="187"/>
-      <c r="AB43" s="186"/>
-      <c r="AC43" s="187"/>
+      <c r="X43" s="78"/>
+      <c r="Y43" s="79"/>
+      <c r="Z43" s="78"/>
+      <c r="AA43" s="79"/>
+      <c r="AB43" s="78"/>
+      <c r="AC43" s="79"/>
     </row>
     <row r="44" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="D44" s="96"/>
-      <c r="E44" s="97"/>
-      <c r="F44" s="97"/>
-      <c r="G44" s="97"/>
-      <c r="H44" s="97"/>
-      <c r="I44" s="98"/>
-      <c r="J44" s="99"/>
-      <c r="K44" s="100"/>
+      <c r="D44" s="116"/>
+      <c r="E44" s="117"/>
+      <c r="F44" s="117"/>
+      <c r="G44" s="117"/>
+      <c r="H44" s="117"/>
+      <c r="I44" s="118"/>
+      <c r="J44" s="102"/>
+      <c r="K44" s="103"/>
       <c r="L44" s="41"/>
       <c r="M44" s="42"/>
       <c r="N44" s="41"/>
       <c r="O44" s="42"/>
-      <c r="P44" s="87"/>
-      <c r="Q44" s="88"/>
-      <c r="R44" s="88"/>
-      <c r="S44" s="89"/>
+      <c r="P44" s="183"/>
+      <c r="Q44" s="184"/>
+      <c r="R44" s="184"/>
+      <c r="S44" s="185"/>
       <c r="T44" s="44"/>
       <c r="U44" s="8"/>
       <c r="V44" s="8"/>
       <c r="W44" s="9"/>
-      <c r="X44" s="190"/>
-      <c r="Y44" s="191"/>
-      <c r="Z44" s="190"/>
-      <c r="AA44" s="191"/>
-      <c r="AB44" s="190"/>
-      <c r="AC44" s="191"/>
+      <c r="X44" s="80"/>
+      <c r="Y44" s="81"/>
+      <c r="Z44" s="80"/>
+      <c r="AA44" s="81"/>
+      <c r="AB44" s="80"/>
+      <c r="AC44" s="81"/>
     </row>
     <row r="45" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="D45" s="90" t="s">
+      <c r="D45" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="E45" s="91"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="91"/>
-      <c r="H45" s="91"/>
-      <c r="I45" s="92"/>
-      <c r="J45" s="80" t="s">
+      <c r="E45" s="114"/>
+      <c r="F45" s="114"/>
+      <c r="G45" s="114"/>
+      <c r="H45" s="114"/>
+      <c r="I45" s="115"/>
+      <c r="J45" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="K45" s="81"/>
-      <c r="L45" s="107"/>
-      <c r="M45" s="108"/>
+      <c r="K45" s="101"/>
+      <c r="L45" s="150"/>
+      <c r="M45" s="147"/>
       <c r="N45" s="39"/>
       <c r="O45" s="40"/>
-      <c r="P45" s="84" t="s">
+      <c r="P45" s="180" t="s">
         <v>37</v>
       </c>
-      <c r="Q45" s="85"/>
-      <c r="R45" s="85"/>
-      <c r="S45" s="86"/>
-      <c r="T45" s="113"/>
-      <c r="U45" s="114"/>
-      <c r="V45" s="114"/>
-      <c r="W45" s="115"/>
-      <c r="X45" s="186"/>
-      <c r="Y45" s="187"/>
-      <c r="Z45" s="186"/>
-      <c r="AA45" s="187"/>
-      <c r="AB45" s="186"/>
-      <c r="AC45" s="187"/>
+      <c r="Q45" s="181"/>
+      <c r="R45" s="181"/>
+      <c r="S45" s="182"/>
+      <c r="T45" s="160"/>
+      <c r="U45" s="161"/>
+      <c r="V45" s="161"/>
+      <c r="W45" s="162"/>
+      <c r="X45" s="78"/>
+      <c r="Y45" s="79"/>
+      <c r="Z45" s="78"/>
+      <c r="AA45" s="79"/>
+      <c r="AB45" s="78"/>
+      <c r="AC45" s="79"/>
     </row>
     <row r="46" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="D46" s="93"/>
-      <c r="E46" s="94"/>
-      <c r="F46" s="94"/>
-      <c r="G46" s="94"/>
-      <c r="H46" s="94"/>
-      <c r="I46" s="95"/>
-      <c r="J46" s="82"/>
-      <c r="K46" s="83"/>
-      <c r="L46" s="109"/>
-      <c r="M46" s="110"/>
+      <c r="D46" s="195"/>
+      <c r="E46" s="196"/>
+      <c r="F46" s="196"/>
+      <c r="G46" s="196"/>
+      <c r="H46" s="196"/>
+      <c r="I46" s="197"/>
+      <c r="J46" s="123"/>
+      <c r="K46" s="124"/>
+      <c r="L46" s="178"/>
+      <c r="M46" s="179"/>
       <c r="N46" s="24"/>
       <c r="O46" s="25"/>
-      <c r="P46" s="128"/>
-      <c r="Q46" s="129"/>
-      <c r="R46" s="129"/>
-      <c r="S46" s="130"/>
-      <c r="T46" s="116"/>
-      <c r="U46" s="117"/>
-      <c r="V46" s="117"/>
-      <c r="W46" s="118"/>
-      <c r="X46" s="188"/>
-      <c r="Y46" s="189"/>
-      <c r="Z46" s="188"/>
-      <c r="AA46" s="189"/>
-      <c r="AB46" s="188"/>
-      <c r="AC46" s="189"/>
+      <c r="P46" s="192"/>
+      <c r="Q46" s="193"/>
+      <c r="R46" s="193"/>
+      <c r="S46" s="194"/>
+      <c r="T46" s="163"/>
+      <c r="U46" s="164"/>
+      <c r="V46" s="164"/>
+      <c r="W46" s="165"/>
+      <c r="X46" s="82"/>
+      <c r="Y46" s="83"/>
+      <c r="Z46" s="82"/>
+      <c r="AA46" s="83"/>
+      <c r="AB46" s="82"/>
+      <c r="AC46" s="83"/>
     </row>
     <row r="47" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="93"/>
-      <c r="E47" s="94"/>
-      <c r="F47" s="94"/>
-      <c r="G47" s="94"/>
-      <c r="H47" s="94"/>
-      <c r="I47" s="95"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="83"/>
-      <c r="L47" s="109"/>
-      <c r="M47" s="110"/>
+      <c r="D47" s="195"/>
+      <c r="E47" s="196"/>
+      <c r="F47" s="196"/>
+      <c r="G47" s="196"/>
+      <c r="H47" s="196"/>
+      <c r="I47" s="197"/>
+      <c r="J47" s="123"/>
+      <c r="K47" s="124"/>
+      <c r="L47" s="178"/>
+      <c r="M47" s="179"/>
       <c r="N47" s="24"/>
       <c r="O47" s="25"/>
-      <c r="P47" s="128"/>
-      <c r="Q47" s="129"/>
-      <c r="R47" s="129"/>
-      <c r="S47" s="130"/>
-      <c r="T47" s="116"/>
-      <c r="U47" s="117"/>
-      <c r="V47" s="117"/>
-      <c r="W47" s="118"/>
-      <c r="X47" s="188"/>
-      <c r="Y47" s="189"/>
-      <c r="Z47" s="188"/>
-      <c r="AA47" s="189"/>
-      <c r="AB47" s="188"/>
-      <c r="AC47" s="189"/>
+      <c r="P47" s="192"/>
+      <c r="Q47" s="193"/>
+      <c r="R47" s="193"/>
+      <c r="S47" s="194"/>
+      <c r="T47" s="163"/>
+      <c r="U47" s="164"/>
+      <c r="V47" s="164"/>
+      <c r="W47" s="165"/>
+      <c r="X47" s="82"/>
+      <c r="Y47" s="83"/>
+      <c r="Z47" s="82"/>
+      <c r="AA47" s="83"/>
+      <c r="AB47" s="82"/>
+      <c r="AC47" s="83"/>
     </row>
     <row r="48" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="D48" s="96"/>
-      <c r="E48" s="97"/>
-      <c r="F48" s="97"/>
-      <c r="G48" s="97"/>
-      <c r="H48" s="97"/>
-      <c r="I48" s="98"/>
-      <c r="J48" s="99"/>
-      <c r="K48" s="100"/>
-      <c r="L48" s="111"/>
-      <c r="M48" s="112"/>
+      <c r="D48" s="116"/>
+      <c r="E48" s="117"/>
+      <c r="F48" s="117"/>
+      <c r="G48" s="117"/>
+      <c r="H48" s="117"/>
+      <c r="I48" s="118"/>
+      <c r="J48" s="102"/>
+      <c r="K48" s="103"/>
+      <c r="L48" s="148"/>
+      <c r="M48" s="149"/>
       <c r="N48" s="41"/>
       <c r="O48" s="42"/>
-      <c r="P48" s="87"/>
-      <c r="Q48" s="88"/>
-      <c r="R48" s="88"/>
-      <c r="S48" s="89"/>
-      <c r="T48" s="119"/>
-      <c r="U48" s="120"/>
-      <c r="V48" s="120"/>
-      <c r="W48" s="121"/>
-      <c r="X48" s="190"/>
-      <c r="Y48" s="191"/>
-      <c r="Z48" s="190"/>
-      <c r="AA48" s="191"/>
-      <c r="AB48" s="190"/>
-      <c r="AC48" s="191"/>
+      <c r="P48" s="183"/>
+      <c r="Q48" s="184"/>
+      <c r="R48" s="184"/>
+      <c r="S48" s="185"/>
+      <c r="T48" s="166"/>
+      <c r="U48" s="167"/>
+      <c r="V48" s="167"/>
+      <c r="W48" s="168"/>
+      <c r="X48" s="80"/>
+      <c r="Y48" s="81"/>
+      <c r="Z48" s="80"/>
+      <c r="AA48" s="81"/>
+      <c r="AB48" s="80"/>
+      <c r="AC48" s="81"/>
     </row>
     <row r="49" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D49" s="51"/>
@@ -6815,20 +6844,20 @@
       <c r="M49" s="17"/>
       <c r="N49" s="16"/>
       <c r="O49" s="17"/>
-      <c r="P49" s="213"/>
-      <c r="Q49" s="213"/>
-      <c r="R49" s="213"/>
-      <c r="S49" s="213"/>
+      <c r="P49" s="76"/>
+      <c r="Q49" s="76"/>
+      <c r="R49" s="76"/>
+      <c r="S49" s="76"/>
       <c r="T49" s="20"/>
       <c r="U49" s="21"/>
       <c r="V49" s="21"/>
       <c r="W49" s="22"/>
-      <c r="X49" s="183"/>
-      <c r="Y49" s="184"/>
-      <c r="Z49" s="185"/>
-      <c r="AA49" s="185"/>
-      <c r="AB49" s="183"/>
-      <c r="AC49" s="184"/>
+      <c r="X49" s="71"/>
+      <c r="Y49" s="72"/>
+      <c r="Z49" s="73"/>
+      <c r="AA49" s="73"/>
+      <c r="AB49" s="71"/>
+      <c r="AC49" s="72"/>
     </row>
     <row r="50" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D50" s="51"/>
@@ -6843,20 +6872,20 @@
       <c r="M50" s="17"/>
       <c r="N50" s="16"/>
       <c r="O50" s="17"/>
-      <c r="P50" s="213"/>
-      <c r="Q50" s="213"/>
-      <c r="R50" s="213"/>
-      <c r="S50" s="213"/>
+      <c r="P50" s="76"/>
+      <c r="Q50" s="76"/>
+      <c r="R50" s="76"/>
+      <c r="S50" s="76"/>
       <c r="T50" s="20"/>
       <c r="U50" s="21"/>
       <c r="V50" s="21"/>
       <c r="W50" s="22"/>
-      <c r="X50" s="183"/>
-      <c r="Y50" s="184"/>
-      <c r="Z50" s="185"/>
-      <c r="AA50" s="185"/>
-      <c r="AB50" s="183"/>
-      <c r="AC50" s="184"/>
+      <c r="X50" s="71"/>
+      <c r="Y50" s="72"/>
+      <c r="Z50" s="73"/>
+      <c r="AA50" s="73"/>
+      <c r="AB50" s="71"/>
+      <c r="AC50" s="72"/>
     </row>
     <row r="51" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D51" s="51"/>
@@ -6871,20 +6900,20 @@
       <c r="M51" s="17"/>
       <c r="N51" s="16"/>
       <c r="O51" s="17"/>
-      <c r="P51" s="213"/>
-      <c r="Q51" s="213"/>
-      <c r="R51" s="213"/>
-      <c r="S51" s="213"/>
+      <c r="P51" s="76"/>
+      <c r="Q51" s="76"/>
+      <c r="R51" s="76"/>
+      <c r="S51" s="76"/>
       <c r="T51" s="20"/>
       <c r="U51" s="21"/>
       <c r="V51" s="21"/>
       <c r="W51" s="22"/>
-      <c r="X51" s="183"/>
-      <c r="Y51" s="184"/>
-      <c r="Z51" s="185"/>
-      <c r="AA51" s="185"/>
-      <c r="AB51" s="183"/>
-      <c r="AC51" s="184"/>
+      <c r="X51" s="71"/>
+      <c r="Y51" s="72"/>
+      <c r="Z51" s="73"/>
+      <c r="AA51" s="73"/>
+      <c r="AB51" s="71"/>
+      <c r="AC51" s="72"/>
     </row>
     <row r="52" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D52" s="51"/>
@@ -6899,20 +6928,20 @@
       <c r="M52" s="17"/>
       <c r="N52" s="16"/>
       <c r="O52" s="17"/>
-      <c r="P52" s="213"/>
-      <c r="Q52" s="213"/>
-      <c r="R52" s="213"/>
-      <c r="S52" s="213"/>
+      <c r="P52" s="76"/>
+      <c r="Q52" s="76"/>
+      <c r="R52" s="76"/>
+      <c r="S52" s="76"/>
       <c r="T52" s="20"/>
       <c r="U52" s="21"/>
       <c r="V52" s="21"/>
       <c r="W52" s="22"/>
-      <c r="X52" s="183"/>
-      <c r="Y52" s="184"/>
-      <c r="Z52" s="185"/>
-      <c r="AA52" s="185"/>
-      <c r="AB52" s="183"/>
-      <c r="AC52" s="184"/>
+      <c r="X52" s="71"/>
+      <c r="Y52" s="72"/>
+      <c r="Z52" s="73"/>
+      <c r="AA52" s="73"/>
+      <c r="AB52" s="71"/>
+      <c r="AC52" s="72"/>
     </row>
     <row r="53" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D53" s="51"/>
@@ -6927,20 +6956,20 @@
       <c r="M53" s="17"/>
       <c r="N53" s="16"/>
       <c r="O53" s="17"/>
-      <c r="P53" s="213"/>
-      <c r="Q53" s="213"/>
-      <c r="R53" s="213"/>
-      <c r="S53" s="213"/>
+      <c r="P53" s="76"/>
+      <c r="Q53" s="76"/>
+      <c r="R53" s="76"/>
+      <c r="S53" s="76"/>
       <c r="T53" s="20"/>
       <c r="U53" s="21"/>
       <c r="V53" s="21"/>
       <c r="W53" s="22"/>
-      <c r="X53" s="183"/>
-      <c r="Y53" s="184"/>
-      <c r="Z53" s="185"/>
-      <c r="AA53" s="185"/>
-      <c r="AB53" s="183"/>
-      <c r="AC53" s="184"/>
+      <c r="X53" s="71"/>
+      <c r="Y53" s="72"/>
+      <c r="Z53" s="73"/>
+      <c r="AA53" s="73"/>
+      <c r="AB53" s="71"/>
+      <c r="AC53" s="72"/>
     </row>
     <row r="54" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D54" s="51"/>
@@ -6955,20 +6984,20 @@
       <c r="M54" s="17"/>
       <c r="N54" s="16"/>
       <c r="O54" s="17"/>
-      <c r="P54" s="213"/>
-      <c r="Q54" s="213"/>
-      <c r="R54" s="213"/>
-      <c r="S54" s="213"/>
+      <c r="P54" s="76"/>
+      <c r="Q54" s="76"/>
+      <c r="R54" s="76"/>
+      <c r="S54" s="76"/>
       <c r="T54" s="20"/>
       <c r="U54" s="21"/>
       <c r="V54" s="21"/>
       <c r="W54" s="22"/>
-      <c r="X54" s="183"/>
-      <c r="Y54" s="184"/>
-      <c r="Z54" s="185"/>
-      <c r="AA54" s="185"/>
-      <c r="AB54" s="183"/>
-      <c r="AC54" s="184"/>
+      <c r="X54" s="71"/>
+      <c r="Y54" s="72"/>
+      <c r="Z54" s="73"/>
+      <c r="AA54" s="73"/>
+      <c r="AB54" s="71"/>
+      <c r="AC54" s="72"/>
     </row>
     <row r="55" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D55" s="51"/>
@@ -6983,20 +7012,20 @@
       <c r="M55" s="17"/>
       <c r="N55" s="16"/>
       <c r="O55" s="17"/>
-      <c r="P55" s="213"/>
-      <c r="Q55" s="213"/>
-      <c r="R55" s="213"/>
-      <c r="S55" s="213"/>
+      <c r="P55" s="76"/>
+      <c r="Q55" s="76"/>
+      <c r="R55" s="76"/>
+      <c r="S55" s="76"/>
       <c r="T55" s="20"/>
       <c r="U55" s="21"/>
       <c r="V55" s="21"/>
       <c r="W55" s="22"/>
-      <c r="X55" s="183"/>
-      <c r="Y55" s="184"/>
-      <c r="Z55" s="185"/>
-      <c r="AA55" s="185"/>
-      <c r="AB55" s="183"/>
-      <c r="AC55" s="184"/>
+      <c r="X55" s="71"/>
+      <c r="Y55" s="72"/>
+      <c r="Z55" s="73"/>
+      <c r="AA55" s="73"/>
+      <c r="AB55" s="71"/>
+      <c r="AC55" s="72"/>
     </row>
     <row r="56" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D56" s="51"/>
@@ -7011,20 +7040,20 @@
       <c r="M56" s="17"/>
       <c r="N56" s="16"/>
       <c r="O56" s="17"/>
-      <c r="P56" s="213"/>
-      <c r="Q56" s="213"/>
-      <c r="R56" s="213"/>
-      <c r="S56" s="213"/>
+      <c r="P56" s="76"/>
+      <c r="Q56" s="76"/>
+      <c r="R56" s="76"/>
+      <c r="S56" s="76"/>
       <c r="T56" s="20"/>
       <c r="U56" s="21"/>
       <c r="V56" s="21"/>
       <c r="W56" s="22"/>
-      <c r="X56" s="183"/>
-      <c r="Y56" s="184"/>
-      <c r="Z56" s="185"/>
-      <c r="AA56" s="185"/>
-      <c r="AB56" s="183"/>
-      <c r="AC56" s="184"/>
+      <c r="X56" s="71"/>
+      <c r="Y56" s="72"/>
+      <c r="Z56" s="73"/>
+      <c r="AA56" s="73"/>
+      <c r="AB56" s="71"/>
+      <c r="AC56" s="72"/>
     </row>
     <row r="57" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D57" s="51"/>
@@ -7039,20 +7068,20 @@
       <c r="M57" s="17"/>
       <c r="N57" s="16"/>
       <c r="O57" s="17"/>
-      <c r="P57" s="213"/>
-      <c r="Q57" s="213"/>
-      <c r="R57" s="213"/>
-      <c r="S57" s="213"/>
+      <c r="P57" s="76"/>
+      <c r="Q57" s="76"/>
+      <c r="R57" s="76"/>
+      <c r="S57" s="76"/>
       <c r="T57" s="20"/>
       <c r="U57" s="21"/>
       <c r="V57" s="21"/>
       <c r="W57" s="22"/>
-      <c r="X57" s="183"/>
-      <c r="Y57" s="184"/>
-      <c r="Z57" s="185"/>
-      <c r="AA57" s="185"/>
-      <c r="AB57" s="183"/>
-      <c r="AC57" s="184"/>
+      <c r="X57" s="71"/>
+      <c r="Y57" s="72"/>
+      <c r="Z57" s="73"/>
+      <c r="AA57" s="73"/>
+      <c r="AB57" s="71"/>
+      <c r="AC57" s="72"/>
     </row>
     <row r="58" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D58" s="51"/>
@@ -7067,20 +7096,20 @@
       <c r="M58" s="17"/>
       <c r="N58" s="16"/>
       <c r="O58" s="17"/>
-      <c r="P58" s="213"/>
-      <c r="Q58" s="213"/>
-      <c r="R58" s="213"/>
-      <c r="S58" s="213"/>
+      <c r="P58" s="76"/>
+      <c r="Q58" s="76"/>
+      <c r="R58" s="76"/>
+      <c r="S58" s="76"/>
       <c r="T58" s="20"/>
       <c r="U58" s="21"/>
       <c r="V58" s="21"/>
       <c r="W58" s="22"/>
-      <c r="X58" s="183"/>
-      <c r="Y58" s="184"/>
-      <c r="Z58" s="185"/>
-      <c r="AA58" s="185"/>
-      <c r="AB58" s="183"/>
-      <c r="AC58" s="184"/>
+      <c r="X58" s="71"/>
+      <c r="Y58" s="72"/>
+      <c r="Z58" s="73"/>
+      <c r="AA58" s="73"/>
+      <c r="AB58" s="71"/>
+      <c r="AC58" s="72"/>
     </row>
     <row r="59" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D59" s="51"/>
@@ -7095,20 +7124,20 @@
       <c r="M59" s="17"/>
       <c r="N59" s="16"/>
       <c r="O59" s="17"/>
-      <c r="P59" s="213"/>
-      <c r="Q59" s="213"/>
-      <c r="R59" s="213"/>
-      <c r="S59" s="213"/>
+      <c r="P59" s="76"/>
+      <c r="Q59" s="76"/>
+      <c r="R59" s="76"/>
+      <c r="S59" s="76"/>
       <c r="T59" s="20"/>
       <c r="U59" s="21"/>
       <c r="V59" s="21"/>
       <c r="W59" s="22"/>
-      <c r="X59" s="183"/>
-      <c r="Y59" s="184"/>
-      <c r="Z59" s="185"/>
-      <c r="AA59" s="185"/>
-      <c r="AB59" s="183"/>
-      <c r="AC59" s="184"/>
+      <c r="X59" s="71"/>
+      <c r="Y59" s="72"/>
+      <c r="Z59" s="73"/>
+      <c r="AA59" s="73"/>
+      <c r="AB59" s="71"/>
+      <c r="AC59" s="72"/>
     </row>
     <row r="60" spans="4:29" x14ac:dyDescent="0.3">
       <c r="D60" s="1"/>
@@ -7123,124 +7152,34 @@
       <c r="M60" s="19"/>
       <c r="N60" s="18"/>
       <c r="O60" s="19"/>
-      <c r="P60" s="212"/>
-      <c r="Q60" s="212"/>
-      <c r="R60" s="212"/>
-      <c r="S60" s="212"/>
+      <c r="P60" s="75"/>
+      <c r="Q60" s="75"/>
+      <c r="R60" s="75"/>
+      <c r="S60" s="75"/>
       <c r="T60" s="23"/>
       <c r="U60" s="4"/>
       <c r="V60" s="4"/>
       <c r="W60" s="5"/>
-      <c r="X60" s="180"/>
-      <c r="Y60" s="181"/>
-      <c r="Z60" s="182"/>
-      <c r="AA60" s="182"/>
-      <c r="AB60" s="180"/>
-      <c r="AC60" s="181"/>
+      <c r="X60" s="68"/>
+      <c r="Y60" s="69"/>
+      <c r="Z60" s="70"/>
+      <c r="AA60" s="70"/>
+      <c r="AB60" s="68"/>
+      <c r="AC60" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="128">
-    <mergeCell ref="X43:Y44"/>
-    <mergeCell ref="Z43:AA44"/>
-    <mergeCell ref="AB43:AC44"/>
-    <mergeCell ref="Z45:AA48"/>
-    <mergeCell ref="X45:Y48"/>
-    <mergeCell ref="X38:Y40"/>
-    <mergeCell ref="Z38:AA40"/>
-    <mergeCell ref="AB38:AC40"/>
-    <mergeCell ref="AB41:AC42"/>
-    <mergeCell ref="Z41:AA42"/>
-    <mergeCell ref="X41:Y42"/>
-    <mergeCell ref="X34:Y35"/>
-    <mergeCell ref="Z34:AA35"/>
-    <mergeCell ref="AB34:AC35"/>
-    <mergeCell ref="AB36:AC37"/>
-    <mergeCell ref="Z36:AA37"/>
-    <mergeCell ref="X36:Y37"/>
-    <mergeCell ref="X30:Y31"/>
-    <mergeCell ref="Z30:AA31"/>
-    <mergeCell ref="AB30:AC31"/>
-    <mergeCell ref="AB32:AC33"/>
-    <mergeCell ref="Z32:AA33"/>
-    <mergeCell ref="X32:Y33"/>
-    <mergeCell ref="X26:Y27"/>
-    <mergeCell ref="Z26:AA27"/>
-    <mergeCell ref="AB26:AC27"/>
-    <mergeCell ref="AB28:AC29"/>
-    <mergeCell ref="Z28:AA29"/>
-    <mergeCell ref="X28:Y29"/>
-    <mergeCell ref="X22:Y23"/>
-    <mergeCell ref="Z22:AA23"/>
-    <mergeCell ref="AB22:AC23"/>
-    <mergeCell ref="AB24:AC25"/>
-    <mergeCell ref="Z24:AA25"/>
-    <mergeCell ref="X24:Y25"/>
-    <mergeCell ref="AB16:AC17"/>
-    <mergeCell ref="X18:Y19"/>
-    <mergeCell ref="Z18:AA19"/>
-    <mergeCell ref="AB18:AC19"/>
-    <mergeCell ref="AB20:AC21"/>
-    <mergeCell ref="Z20:AA21"/>
-    <mergeCell ref="AB7:AC8"/>
-    <mergeCell ref="X9:Y12"/>
-    <mergeCell ref="Z9:AA12"/>
-    <mergeCell ref="AB9:AC12"/>
-    <mergeCell ref="X13:Y15"/>
-    <mergeCell ref="Z13:AA15"/>
-    <mergeCell ref="AB13:AC15"/>
-    <mergeCell ref="X20:Y21"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="X7:Y8"/>
-    <mergeCell ref="Z7:AA8"/>
-    <mergeCell ref="X16:Y17"/>
-    <mergeCell ref="Z16:AA17"/>
-    <mergeCell ref="H2:U2"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="J43:K44"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I8"/>
-    <mergeCell ref="D20:I21"/>
-    <mergeCell ref="D22:I23"/>
-    <mergeCell ref="J28:K29"/>
-    <mergeCell ref="J30:K31"/>
-    <mergeCell ref="J32:K33"/>
-    <mergeCell ref="J34:K35"/>
-    <mergeCell ref="J6:K8"/>
-    <mergeCell ref="J20:K21"/>
-    <mergeCell ref="J22:K23"/>
-    <mergeCell ref="J24:K25"/>
-    <mergeCell ref="D13:I15"/>
-    <mergeCell ref="D43:I44"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D24:I25"/>
-    <mergeCell ref="D28:I29"/>
-    <mergeCell ref="D30:I31"/>
-    <mergeCell ref="D32:I33"/>
-    <mergeCell ref="D34:I35"/>
-    <mergeCell ref="D36:I37"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D18:I19"/>
-    <mergeCell ref="J16:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L7:M8"/>
-    <mergeCell ref="N7:O8"/>
-    <mergeCell ref="P13:S15"/>
-    <mergeCell ref="T9:W12"/>
-    <mergeCell ref="T6:W8"/>
-    <mergeCell ref="D9:I12"/>
-    <mergeCell ref="J9:K12"/>
-    <mergeCell ref="P9:S12"/>
+  <mergeCells count="129">
+    <mergeCell ref="B26:C42"/>
+    <mergeCell ref="J36:K37"/>
+    <mergeCell ref="P36:S37"/>
+    <mergeCell ref="D38:I40"/>
+    <mergeCell ref="J38:K40"/>
+    <mergeCell ref="P38:S40"/>
+    <mergeCell ref="J41:K42"/>
+    <mergeCell ref="J13:K15"/>
+    <mergeCell ref="L13:M15"/>
+    <mergeCell ref="N13:O15"/>
+    <mergeCell ref="B6:C25"/>
     <mergeCell ref="J45:K48"/>
     <mergeCell ref="L45:M48"/>
     <mergeCell ref="AB45:AC48"/>
@@ -7257,17 +7196,108 @@
     <mergeCell ref="J26:K27"/>
     <mergeCell ref="P26:S27"/>
     <mergeCell ref="D41:I42"/>
-    <mergeCell ref="B6:C26"/>
-    <mergeCell ref="B27:C43"/>
-    <mergeCell ref="J36:K37"/>
-    <mergeCell ref="P36:S37"/>
-    <mergeCell ref="D38:I40"/>
-    <mergeCell ref="J38:K40"/>
-    <mergeCell ref="P38:S40"/>
-    <mergeCell ref="J41:K42"/>
-    <mergeCell ref="J13:K15"/>
-    <mergeCell ref="L13:M15"/>
-    <mergeCell ref="N13:O15"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D18:I19"/>
+    <mergeCell ref="J16:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L7:M8"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="P13:S15"/>
+    <mergeCell ref="D9:I12"/>
+    <mergeCell ref="J9:K12"/>
+    <mergeCell ref="P9:S12"/>
+    <mergeCell ref="J43:K44"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I8"/>
+    <mergeCell ref="D20:I21"/>
+    <mergeCell ref="D22:I23"/>
+    <mergeCell ref="J28:K29"/>
+    <mergeCell ref="J30:K31"/>
+    <mergeCell ref="J32:K33"/>
+    <mergeCell ref="J34:K35"/>
+    <mergeCell ref="J6:K8"/>
+    <mergeCell ref="J20:K21"/>
+    <mergeCell ref="J22:K23"/>
+    <mergeCell ref="J24:K25"/>
+    <mergeCell ref="D13:I15"/>
+    <mergeCell ref="D43:I44"/>
+    <mergeCell ref="D24:I25"/>
+    <mergeCell ref="D28:I29"/>
+    <mergeCell ref="D30:I31"/>
+    <mergeCell ref="D32:I33"/>
+    <mergeCell ref="D34:I35"/>
+    <mergeCell ref="D36:I37"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="X7:Y8"/>
+    <mergeCell ref="Z7:AA8"/>
+    <mergeCell ref="X16:Y17"/>
+    <mergeCell ref="Z16:AA17"/>
+    <mergeCell ref="H2:U2"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="T9:W12"/>
+    <mergeCell ref="T6:W8"/>
+    <mergeCell ref="H4:U4"/>
+    <mergeCell ref="AB16:AC17"/>
+    <mergeCell ref="X18:Y19"/>
+    <mergeCell ref="Z18:AA19"/>
+    <mergeCell ref="AB18:AC19"/>
+    <mergeCell ref="AB20:AC21"/>
+    <mergeCell ref="Z20:AA21"/>
+    <mergeCell ref="AB7:AC8"/>
+    <mergeCell ref="X9:Y12"/>
+    <mergeCell ref="Z9:AA12"/>
+    <mergeCell ref="AB9:AC12"/>
+    <mergeCell ref="X13:Y15"/>
+    <mergeCell ref="Z13:AA15"/>
+    <mergeCell ref="AB13:AC15"/>
+    <mergeCell ref="X20:Y21"/>
+    <mergeCell ref="X26:Y27"/>
+    <mergeCell ref="Z26:AA27"/>
+    <mergeCell ref="AB26:AC27"/>
+    <mergeCell ref="AB28:AC29"/>
+    <mergeCell ref="Z28:AA29"/>
+    <mergeCell ref="X28:Y29"/>
+    <mergeCell ref="X22:Y23"/>
+    <mergeCell ref="Z22:AA23"/>
+    <mergeCell ref="AB22:AC23"/>
+    <mergeCell ref="AB24:AC25"/>
+    <mergeCell ref="Z24:AA25"/>
+    <mergeCell ref="X24:Y25"/>
+    <mergeCell ref="X34:Y35"/>
+    <mergeCell ref="Z34:AA35"/>
+    <mergeCell ref="AB34:AC35"/>
+    <mergeCell ref="AB36:AC37"/>
+    <mergeCell ref="Z36:AA37"/>
+    <mergeCell ref="X36:Y37"/>
+    <mergeCell ref="X30:Y31"/>
+    <mergeCell ref="Z30:AA31"/>
+    <mergeCell ref="AB30:AC31"/>
+    <mergeCell ref="AB32:AC33"/>
+    <mergeCell ref="Z32:AA33"/>
+    <mergeCell ref="X32:Y33"/>
+    <mergeCell ref="X43:Y44"/>
+    <mergeCell ref="Z43:AA44"/>
+    <mergeCell ref="AB43:AC44"/>
+    <mergeCell ref="Z45:AA48"/>
+    <mergeCell ref="X45:Y48"/>
+    <mergeCell ref="X38:Y40"/>
+    <mergeCell ref="Z38:AA40"/>
+    <mergeCell ref="AB38:AC40"/>
+    <mergeCell ref="AB41:AC42"/>
+    <mergeCell ref="Z41:AA42"/>
+    <mergeCell ref="X41:Y42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
commit merge user cua Sáng
</commit_message>
<xml_diff>
--- a/Documents/TaskMember.xlsx
+++ b/Documents/TaskMember.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceGit\BusBooking_Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9A1500-4A3F-447C-A2E7-9BDE952B65D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC27B4D-5E90-4415-A70D-7E36289E10C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="302" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,10 +77,6 @@
   </si>
   <si>
     <t>Các Page chi tiết phải có button New, Update, Remove, Search</t>
-  </si>
-  <si>
-    <t>Mã Trung Kiên, 
-Nguyễn Hoàng Sơn</t>
   </si>
   <si>
     <t>Generate mã 6 số kiểm tra khi nhân viên login</t>
@@ -197,6 +193,10 @@
   </si>
   <si>
     <t>Lấy thông tin và insert vào Booking table</t>
+  </si>
+  <si>
+    <t>Mã Trung Kiên, 
+Nguyễn Hồng Sơn</t>
   </si>
 </sst>
 </file>
@@ -621,6 +621,90 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -631,457 +715,373 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1376,7 +1376,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>30480</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1441,7 +1441,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>114300</xdr:colOff>
+          <xdr:colOff>121920</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
@@ -1510,7 +1510,7 @@
           <xdr:col>28</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1575,9 +1575,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>22860</xdr:colOff>
+          <xdr:colOff>30480</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>129540</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1644,7 +1644,7 @@
           <xdr:col>26</xdr:col>
           <xdr:colOff>106680</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1778,7 +1778,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>30480</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1843,7 +1843,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>114300</xdr:colOff>
+          <xdr:colOff>121920</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
@@ -1971,15 +1971,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>428898</xdr:colOff>
+          <xdr:colOff>426720</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>63138</xdr:colOff>
+          <xdr:colOff>68580</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2038,13 +2038,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>25</xdr:col>
-          <xdr:colOff>512718</xdr:colOff>
+          <xdr:colOff>510540</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>15240</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>146958</xdr:colOff>
+          <xdr:colOff>144780</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
@@ -2105,13 +2105,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>550818</xdr:colOff>
+          <xdr:colOff>548640</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>15240</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>185058</xdr:colOff>
+          <xdr:colOff>182880</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>53340</xdr:rowOff>
         </xdr:to>
@@ -2172,13 +2172,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>428898</xdr:colOff>
+          <xdr:colOff>426720</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>63138</xdr:colOff>
+          <xdr:colOff>68580</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
@@ -2239,13 +2239,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>25</xdr:col>
-          <xdr:colOff>512718</xdr:colOff>
+          <xdr:colOff>510540</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>53340</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>146958</xdr:colOff>
+          <xdr:colOff>144780</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>83820</xdr:rowOff>
         </xdr:to>
@@ -2306,15 +2306,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>550818</xdr:colOff>
+          <xdr:colOff>548640</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>53340</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>185058</xdr:colOff>
+          <xdr:colOff>182880</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>91440</xdr:rowOff>
+          <xdr:rowOff>83820</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2373,13 +2373,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>428898</xdr:colOff>
+          <xdr:colOff>426720</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>63138</xdr:colOff>
+          <xdr:colOff>68580</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
@@ -2440,13 +2440,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>25</xdr:col>
-          <xdr:colOff>512718</xdr:colOff>
+          <xdr:colOff>510540</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>53340</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>146958</xdr:colOff>
+          <xdr:colOff>144780</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>83820</xdr:rowOff>
         </xdr:to>
@@ -2507,15 +2507,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>550818</xdr:colOff>
+          <xdr:colOff>548640</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>53340</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>185058</xdr:colOff>
+          <xdr:colOff>182880</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>91440</xdr:rowOff>
+          <xdr:rowOff>83820</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2714,9 +2714,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>190500</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2783,7 +2783,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>91440</xdr:rowOff>
+          <xdr:rowOff>83820</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2848,7 +2848,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>99060</xdr:rowOff>
         </xdr:to>
@@ -2984,7 +2984,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3049,7 +3049,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>24</xdr:row>
           <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
@@ -3185,7 +3185,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3250,7 +3250,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
@@ -3386,7 +3386,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3451,7 +3451,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>28</xdr:row>
           <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
@@ -3587,7 +3587,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3652,7 +3652,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
@@ -3782,13 +3782,13 @@
           <xdr:col>23</xdr:col>
           <xdr:colOff>449580</xdr:colOff>
           <xdr:row>48</xdr:row>
-          <xdr:rowOff>119743</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>49</xdr:row>
-          <xdr:rowOff>157842</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3849,13 +3849,13 @@
           <xdr:col>25</xdr:col>
           <xdr:colOff>533400</xdr:colOff>
           <xdr:row>48</xdr:row>
-          <xdr:rowOff>134983</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>49</xdr:row>
-          <xdr:rowOff>165462</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3916,13 +3916,13 @@
           <xdr:col>27</xdr:col>
           <xdr:colOff>571500</xdr:colOff>
           <xdr:row>48</xdr:row>
-          <xdr:rowOff>134983</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
           <xdr:colOff>205740</xdr:colOff>
           <xdr:row>49</xdr:row>
-          <xdr:rowOff>173082</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3989,7 +3989,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4054,7 +4054,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
@@ -4190,7 +4190,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4255,7 +4255,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>34</xdr:row>
           <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
@@ -4391,7 +4391,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4456,7 +4456,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>36</xdr:row>
           <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
@@ -4592,7 +4592,7 @@
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4657,7 +4657,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>39</xdr:row>
           <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
@@ -4791,7 +4791,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>91440</xdr:colOff>
+          <xdr:colOff>83820</xdr:colOff>
           <xdr:row>41</xdr:row>
           <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
@@ -4858,9 +4858,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>175260</xdr:colOff>
+          <xdr:colOff>182880</xdr:colOff>
           <xdr:row>41</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:rowOff>83820</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4925,7 +4925,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
-          <xdr:colOff>213360</xdr:colOff>
+          <xdr:colOff>220980</xdr:colOff>
           <xdr:row>41</xdr:row>
           <xdr:rowOff>83820</xdr:rowOff>
         </xdr:to>
@@ -5059,9 +5059,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>44</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5260,9 +5260,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>47</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5390,13 +5390,13 @@
           <xdr:col>23</xdr:col>
           <xdr:colOff>449580</xdr:colOff>
           <xdr:row>51</xdr:row>
-          <xdr:rowOff>78377</xdr:rowOff>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
           <xdr:colOff>83820</xdr:colOff>
           <xdr:row>52</xdr:row>
-          <xdr:rowOff>116477</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5406,7 +5406,7 @@
                   <a14:compatExt spid="_x0000_s1085"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C9E2993-10EE-42C1-A125-2AF71F9C466B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5457,13 +5457,13 @@
           <xdr:col>25</xdr:col>
           <xdr:colOff>533400</xdr:colOff>
           <xdr:row>51</xdr:row>
-          <xdr:rowOff>93617</xdr:rowOff>
+          <xdr:rowOff>91440</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>26</xdr:col>
-          <xdr:colOff>167640</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>52</xdr:row>
-          <xdr:rowOff>124097</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5473,7 +5473,7 @@
                   <a14:compatExt spid="_x0000_s1086"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E688482-750F-427C-B8A0-004BA237B25F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5524,13 +5524,13 @@
           <xdr:col>27</xdr:col>
           <xdr:colOff>571500</xdr:colOff>
           <xdr:row>51</xdr:row>
-          <xdr:rowOff>93617</xdr:rowOff>
+          <xdr:rowOff>91440</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>28</xdr:col>
           <xdr:colOff>205740</xdr:colOff>
           <xdr:row>52</xdr:row>
-          <xdr:rowOff>131717</xdr:rowOff>
+          <xdr:rowOff>129540</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5540,7 +5540,7 @@
                   <a14:compatExt spid="_x0000_s1087"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F562702-64BC-49B2-933B-A9C2114C97D1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5852,8 +5852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AC56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20:O21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5871,178 +5871,178 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="21" x14ac:dyDescent="0.4">
-      <c r="H2" s="117" t="s">
+      <c r="H2" s="202" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="117"/>
-      <c r="P2" s="117"/>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="117"/>
-      <c r="S2" s="117"/>
-      <c r="T2" s="117"/>
-      <c r="U2" s="117"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="202"/>
+      <c r="K2" s="202"/>
+      <c r="L2" s="202"/>
+      <c r="M2" s="202"/>
+      <c r="N2" s="202"/>
+      <c r="O2" s="202"/>
+      <c r="P2" s="202"/>
+      <c r="Q2" s="202"/>
+      <c r="R2" s="202"/>
+      <c r="S2" s="202"/>
+      <c r="T2" s="202"/>
+      <c r="U2" s="202"/>
     </row>
     <row r="4" spans="2:29" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="H4" s="138" t="s">
-        <v>41</v>
+      <c r="H4" s="216" t="s">
+        <v>40</v>
       </c>
-      <c r="I4" s="139"/>
-      <c r="J4" s="139"/>
-      <c r="K4" s="139"/>
-      <c r="L4" s="139"/>
-      <c r="M4" s="139"/>
-      <c r="N4" s="139"/>
-      <c r="O4" s="139"/>
-      <c r="P4" s="139"/>
-      <c r="Q4" s="139"/>
-      <c r="R4" s="139"/>
-      <c r="S4" s="139"/>
-      <c r="T4" s="139"/>
-      <c r="U4" s="139"/>
+      <c r="I4" s="217"/>
+      <c r="J4" s="217"/>
+      <c r="K4" s="217"/>
+      <c r="L4" s="217"/>
+      <c r="M4" s="217"/>
+      <c r="N4" s="217"/>
+      <c r="O4" s="217"/>
+      <c r="P4" s="217"/>
+      <c r="Q4" s="217"/>
+      <c r="R4" s="217"/>
+      <c r="S4" s="217"/>
+      <c r="T4" s="217"/>
+      <c r="U4" s="217"/>
     </row>
     <row r="5" spans="2:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="147" t="s">
+      <c r="B5" s="159" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="148"/>
-      <c r="D5" s="127" t="s">
+      <c r="C5" s="160"/>
+      <c r="D5" s="208" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
-      <c r="I5" s="129"/>
-      <c r="J5" s="153" t="s">
+      <c r="E5" s="209"/>
+      <c r="F5" s="209"/>
+      <c r="G5" s="209"/>
+      <c r="H5" s="209"/>
+      <c r="I5" s="210"/>
+      <c r="J5" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="154"/>
-      <c r="L5" s="124" t="s">
+      <c r="K5" s="162"/>
+      <c r="L5" s="163" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="125"/>
-      <c r="N5" s="124" t="s">
+      <c r="M5" s="164"/>
+      <c r="N5" s="163" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="125"/>
-      <c r="P5" s="130" t="s">
-        <v>23</v>
+      <c r="O5" s="164"/>
+      <c r="P5" s="211" t="s">
+        <v>22</v>
       </c>
-      <c r="Q5" s="131"/>
-      <c r="R5" s="131"/>
-      <c r="S5" s="132"/>
-      <c r="T5" s="133" t="s">
+      <c r="Q5" s="212"/>
+      <c r="R5" s="212"/>
+      <c r="S5" s="213"/>
+      <c r="T5" s="214" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="134"/>
-      <c r="V5" s="134"/>
-      <c r="W5" s="134"/>
-      <c r="X5" s="126" t="s">
+      <c r="U5" s="215"/>
+      <c r="V5" s="215"/>
+      <c r="W5" s="215"/>
+      <c r="X5" s="207" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y5" s="206"/>
+      <c r="Z5" s="205" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="123"/>
-      <c r="Z5" s="122" t="s">
+      <c r="AA5" s="206"/>
+      <c r="AB5" s="207" t="s">
         <v>38</v>
       </c>
-      <c r="AA5" s="123"/>
-      <c r="AB5" s="126" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC5" s="123"/>
+      <c r="AC5" s="206"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B6" s="210" t="s">
+      <c r="B6" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="211"/>
-      <c r="D6" s="184" t="s">
+      <c r="C6" s="140"/>
+      <c r="D6" s="191" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="185"/>
-      <c r="F6" s="185"/>
-      <c r="G6" s="185"/>
-      <c r="H6" s="185"/>
-      <c r="I6" s="186"/>
-      <c r="J6" s="149" t="s">
+      <c r="E6" s="192"/>
+      <c r="F6" s="192"/>
+      <c r="G6" s="192"/>
+      <c r="H6" s="192"/>
+      <c r="I6" s="193"/>
+      <c r="J6" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="150"/>
-      <c r="L6" s="118">
+      <c r="K6" s="81"/>
+      <c r="L6" s="203">
         <v>43981</v>
       </c>
-      <c r="M6" s="119"/>
-      <c r="N6" s="118">
+      <c r="M6" s="204"/>
+      <c r="N6" s="203">
         <v>43981</v>
       </c>
-      <c r="O6" s="119"/>
+      <c r="O6" s="204"/>
       <c r="P6" s="56"/>
       <c r="Q6" s="56"/>
       <c r="R6" s="56"/>
       <c r="S6" s="56"/>
-      <c r="T6" s="99"/>
-      <c r="U6" s="100"/>
-      <c r="V6" s="100"/>
-      <c r="W6" s="101"/>
-      <c r="X6" s="120"/>
-      <c r="Y6" s="121"/>
-      <c r="Z6" s="120"/>
-      <c r="AA6" s="121"/>
-      <c r="AB6" s="120"/>
-      <c r="AC6" s="121"/>
+      <c r="T6" s="94"/>
+      <c r="U6" s="95"/>
+      <c r="V6" s="95"/>
+      <c r="W6" s="96"/>
+      <c r="X6" s="200"/>
+      <c r="Y6" s="201"/>
+      <c r="Z6" s="200"/>
+      <c r="AA6" s="201"/>
+      <c r="AB6" s="200"/>
+      <c r="AC6" s="201"/>
     </row>
     <row r="7" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="212"/>
-      <c r="C7" s="213"/>
-      <c r="D7" s="164" t="s">
+      <c r="B7" s="141"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="165"/>
-      <c r="F7" s="165"/>
-      <c r="G7" s="165"/>
-      <c r="H7" s="165"/>
-      <c r="I7" s="166"/>
-      <c r="J7" s="173"/>
-      <c r="K7" s="174"/>
-      <c r="L7" s="82">
+      <c r="E7" s="174"/>
+      <c r="F7" s="174"/>
+      <c r="G7" s="174"/>
+      <c r="H7" s="174"/>
+      <c r="I7" s="175"/>
+      <c r="J7" s="128"/>
+      <c r="K7" s="129"/>
+      <c r="L7" s="84">
         <v>43982</v>
       </c>
-      <c r="M7" s="83"/>
-      <c r="N7" s="82">
+      <c r="M7" s="85"/>
+      <c r="N7" s="84">
         <v>43985</v>
       </c>
-      <c r="O7" s="83"/>
+      <c r="O7" s="85"/>
       <c r="P7" s="58"/>
       <c r="Q7" s="58"/>
       <c r="R7" s="58"/>
       <c r="S7" s="58"/>
-      <c r="T7" s="135"/>
-      <c r="U7" s="136"/>
-      <c r="V7" s="136"/>
-      <c r="W7" s="137"/>
-      <c r="X7" s="105"/>
-      <c r="Y7" s="106"/>
-      <c r="Z7" s="105"/>
-      <c r="AA7" s="106"/>
-      <c r="AB7" s="105"/>
-      <c r="AC7" s="106"/>
+      <c r="T7" s="123"/>
+      <c r="U7" s="124"/>
+      <c r="V7" s="124"/>
+      <c r="W7" s="125"/>
+      <c r="X7" s="100"/>
+      <c r="Y7" s="101"/>
+      <c r="Z7" s="100"/>
+      <c r="AA7" s="101"/>
+      <c r="AB7" s="100"/>
+      <c r="AC7" s="101"/>
     </row>
     <row r="8" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B8" s="212"/>
-      <c r="C8" s="213"/>
-      <c r="D8" s="170"/>
-      <c r="E8" s="171"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="171"/>
-      <c r="H8" s="171"/>
-      <c r="I8" s="172"/>
-      <c r="J8" s="151"/>
-      <c r="K8" s="152"/>
+      <c r="B8" s="141"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="180"/>
+      <c r="G8" s="180"/>
+      <c r="H8" s="180"/>
+      <c r="I8" s="181"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="83"/>
       <c r="L8" s="86"/>
       <c r="M8" s="87"/>
       <c r="N8" s="86"/>
@@ -6051,374 +6051,374 @@
       <c r="Q8" s="57"/>
       <c r="R8" s="57"/>
       <c r="S8" s="57"/>
-      <c r="T8" s="102"/>
-      <c r="U8" s="103"/>
-      <c r="V8" s="103"/>
-      <c r="W8" s="104"/>
-      <c r="X8" s="107"/>
-      <c r="Y8" s="108"/>
-      <c r="Z8" s="107"/>
-      <c r="AA8" s="108"/>
-      <c r="AB8" s="107"/>
-      <c r="AC8" s="108"/>
+      <c r="T8" s="97"/>
+      <c r="U8" s="98"/>
+      <c r="V8" s="98"/>
+      <c r="W8" s="99"/>
+      <c r="X8" s="102"/>
+      <c r="Y8" s="103"/>
+      <c r="Z8" s="102"/>
+      <c r="AA8" s="103"/>
+      <c r="AB8" s="102"/>
+      <c r="AC8" s="103"/>
     </row>
     <row r="9" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="212"/>
-      <c r="C9" s="213"/>
-      <c r="D9" s="164" t="s">
-        <v>19</v>
+      <c r="B9" s="141"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="104" t="s">
+        <v>18</v>
       </c>
-      <c r="E9" s="165"/>
-      <c r="F9" s="165"/>
-      <c r="G9" s="165"/>
-      <c r="H9" s="165"/>
-      <c r="I9" s="166"/>
-      <c r="J9" s="149" t="s">
+      <c r="E9" s="174"/>
+      <c r="F9" s="174"/>
+      <c r="G9" s="174"/>
+      <c r="H9" s="174"/>
+      <c r="I9" s="175"/>
+      <c r="J9" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="150"/>
-      <c r="L9" s="146"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="146"/>
-      <c r="O9" s="83"/>
-      <c r="P9" s="175" t="s">
-        <v>24</v>
+      <c r="K9" s="81"/>
+      <c r="L9" s="158"/>
+      <c r="M9" s="85"/>
+      <c r="N9" s="158"/>
+      <c r="O9" s="85"/>
+      <c r="P9" s="182" t="s">
+        <v>23</v>
       </c>
-      <c r="Q9" s="176"/>
-      <c r="R9" s="176"/>
-      <c r="S9" s="177"/>
-      <c r="T9" s="99"/>
-      <c r="U9" s="100"/>
-      <c r="V9" s="100"/>
-      <c r="W9" s="101"/>
-      <c r="X9" s="105"/>
-      <c r="Y9" s="106"/>
-      <c r="Z9" s="105"/>
-      <c r="AA9" s="106"/>
-      <c r="AB9" s="105"/>
-      <c r="AC9" s="106"/>
+      <c r="Q9" s="183"/>
+      <c r="R9" s="183"/>
+      <c r="S9" s="184"/>
+      <c r="T9" s="94"/>
+      <c r="U9" s="95"/>
+      <c r="V9" s="95"/>
+      <c r="W9" s="96"/>
+      <c r="X9" s="100"/>
+      <c r="Y9" s="101"/>
+      <c r="Z9" s="100"/>
+      <c r="AA9" s="101"/>
+      <c r="AB9" s="100"/>
+      <c r="AC9" s="101"/>
     </row>
     <row r="10" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="212"/>
-      <c r="C10" s="213"/>
-      <c r="D10" s="167"/>
-      <c r="E10" s="168"/>
-      <c r="F10" s="168"/>
-      <c r="G10" s="168"/>
-      <c r="H10" s="168"/>
-      <c r="I10" s="169"/>
-      <c r="J10" s="173"/>
-      <c r="K10" s="174"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="85"/>
-      <c r="N10" s="84"/>
-      <c r="O10" s="85"/>
-      <c r="P10" s="178"/>
-      <c r="Q10" s="179"/>
-      <c r="R10" s="179"/>
-      <c r="S10" s="180"/>
-      <c r="T10" s="135"/>
-      <c r="U10" s="136"/>
-      <c r="V10" s="136"/>
-      <c r="W10" s="137"/>
-      <c r="X10" s="109"/>
-      <c r="Y10" s="110"/>
-      <c r="Z10" s="109"/>
-      <c r="AA10" s="110"/>
-      <c r="AB10" s="109"/>
-      <c r="AC10" s="110"/>
+      <c r="B10" s="141"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="176"/>
+      <c r="E10" s="177"/>
+      <c r="F10" s="177"/>
+      <c r="G10" s="177"/>
+      <c r="H10" s="177"/>
+      <c r="I10" s="178"/>
+      <c r="J10" s="128"/>
+      <c r="K10" s="129"/>
+      <c r="L10" s="136"/>
+      <c r="M10" s="137"/>
+      <c r="N10" s="136"/>
+      <c r="O10" s="137"/>
+      <c r="P10" s="185"/>
+      <c r="Q10" s="186"/>
+      <c r="R10" s="186"/>
+      <c r="S10" s="187"/>
+      <c r="T10" s="123"/>
+      <c r="U10" s="124"/>
+      <c r="V10" s="124"/>
+      <c r="W10" s="125"/>
+      <c r="X10" s="126"/>
+      <c r="Y10" s="127"/>
+      <c r="Z10" s="126"/>
+      <c r="AA10" s="127"/>
+      <c r="AB10" s="126"/>
+      <c r="AC10" s="127"/>
     </row>
     <row r="11" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="212"/>
-      <c r="C11" s="213"/>
-      <c r="D11" s="167"/>
-      <c r="E11" s="168"/>
-      <c r="F11" s="168"/>
-      <c r="G11" s="168"/>
-      <c r="H11" s="168"/>
-      <c r="I11" s="169"/>
-      <c r="J11" s="173"/>
-      <c r="K11" s="174"/>
-      <c r="L11" s="84"/>
-      <c r="M11" s="85"/>
-      <c r="N11" s="84"/>
-      <c r="O11" s="85"/>
-      <c r="P11" s="178"/>
-      <c r="Q11" s="179"/>
-      <c r="R11" s="179"/>
-      <c r="S11" s="180"/>
-      <c r="T11" s="135"/>
-      <c r="U11" s="136"/>
-      <c r="V11" s="136"/>
-      <c r="W11" s="137"/>
-      <c r="X11" s="109"/>
-      <c r="Y11" s="110"/>
-      <c r="Z11" s="109"/>
-      <c r="AA11" s="110"/>
-      <c r="AB11" s="109"/>
-      <c r="AC11" s="110"/>
+      <c r="B11" s="141"/>
+      <c r="C11" s="142"/>
+      <c r="D11" s="176"/>
+      <c r="E11" s="177"/>
+      <c r="F11" s="177"/>
+      <c r="G11" s="177"/>
+      <c r="H11" s="177"/>
+      <c r="I11" s="178"/>
+      <c r="J11" s="128"/>
+      <c r="K11" s="129"/>
+      <c r="L11" s="136"/>
+      <c r="M11" s="137"/>
+      <c r="N11" s="136"/>
+      <c r="O11" s="137"/>
+      <c r="P11" s="185"/>
+      <c r="Q11" s="186"/>
+      <c r="R11" s="186"/>
+      <c r="S11" s="187"/>
+      <c r="T11" s="123"/>
+      <c r="U11" s="124"/>
+      <c r="V11" s="124"/>
+      <c r="W11" s="125"/>
+      <c r="X11" s="126"/>
+      <c r="Y11" s="127"/>
+      <c r="Z11" s="126"/>
+      <c r="AA11" s="127"/>
+      <c r="AB11" s="126"/>
+      <c r="AC11" s="127"/>
     </row>
     <row r="12" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B12" s="212"/>
-      <c r="C12" s="213"/>
-      <c r="D12" s="170"/>
-      <c r="E12" s="171"/>
-      <c r="F12" s="171"/>
-      <c r="G12" s="171"/>
-      <c r="H12" s="171"/>
-      <c r="I12" s="172"/>
-      <c r="J12" s="151"/>
-      <c r="K12" s="152"/>
+      <c r="B12" s="141"/>
+      <c r="C12" s="142"/>
+      <c r="D12" s="179"/>
+      <c r="E12" s="180"/>
+      <c r="F12" s="180"/>
+      <c r="G12" s="180"/>
+      <c r="H12" s="180"/>
+      <c r="I12" s="181"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="83"/>
       <c r="L12" s="86"/>
       <c r="M12" s="87"/>
       <c r="N12" s="86"/>
       <c r="O12" s="87"/>
-      <c r="P12" s="181"/>
-      <c r="Q12" s="182"/>
-      <c r="R12" s="182"/>
-      <c r="S12" s="183"/>
-      <c r="T12" s="102"/>
-      <c r="U12" s="103"/>
-      <c r="V12" s="103"/>
-      <c r="W12" s="104"/>
-      <c r="X12" s="107"/>
-      <c r="Y12" s="108"/>
-      <c r="Z12" s="107"/>
-      <c r="AA12" s="108"/>
-      <c r="AB12" s="107"/>
-      <c r="AC12" s="108"/>
+      <c r="P12" s="188"/>
+      <c r="Q12" s="189"/>
+      <c r="R12" s="189"/>
+      <c r="S12" s="190"/>
+      <c r="T12" s="97"/>
+      <c r="U12" s="98"/>
+      <c r="V12" s="98"/>
+      <c r="W12" s="99"/>
+      <c r="X12" s="102"/>
+      <c r="Y12" s="103"/>
+      <c r="Z12" s="102"/>
+      <c r="AA12" s="103"/>
+      <c r="AB12" s="102"/>
+      <c r="AC12" s="103"/>
     </row>
     <row r="13" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="212"/>
-      <c r="C13" s="213"/>
-      <c r="D13" s="164" t="s">
-        <v>25</v>
+      <c r="B13" s="141"/>
+      <c r="C13" s="142"/>
+      <c r="D13" s="104" t="s">
+        <v>24</v>
       </c>
-      <c r="E13" s="165"/>
-      <c r="F13" s="165"/>
-      <c r="G13" s="165"/>
-      <c r="H13" s="165"/>
-      <c r="I13" s="166"/>
-      <c r="J13" s="196" t="s">
-        <v>17</v>
+      <c r="E13" s="174"/>
+      <c r="F13" s="174"/>
+      <c r="G13" s="174"/>
+      <c r="H13" s="174"/>
+      <c r="I13" s="175"/>
+      <c r="J13" s="108" t="s">
+        <v>54</v>
       </c>
-      <c r="K13" s="197"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="83"/>
-      <c r="N13" s="209"/>
-      <c r="O13" s="83"/>
-      <c r="P13" s="155" t="s">
-        <v>40</v>
+      <c r="K13" s="109"/>
+      <c r="L13" s="84"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="138"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="165" t="s">
+        <v>39</v>
       </c>
-      <c r="Q13" s="156"/>
-      <c r="R13" s="156"/>
-      <c r="S13" s="157"/>
+      <c r="Q13" s="166"/>
+      <c r="R13" s="166"/>
+      <c r="S13" s="167"/>
       <c r="T13" s="26"/>
       <c r="U13" s="27"/>
       <c r="V13" s="27"/>
       <c r="W13" s="28"/>
-      <c r="X13" s="105"/>
-      <c r="Y13" s="106"/>
-      <c r="Z13" s="105"/>
-      <c r="AA13" s="106"/>
-      <c r="AB13" s="105"/>
-      <c r="AC13" s="106"/>
+      <c r="X13" s="100"/>
+      <c r="Y13" s="101"/>
+      <c r="Z13" s="100"/>
+      <c r="AA13" s="101"/>
+      <c r="AB13" s="100"/>
+      <c r="AC13" s="101"/>
     </row>
     <row r="14" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B14" s="212"/>
-      <c r="C14" s="213"/>
-      <c r="D14" s="167"/>
-      <c r="E14" s="168"/>
-      <c r="F14" s="168"/>
-      <c r="G14" s="168"/>
-      <c r="H14" s="168"/>
-      <c r="I14" s="169"/>
-      <c r="J14" s="207"/>
-      <c r="K14" s="208"/>
-      <c r="L14" s="84"/>
-      <c r="M14" s="85"/>
-      <c r="N14" s="84"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="158"/>
-      <c r="Q14" s="159"/>
-      <c r="R14" s="159"/>
-      <c r="S14" s="160"/>
+      <c r="B14" s="141"/>
+      <c r="C14" s="142"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
+      <c r="F14" s="177"/>
+      <c r="G14" s="177"/>
+      <c r="H14" s="177"/>
+      <c r="I14" s="178"/>
+      <c r="J14" s="110"/>
+      <c r="K14" s="111"/>
+      <c r="L14" s="136"/>
+      <c r="M14" s="137"/>
+      <c r="N14" s="136"/>
+      <c r="O14" s="137"/>
+      <c r="P14" s="168"/>
+      <c r="Q14" s="169"/>
+      <c r="R14" s="169"/>
+      <c r="S14" s="170"/>
       <c r="T14" s="26"/>
       <c r="U14" s="27"/>
       <c r="V14" s="27"/>
       <c r="W14" s="28"/>
-      <c r="X14" s="109"/>
-      <c r="Y14" s="110"/>
-      <c r="Z14" s="109"/>
-      <c r="AA14" s="110"/>
-      <c r="AB14" s="109"/>
-      <c r="AC14" s="110"/>
+      <c r="X14" s="126"/>
+      <c r="Y14" s="127"/>
+      <c r="Z14" s="126"/>
+      <c r="AA14" s="127"/>
+      <c r="AB14" s="126"/>
+      <c r="AC14" s="127"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B15" s="212"/>
-      <c r="C15" s="213"/>
-      <c r="D15" s="170"/>
-      <c r="E15" s="171"/>
-      <c r="F15" s="171"/>
-      <c r="G15" s="171"/>
-      <c r="H15" s="171"/>
-      <c r="I15" s="172"/>
-      <c r="J15" s="198"/>
-      <c r="K15" s="199"/>
+      <c r="B15" s="141"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="179"/>
+      <c r="E15" s="180"/>
+      <c r="F15" s="180"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="181"/>
+      <c r="J15" s="112"/>
+      <c r="K15" s="113"/>
       <c r="L15" s="86"/>
       <c r="M15" s="87"/>
       <c r="N15" s="86"/>
       <c r="O15" s="87"/>
-      <c r="P15" s="161"/>
-      <c r="Q15" s="162"/>
-      <c r="R15" s="162"/>
-      <c r="S15" s="163"/>
+      <c r="P15" s="171"/>
+      <c r="Q15" s="172"/>
+      <c r="R15" s="172"/>
+      <c r="S15" s="173"/>
       <c r="T15" s="26"/>
       <c r="U15" s="27"/>
       <c r="V15" s="27"/>
       <c r="W15" s="28"/>
-      <c r="X15" s="107"/>
-      <c r="Y15" s="108"/>
-      <c r="Z15" s="107"/>
-      <c r="AA15" s="108"/>
-      <c r="AB15" s="107"/>
-      <c r="AC15" s="108"/>
+      <c r="X15" s="102"/>
+      <c r="Y15" s="103"/>
+      <c r="Z15" s="102"/>
+      <c r="AA15" s="103"/>
+      <c r="AB15" s="102"/>
+      <c r="AC15" s="103"/>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B16" s="212"/>
-      <c r="C16" s="213"/>
-      <c r="D16" s="164" t="s">
-        <v>20</v>
+      <c r="B16" s="141"/>
+      <c r="C16" s="142"/>
+      <c r="D16" s="104" t="s">
+        <v>19</v>
       </c>
-      <c r="E16" s="165"/>
-      <c r="F16" s="165"/>
-      <c r="G16" s="165"/>
-      <c r="H16" s="165"/>
-      <c r="I16" s="166"/>
-      <c r="J16" s="149" t="s">
+      <c r="E16" s="174"/>
+      <c r="F16" s="174"/>
+      <c r="G16" s="174"/>
+      <c r="H16" s="174"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="150"/>
-      <c r="L16" s="146"/>
-      <c r="M16" s="83"/>
-      <c r="N16" s="146"/>
-      <c r="O16" s="83"/>
-      <c r="P16" s="187" t="s">
-        <v>27</v>
+      <c r="K16" s="81"/>
+      <c r="L16" s="158"/>
+      <c r="M16" s="85"/>
+      <c r="N16" s="158"/>
+      <c r="O16" s="85"/>
+      <c r="P16" s="88" t="s">
+        <v>26</v>
       </c>
-      <c r="Q16" s="188"/>
-      <c r="R16" s="188"/>
-      <c r="S16" s="189"/>
+      <c r="Q16" s="89"/>
+      <c r="R16" s="89"/>
+      <c r="S16" s="90"/>
       <c r="T16" s="43"/>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="7"/>
-      <c r="X16" s="105"/>
-      <c r="Y16" s="106"/>
-      <c r="Z16" s="105"/>
-      <c r="AA16" s="106"/>
-      <c r="AB16" s="105"/>
-      <c r="AC16" s="106"/>
+      <c r="X16" s="100"/>
+      <c r="Y16" s="101"/>
+      <c r="Z16" s="100"/>
+      <c r="AA16" s="101"/>
+      <c r="AB16" s="100"/>
+      <c r="AC16" s="101"/>
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B17" s="212"/>
-      <c r="C17" s="213"/>
-      <c r="D17" s="170"/>
-      <c r="E17" s="171"/>
-      <c r="F17" s="171"/>
-      <c r="G17" s="171"/>
-      <c r="H17" s="171"/>
-      <c r="I17" s="172"/>
-      <c r="J17" s="151"/>
-      <c r="K17" s="152"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="142"/>
+      <c r="D17" s="179"/>
+      <c r="E17" s="180"/>
+      <c r="F17" s="180"/>
+      <c r="G17" s="180"/>
+      <c r="H17" s="180"/>
+      <c r="I17" s="181"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="83"/>
       <c r="L17" s="86"/>
       <c r="M17" s="87"/>
       <c r="N17" s="86"/>
       <c r="O17" s="87"/>
-      <c r="P17" s="190"/>
-      <c r="Q17" s="191"/>
-      <c r="R17" s="191"/>
-      <c r="S17" s="192"/>
+      <c r="P17" s="91"/>
+      <c r="Q17" s="92"/>
+      <c r="R17" s="92"/>
+      <c r="S17" s="93"/>
       <c r="T17" s="44"/>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
       <c r="W17" s="9"/>
-      <c r="X17" s="107"/>
-      <c r="Y17" s="108"/>
-      <c r="Z17" s="107"/>
-      <c r="AA17" s="108"/>
-      <c r="AB17" s="107"/>
-      <c r="AC17" s="108"/>
+      <c r="X17" s="102"/>
+      <c r="Y17" s="103"/>
+      <c r="Z17" s="102"/>
+      <c r="AA17" s="103"/>
+      <c r="AB17" s="102"/>
+      <c r="AC17" s="103"/>
     </row>
     <row r="18" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B18" s="212"/>
-      <c r="C18" s="213"/>
+      <c r="B18" s="141"/>
+      <c r="C18" s="142"/>
       <c r="D18" s="74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="75"/>
       <c r="F18" s="75"/>
       <c r="G18" s="75"/>
       <c r="H18" s="75"/>
       <c r="I18" s="76"/>
-      <c r="J18" s="149" t="s">
+      <c r="J18" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="150"/>
+      <c r="K18" s="81"/>
       <c r="L18" s="54"/>
       <c r="M18" s="55"/>
       <c r="N18" s="54"/>
       <c r="O18" s="55"/>
-      <c r="P18" s="187" t="s">
-        <v>29</v>
+      <c r="P18" s="88" t="s">
+        <v>28</v>
       </c>
-      <c r="Q18" s="188"/>
-      <c r="R18" s="188"/>
-      <c r="S18" s="189"/>
+      <c r="Q18" s="89"/>
+      <c r="R18" s="89"/>
+      <c r="S18" s="90"/>
       <c r="T18" s="26"/>
       <c r="U18" s="27"/>
       <c r="V18" s="27"/>
       <c r="W18" s="28"/>
-      <c r="X18" s="105"/>
-      <c r="Y18" s="106"/>
-      <c r="Z18" s="105"/>
-      <c r="AA18" s="106"/>
-      <c r="AB18" s="105"/>
-      <c r="AC18" s="106"/>
+      <c r="X18" s="100"/>
+      <c r="Y18" s="101"/>
+      <c r="Z18" s="100"/>
+      <c r="AA18" s="101"/>
+      <c r="AB18" s="100"/>
+      <c r="AC18" s="101"/>
     </row>
     <row r="19" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B19" s="212"/>
-      <c r="C19" s="213"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="90"/>
-      <c r="J19" s="151"/>
-      <c r="K19" s="152"/>
+      <c r="B19" s="141"/>
+      <c r="C19" s="142"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="83"/>
       <c r="L19" s="54"/>
       <c r="M19" s="55"/>
       <c r="N19" s="54"/>
       <c r="O19" s="55"/>
-      <c r="P19" s="190"/>
-      <c r="Q19" s="191"/>
-      <c r="R19" s="191"/>
-      <c r="S19" s="192"/>
+      <c r="P19" s="91"/>
+      <c r="Q19" s="92"/>
+      <c r="R19" s="92"/>
+      <c r="S19" s="93"/>
       <c r="T19" s="26"/>
       <c r="U19" s="27"/>
       <c r="V19" s="27"/>
       <c r="W19" s="28"/>
-      <c r="X19" s="107"/>
-      <c r="Y19" s="108"/>
-      <c r="Z19" s="107"/>
-      <c r="AA19" s="108"/>
-      <c r="AB19" s="107"/>
-      <c r="AC19" s="108"/>
+      <c r="X19" s="102"/>
+      <c r="Y19" s="103"/>
+      <c r="Z19" s="102"/>
+      <c r="AA19" s="103"/>
+      <c r="AB19" s="102"/>
+      <c r="AC19" s="103"/>
     </row>
     <row r="20" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B20" s="212"/>
-      <c r="C20" s="213"/>
+      <c r="B20" s="141"/>
+      <c r="C20" s="142"/>
       <c r="D20" s="74" t="s">
         <v>11</v>
       </c>
@@ -6427,68 +6427,68 @@
       <c r="G20" s="75"/>
       <c r="H20" s="75"/>
       <c r="I20" s="76"/>
-      <c r="J20" s="149" t="s">
+      <c r="J20" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="150"/>
-      <c r="L20" s="216">
+      <c r="K20" s="81"/>
+      <c r="L20" s="114">
         <v>43982</v>
       </c>
-      <c r="M20" s="217"/>
-      <c r="N20" s="216">
+      <c r="M20" s="145"/>
+      <c r="N20" s="114">
         <v>43984</v>
       </c>
-      <c r="O20" s="217"/>
-      <c r="P20" s="93" t="s">
-        <v>28</v>
+      <c r="O20" s="145"/>
+      <c r="P20" s="130" t="s">
+        <v>27</v>
       </c>
-      <c r="Q20" s="94"/>
-      <c r="R20" s="94"/>
-      <c r="S20" s="95"/>
+      <c r="Q20" s="131"/>
+      <c r="R20" s="131"/>
+      <c r="S20" s="132"/>
       <c r="T20" s="43"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="7"/>
-      <c r="X20" s="105"/>
-      <c r="Y20" s="106"/>
-      <c r="Z20" s="105"/>
-      <c r="AA20" s="106"/>
-      <c r="AB20" s="105"/>
-      <c r="AC20" s="106"/>
+      <c r="X20" s="100"/>
+      <c r="Y20" s="101"/>
+      <c r="Z20" s="100"/>
+      <c r="AA20" s="101"/>
+      <c r="AB20" s="100"/>
+      <c r="AC20" s="101"/>
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B21" s="212"/>
-      <c r="C21" s="213"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="89"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="90"/>
-      <c r="J21" s="151"/>
-      <c r="K21" s="152"/>
-      <c r="L21" s="218"/>
-      <c r="M21" s="219"/>
-      <c r="N21" s="218"/>
-      <c r="O21" s="219"/>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="97"/>
-      <c r="R21" s="97"/>
-      <c r="S21" s="98"/>
+      <c r="B21" s="141"/>
+      <c r="C21" s="142"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="83"/>
+      <c r="L21" s="146"/>
+      <c r="M21" s="147"/>
+      <c r="N21" s="146"/>
+      <c r="O21" s="147"/>
+      <c r="P21" s="133"/>
+      <c r="Q21" s="134"/>
+      <c r="R21" s="134"/>
+      <c r="S21" s="135"/>
       <c r="T21" s="44"/>
       <c r="U21" s="8"/>
       <c r="V21" s="8"/>
       <c r="W21" s="9"/>
-      <c r="X21" s="107"/>
-      <c r="Y21" s="108"/>
-      <c r="Z21" s="107"/>
-      <c r="AA21" s="108"/>
-      <c r="AB21" s="107"/>
-      <c r="AC21" s="108"/>
+      <c r="X21" s="102"/>
+      <c r="Y21" s="103"/>
+      <c r="Z21" s="102"/>
+      <c r="AA21" s="103"/>
+      <c r="AB21" s="102"/>
+      <c r="AC21" s="103"/>
     </row>
     <row r="22" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B22" s="212"/>
-      <c r="C22" s="213"/>
+      <c r="B22" s="141"/>
+      <c r="C22" s="142"/>
       <c r="D22" s="74" t="s">
         <v>7</v>
       </c>
@@ -6497,10 +6497,10 @@
       <c r="G22" s="75"/>
       <c r="H22" s="75"/>
       <c r="I22" s="76"/>
-      <c r="J22" s="149" t="s">
+      <c r="J22" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="K22" s="150"/>
+      <c r="K22" s="81"/>
       <c r="L22" s="14"/>
       <c r="M22" s="15"/>
       <c r="N22" s="14"/>
@@ -6513,24 +6513,24 @@
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="7"/>
-      <c r="X22" s="105"/>
-      <c r="Y22" s="106"/>
-      <c r="Z22" s="105"/>
-      <c r="AA22" s="106"/>
-      <c r="AB22" s="105"/>
-      <c r="AC22" s="106"/>
+      <c r="X22" s="100"/>
+      <c r="Y22" s="101"/>
+      <c r="Z22" s="100"/>
+      <c r="AA22" s="101"/>
+      <c r="AB22" s="100"/>
+      <c r="AC22" s="101"/>
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B23" s="212"/>
-      <c r="C23" s="213"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="89"/>
-      <c r="I23" s="90"/>
-      <c r="J23" s="151"/>
-      <c r="K23" s="152"/>
+      <c r="B23" s="141"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="82"/>
+      <c r="K23" s="83"/>
       <c r="L23" s="18"/>
       <c r="M23" s="19"/>
       <c r="N23" s="18"/>
@@ -6543,16 +6543,16 @@
       <c r="U23" s="8"/>
       <c r="V23" s="8"/>
       <c r="W23" s="9"/>
-      <c r="X23" s="107"/>
-      <c r="Y23" s="108"/>
-      <c r="Z23" s="107"/>
-      <c r="AA23" s="108"/>
-      <c r="AB23" s="107"/>
-      <c r="AC23" s="108"/>
+      <c r="X23" s="102"/>
+      <c r="Y23" s="103"/>
+      <c r="Z23" s="102"/>
+      <c r="AA23" s="103"/>
+      <c r="AB23" s="102"/>
+      <c r="AC23" s="103"/>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B24" s="212"/>
-      <c r="C24" s="213"/>
+      <c r="B24" s="141"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="74" t="s">
         <v>9</v>
       </c>
@@ -6561,10 +6561,10 @@
       <c r="G24" s="75"/>
       <c r="H24" s="75"/>
       <c r="I24" s="76"/>
-      <c r="J24" s="149" t="s">
+      <c r="J24" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="150"/>
+      <c r="K24" s="81"/>
       <c r="L24" s="14"/>
       <c r="M24" s="15"/>
       <c r="N24" s="14"/>
@@ -6577,24 +6577,24 @@
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="7"/>
-      <c r="X24" s="105"/>
-      <c r="Y24" s="106"/>
-      <c r="Z24" s="105"/>
-      <c r="AA24" s="106"/>
-      <c r="AB24" s="105"/>
-      <c r="AC24" s="106"/>
+      <c r="X24" s="100"/>
+      <c r="Y24" s="101"/>
+      <c r="Z24" s="100"/>
+      <c r="AA24" s="101"/>
+      <c r="AB24" s="100"/>
+      <c r="AC24" s="101"/>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B25" s="214"/>
-      <c r="C25" s="215"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="89"/>
-      <c r="H25" s="89"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="151"/>
-      <c r="K25" s="152"/>
+      <c r="B25" s="143"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="83"/>
       <c r="L25" s="18"/>
       <c r="M25" s="19"/>
       <c r="N25" s="18"/>
@@ -6607,228 +6607,228 @@
       <c r="U25" s="8"/>
       <c r="V25" s="8"/>
       <c r="W25" s="9"/>
-      <c r="X25" s="107"/>
-      <c r="Y25" s="108"/>
-      <c r="Z25" s="107"/>
-      <c r="AA25" s="108"/>
-      <c r="AB25" s="107"/>
-      <c r="AC25" s="108"/>
+      <c r="X25" s="102"/>
+      <c r="Y25" s="103"/>
+      <c r="Z25" s="102"/>
+      <c r="AA25" s="103"/>
+      <c r="AB25" s="102"/>
+      <c r="AC25" s="103"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B26" s="200" t="s">
-        <v>36</v>
+      <c r="B26" s="148" t="s">
+        <v>35</v>
       </c>
-      <c r="C26" s="201"/>
+      <c r="C26" s="149"/>
       <c r="D26" s="74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E26" s="75"/>
       <c r="F26" s="75"/>
       <c r="G26" s="75"/>
       <c r="H26" s="75"/>
       <c r="I26" s="76"/>
-      <c r="J26" s="196" t="s">
-        <v>17</v>
+      <c r="J26" s="108" t="s">
+        <v>54</v>
       </c>
-      <c r="K26" s="150"/>
-      <c r="L26" s="216"/>
-      <c r="M26" s="217"/>
-      <c r="N26" s="216"/>
-      <c r="O26" s="217"/>
-      <c r="P26" s="187" t="s">
-        <v>44</v>
+      <c r="K26" s="81"/>
+      <c r="L26" s="114"/>
+      <c r="M26" s="145"/>
+      <c r="N26" s="114"/>
+      <c r="O26" s="145"/>
+      <c r="P26" s="88" t="s">
+        <v>43</v>
       </c>
-      <c r="Q26" s="188"/>
-      <c r="R26" s="188"/>
-      <c r="S26" s="189"/>
+      <c r="Q26" s="89"/>
+      <c r="R26" s="89"/>
+      <c r="S26" s="90"/>
       <c r="T26" s="26"/>
       <c r="U26" s="27"/>
       <c r="V26" s="27"/>
       <c r="W26" s="28"/>
-      <c r="X26" s="105"/>
-      <c r="Y26" s="106"/>
-      <c r="Z26" s="105"/>
-      <c r="AA26" s="106"/>
-      <c r="AB26" s="105"/>
-      <c r="AC26" s="106"/>
+      <c r="X26" s="100"/>
+      <c r="Y26" s="101"/>
+      <c r="Z26" s="100"/>
+      <c r="AA26" s="101"/>
+      <c r="AB26" s="100"/>
+      <c r="AC26" s="101"/>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B27" s="202"/>
-      <c r="C27" s="203"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
-      <c r="H27" s="89"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="151"/>
-      <c r="K27" s="152"/>
-      <c r="L27" s="218"/>
-      <c r="M27" s="219"/>
-      <c r="N27" s="218"/>
-      <c r="O27" s="219"/>
-      <c r="P27" s="190"/>
-      <c r="Q27" s="191"/>
-      <c r="R27" s="191"/>
-      <c r="S27" s="192"/>
+      <c r="B27" s="150"/>
+      <c r="C27" s="151"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="83"/>
+      <c r="L27" s="146"/>
+      <c r="M27" s="147"/>
+      <c r="N27" s="146"/>
+      <c r="O27" s="147"/>
+      <c r="P27" s="91"/>
+      <c r="Q27" s="92"/>
+      <c r="R27" s="92"/>
+      <c r="S27" s="93"/>
       <c r="T27" s="26"/>
       <c r="U27" s="27"/>
       <c r="V27" s="27"/>
       <c r="W27" s="28"/>
-      <c r="X27" s="107"/>
-      <c r="Y27" s="108"/>
-      <c r="Z27" s="107"/>
-      <c r="AA27" s="108"/>
-      <c r="AB27" s="107"/>
-      <c r="AC27" s="108"/>
+      <c r="X27" s="102"/>
+      <c r="Y27" s="103"/>
+      <c r="Z27" s="102"/>
+      <c r="AA27" s="103"/>
+      <c r="AB27" s="102"/>
+      <c r="AC27" s="103"/>
     </row>
     <row r="28" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B28" s="202"/>
-      <c r="C28" s="203"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="151"/>
       <c r="D28" s="74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" s="75"/>
       <c r="F28" s="75"/>
       <c r="G28" s="75"/>
       <c r="H28" s="75"/>
       <c r="I28" s="76"/>
-      <c r="J28" s="149" t="s">
+      <c r="J28" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="K28" s="150"/>
-      <c r="L28" s="216"/>
-      <c r="M28" s="217"/>
-      <c r="N28" s="216"/>
-      <c r="O28" s="217"/>
-      <c r="P28" s="93"/>
-      <c r="Q28" s="94"/>
-      <c r="R28" s="94"/>
-      <c r="S28" s="95"/>
+      <c r="K28" s="81"/>
+      <c r="L28" s="114"/>
+      <c r="M28" s="145"/>
+      <c r="N28" s="114"/>
+      <c r="O28" s="145"/>
+      <c r="P28" s="130"/>
+      <c r="Q28" s="131"/>
+      <c r="R28" s="131"/>
+      <c r="S28" s="132"/>
       <c r="T28" s="43"/>
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
       <c r="W28" s="7"/>
-      <c r="X28" s="105"/>
-      <c r="Y28" s="106"/>
-      <c r="Z28" s="105"/>
-      <c r="AA28" s="106"/>
-      <c r="AB28" s="105"/>
-      <c r="AC28" s="106"/>
+      <c r="X28" s="100"/>
+      <c r="Y28" s="101"/>
+      <c r="Z28" s="100"/>
+      <c r="AA28" s="101"/>
+      <c r="AB28" s="100"/>
+      <c r="AC28" s="101"/>
     </row>
     <row r="29" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="202"/>
-      <c r="C29" s="203"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="89"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="89"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="151"/>
-      <c r="K29" s="152"/>
-      <c r="L29" s="218"/>
-      <c r="M29" s="219"/>
-      <c r="N29" s="218"/>
-      <c r="O29" s="219"/>
-      <c r="P29" s="96"/>
-      <c r="Q29" s="97"/>
-      <c r="R29" s="97"/>
-      <c r="S29" s="98"/>
+      <c r="B29" s="150"/>
+      <c r="C29" s="151"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="83"/>
+      <c r="L29" s="146"/>
+      <c r="M29" s="147"/>
+      <c r="N29" s="146"/>
+      <c r="O29" s="147"/>
+      <c r="P29" s="133"/>
+      <c r="Q29" s="134"/>
+      <c r="R29" s="134"/>
+      <c r="S29" s="135"/>
       <c r="T29" s="44"/>
       <c r="U29" s="8"/>
       <c r="V29" s="8"/>
       <c r="W29" s="9"/>
-      <c r="X29" s="107"/>
-      <c r="Y29" s="108"/>
-      <c r="Z29" s="107"/>
-      <c r="AA29" s="108"/>
-      <c r="AB29" s="107"/>
-      <c r="AC29" s="108"/>
+      <c r="X29" s="102"/>
+      <c r="Y29" s="103"/>
+      <c r="Z29" s="102"/>
+      <c r="AA29" s="103"/>
+      <c r="AB29" s="102"/>
+      <c r="AC29" s="103"/>
     </row>
     <row r="30" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B30" s="202"/>
-      <c r="C30" s="203"/>
-      <c r="D30" s="140" t="s">
+      <c r="B30" s="150"/>
+      <c r="C30" s="151"/>
+      <c r="D30" s="194" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="141"/>
-      <c r="F30" s="141"/>
-      <c r="G30" s="141"/>
-      <c r="H30" s="141"/>
-      <c r="I30" s="142"/>
-      <c r="J30" s="149"/>
-      <c r="K30" s="150"/>
+      <c r="E30" s="195"/>
+      <c r="F30" s="195"/>
+      <c r="G30" s="195"/>
+      <c r="H30" s="195"/>
+      <c r="I30" s="196"/>
+      <c r="J30" s="80"/>
+      <c r="K30" s="81"/>
       <c r="L30" s="14"/>
       <c r="M30" s="15"/>
       <c r="N30" s="14"/>
       <c r="O30" s="15"/>
-      <c r="P30" s="93" t="s">
-        <v>26</v>
+      <c r="P30" s="130" t="s">
+        <v>25</v>
       </c>
-      <c r="Q30" s="94"/>
-      <c r="R30" s="94"/>
-      <c r="S30" s="95"/>
+      <c r="Q30" s="131"/>
+      <c r="R30" s="131"/>
+      <c r="S30" s="132"/>
       <c r="T30" s="43"/>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
       <c r="W30" s="7"/>
-      <c r="X30" s="105"/>
-      <c r="Y30" s="106"/>
-      <c r="Z30" s="105"/>
-      <c r="AA30" s="106"/>
-      <c r="AB30" s="105"/>
-      <c r="AC30" s="106"/>
+      <c r="X30" s="100"/>
+      <c r="Y30" s="101"/>
+      <c r="Z30" s="100"/>
+      <c r="AA30" s="101"/>
+      <c r="AB30" s="100"/>
+      <c r="AC30" s="101"/>
     </row>
     <row r="31" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B31" s="202"/>
-      <c r="C31" s="203"/>
-      <c r="D31" s="143"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="144"/>
-      <c r="H31" s="144"/>
-      <c r="I31" s="145"/>
-      <c r="J31" s="151"/>
-      <c r="K31" s="152"/>
+      <c r="B31" s="150"/>
+      <c r="C31" s="151"/>
+      <c r="D31" s="197"/>
+      <c r="E31" s="198"/>
+      <c r="F31" s="198"/>
+      <c r="G31" s="198"/>
+      <c r="H31" s="198"/>
+      <c r="I31" s="199"/>
+      <c r="J31" s="82"/>
+      <c r="K31" s="83"/>
       <c r="L31" s="18"/>
       <c r="M31" s="19"/>
       <c r="N31" s="18"/>
       <c r="O31" s="19"/>
-      <c r="P31" s="96"/>
-      <c r="Q31" s="97"/>
-      <c r="R31" s="97"/>
-      <c r="S31" s="98"/>
+      <c r="P31" s="133"/>
+      <c r="Q31" s="134"/>
+      <c r="R31" s="134"/>
+      <c r="S31" s="135"/>
       <c r="T31" s="44"/>
       <c r="U31" s="8"/>
       <c r="V31" s="8"/>
       <c r="W31" s="9"/>
-      <c r="X31" s="107"/>
-      <c r="Y31" s="108"/>
-      <c r="Z31" s="107"/>
-      <c r="AA31" s="108"/>
-      <c r="AB31" s="107"/>
-      <c r="AC31" s="108"/>
+      <c r="X31" s="102"/>
+      <c r="Y31" s="103"/>
+      <c r="Z31" s="102"/>
+      <c r="AA31" s="103"/>
+      <c r="AB31" s="102"/>
+      <c r="AC31" s="103"/>
     </row>
     <row r="32" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B32" s="202"/>
-      <c r="C32" s="203"/>
+      <c r="B32" s="150"/>
+      <c r="C32" s="151"/>
       <c r="D32" s="74" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E32" s="75"/>
       <c r="F32" s="75"/>
       <c r="G32" s="75"/>
       <c r="H32" s="75"/>
       <c r="I32" s="76"/>
-      <c r="J32" s="149" t="s">
+      <c r="J32" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="150"/>
-      <c r="L32" s="146"/>
-      <c r="M32" s="83"/>
-      <c r="N32" s="146"/>
-      <c r="O32" s="83"/>
+      <c r="K32" s="81"/>
+      <c r="L32" s="158"/>
+      <c r="M32" s="85"/>
+      <c r="N32" s="158"/>
+      <c r="O32" s="85"/>
       <c r="P32" s="70"/>
       <c r="Q32" s="70"/>
       <c r="R32" s="70"/>
@@ -6837,24 +6837,24 @@
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
       <c r="W32" s="7"/>
-      <c r="X32" s="105"/>
-      <c r="Y32" s="106"/>
-      <c r="Z32" s="105"/>
-      <c r="AA32" s="106"/>
-      <c r="AB32" s="105"/>
-      <c r="AC32" s="106"/>
+      <c r="X32" s="100"/>
+      <c r="Y32" s="101"/>
+      <c r="Z32" s="100"/>
+      <c r="AA32" s="101"/>
+      <c r="AB32" s="100"/>
+      <c r="AC32" s="101"/>
     </row>
     <row r="33" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B33" s="202"/>
-      <c r="C33" s="203"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="89"/>
-      <c r="G33" s="89"/>
-      <c r="H33" s="89"/>
-      <c r="I33" s="90"/>
-      <c r="J33" s="151"/>
-      <c r="K33" s="152"/>
+      <c r="B33" s="150"/>
+      <c r="C33" s="151"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="78"/>
+      <c r="H33" s="78"/>
+      <c r="I33" s="79"/>
+      <c r="J33" s="82"/>
+      <c r="K33" s="83"/>
       <c r="L33" s="86"/>
       <c r="M33" s="87"/>
       <c r="N33" s="86"/>
@@ -6867,190 +6867,190 @@
       <c r="U33" s="8"/>
       <c r="V33" s="8"/>
       <c r="W33" s="9"/>
-      <c r="X33" s="107"/>
-      <c r="Y33" s="108"/>
-      <c r="Z33" s="107"/>
-      <c r="AA33" s="108"/>
-      <c r="AB33" s="107"/>
-      <c r="AC33" s="108"/>
+      <c r="X33" s="102"/>
+      <c r="Y33" s="103"/>
+      <c r="Z33" s="102"/>
+      <c r="AA33" s="103"/>
+      <c r="AB33" s="102"/>
+      <c r="AC33" s="103"/>
     </row>
     <row r="34" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B34" s="202"/>
-      <c r="C34" s="203"/>
+      <c r="B34" s="150"/>
+      <c r="C34" s="151"/>
       <c r="D34" s="74" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E34" s="75"/>
       <c r="F34" s="75"/>
       <c r="G34" s="75"/>
       <c r="H34" s="75"/>
       <c r="I34" s="76"/>
-      <c r="J34" s="149" t="s">
+      <c r="J34" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="K34" s="150"/>
+      <c r="K34" s="81"/>
       <c r="L34" s="29"/>
       <c r="M34" s="30"/>
       <c r="N34" s="29"/>
       <c r="O34" s="30"/>
-      <c r="P34" s="93" t="s">
-        <v>33</v>
+      <c r="P34" s="130" t="s">
+        <v>32</v>
       </c>
-      <c r="Q34" s="94"/>
-      <c r="R34" s="94"/>
-      <c r="S34" s="95"/>
+      <c r="Q34" s="131"/>
+      <c r="R34" s="131"/>
+      <c r="S34" s="132"/>
       <c r="T34" s="45"/>
       <c r="U34" s="46"/>
       <c r="V34" s="46"/>
       <c r="W34" s="47"/>
-      <c r="X34" s="111"/>
-      <c r="Y34" s="112"/>
-      <c r="Z34" s="111"/>
-      <c r="AA34" s="112"/>
-      <c r="AB34" s="111"/>
-      <c r="AC34" s="112"/>
+      <c r="X34" s="218"/>
+      <c r="Y34" s="219"/>
+      <c r="Z34" s="218"/>
+      <c r="AA34" s="219"/>
+      <c r="AB34" s="218"/>
+      <c r="AC34" s="219"/>
     </row>
     <row r="35" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B35" s="202"/>
-      <c r="C35" s="203"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
-      <c r="I35" s="90"/>
-      <c r="J35" s="173"/>
-      <c r="K35" s="174"/>
+      <c r="B35" s="150"/>
+      <c r="C35" s="151"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="78"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="128"/>
+      <c r="K35" s="129"/>
       <c r="L35" s="34"/>
       <c r="M35" s="35"/>
       <c r="N35" s="34"/>
       <c r="O35" s="35"/>
-      <c r="P35" s="96"/>
-      <c r="Q35" s="97"/>
-      <c r="R35" s="97"/>
-      <c r="S35" s="98"/>
+      <c r="P35" s="133"/>
+      <c r="Q35" s="134"/>
+      <c r="R35" s="134"/>
+      <c r="S35" s="135"/>
       <c r="T35" s="48"/>
       <c r="U35" s="49"/>
       <c r="V35" s="49"/>
       <c r="W35" s="50"/>
-      <c r="X35" s="115"/>
-      <c r="Y35" s="116"/>
-      <c r="Z35" s="115"/>
-      <c r="AA35" s="116"/>
-      <c r="AB35" s="115"/>
-      <c r="AC35" s="116"/>
+      <c r="X35" s="220"/>
+      <c r="Y35" s="221"/>
+      <c r="Z35" s="220"/>
+      <c r="AA35" s="221"/>
+      <c r="AB35" s="220"/>
+      <c r="AC35" s="221"/>
     </row>
     <row r="36" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B36" s="202"/>
-      <c r="C36" s="203"/>
+      <c r="B36" s="150"/>
+      <c r="C36" s="151"/>
       <c r="D36" s="74" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E36" s="75"/>
       <c r="F36" s="75"/>
       <c r="G36" s="75"/>
       <c r="H36" s="75"/>
       <c r="I36" s="76"/>
-      <c r="J36" s="149" t="s">
+      <c r="J36" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="150"/>
+      <c r="K36" s="81"/>
       <c r="L36" s="29"/>
       <c r="M36" s="30"/>
       <c r="N36" s="29"/>
       <c r="O36" s="30"/>
-      <c r="P36" s="187" t="s">
-        <v>35</v>
+      <c r="P36" s="88" t="s">
+        <v>34</v>
       </c>
-      <c r="Q36" s="188"/>
-      <c r="R36" s="188"/>
-      <c r="S36" s="189"/>
+      <c r="Q36" s="89"/>
+      <c r="R36" s="89"/>
+      <c r="S36" s="90"/>
       <c r="T36" s="31"/>
       <c r="U36" s="32"/>
       <c r="V36" s="32"/>
       <c r="W36" s="33"/>
-      <c r="X36" s="111"/>
-      <c r="Y36" s="112"/>
-      <c r="Z36" s="111"/>
-      <c r="AA36" s="112"/>
-      <c r="AB36" s="111"/>
-      <c r="AC36" s="112"/>
+      <c r="X36" s="218"/>
+      <c r="Y36" s="219"/>
+      <c r="Z36" s="218"/>
+      <c r="AA36" s="219"/>
+      <c r="AB36" s="218"/>
+      <c r="AC36" s="219"/>
     </row>
     <row r="37" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B37" s="202"/>
-      <c r="C37" s="203"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="173"/>
-      <c r="K37" s="174"/>
+      <c r="B37" s="150"/>
+      <c r="C37" s="151"/>
+      <c r="D37" s="105"/>
+      <c r="E37" s="106"/>
+      <c r="F37" s="106"/>
+      <c r="G37" s="106"/>
+      <c r="H37" s="106"/>
+      <c r="I37" s="107"/>
+      <c r="J37" s="128"/>
+      <c r="K37" s="129"/>
       <c r="L37" s="59"/>
       <c r="M37" s="60"/>
       <c r="N37" s="59"/>
       <c r="O37" s="60"/>
-      <c r="P37" s="204"/>
-      <c r="Q37" s="205"/>
-      <c r="R37" s="205"/>
-      <c r="S37" s="206"/>
+      <c r="P37" s="120"/>
+      <c r="Q37" s="121"/>
+      <c r="R37" s="121"/>
+      <c r="S37" s="122"/>
       <c r="T37" s="61"/>
       <c r="U37" s="62"/>
       <c r="V37" s="62"/>
       <c r="W37" s="63"/>
-      <c r="X37" s="113"/>
-      <c r="Y37" s="114"/>
-      <c r="Z37" s="113"/>
-      <c r="AA37" s="114"/>
-      <c r="AB37" s="113"/>
-      <c r="AC37" s="114"/>
+      <c r="X37" s="222"/>
+      <c r="Y37" s="223"/>
+      <c r="Z37" s="222"/>
+      <c r="AA37" s="223"/>
+      <c r="AB37" s="222"/>
+      <c r="AC37" s="223"/>
     </row>
     <row r="38" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B38" s="202"/>
-      <c r="C38" s="203"/>
-      <c r="D38" s="88"/>
-      <c r="E38" s="89"/>
-      <c r="F38" s="89"/>
-      <c r="G38" s="89"/>
-      <c r="H38" s="89"/>
-      <c r="I38" s="90"/>
-      <c r="J38" s="151"/>
-      <c r="K38" s="152"/>
+      <c r="B38" s="150"/>
+      <c r="C38" s="151"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="78"/>
+      <c r="H38" s="78"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="82"/>
+      <c r="K38" s="83"/>
       <c r="L38" s="59"/>
       <c r="M38" s="60"/>
       <c r="N38" s="59"/>
       <c r="O38" s="60"/>
-      <c r="P38" s="204"/>
-      <c r="Q38" s="205"/>
-      <c r="R38" s="205"/>
-      <c r="S38" s="206"/>
+      <c r="P38" s="120"/>
+      <c r="Q38" s="121"/>
+      <c r="R38" s="121"/>
+      <c r="S38" s="122"/>
       <c r="T38" s="36"/>
       <c r="U38" s="37"/>
       <c r="V38" s="37"/>
       <c r="W38" s="38"/>
-      <c r="X38" s="115"/>
-      <c r="Y38" s="116"/>
-      <c r="Z38" s="115"/>
-      <c r="AA38" s="116"/>
-      <c r="AB38" s="115"/>
-      <c r="AC38" s="116"/>
+      <c r="X38" s="220"/>
+      <c r="Y38" s="221"/>
+      <c r="Z38" s="220"/>
+      <c r="AA38" s="221"/>
+      <c r="AB38" s="220"/>
+      <c r="AC38" s="221"/>
     </row>
     <row r="39" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="202"/>
-      <c r="C39" s="203"/>
+      <c r="B39" s="150"/>
+      <c r="C39" s="151"/>
       <c r="D39" s="74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E39" s="75"/>
       <c r="F39" s="75"/>
       <c r="G39" s="75"/>
       <c r="H39" s="75"/>
       <c r="I39" s="76"/>
-      <c r="J39" s="149" t="s">
+      <c r="J39" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="K39" s="150"/>
+      <c r="K39" s="81"/>
       <c r="L39" s="39"/>
       <c r="M39" s="40"/>
       <c r="N39" s="39"/>
@@ -7063,24 +7063,24 @@
       <c r="U39" s="6"/>
       <c r="V39" s="6"/>
       <c r="W39" s="7"/>
-      <c r="X39" s="105"/>
-      <c r="Y39" s="106"/>
-      <c r="Z39" s="105"/>
-      <c r="AA39" s="106"/>
-      <c r="AB39" s="105"/>
-      <c r="AC39" s="106"/>
+      <c r="X39" s="100"/>
+      <c r="Y39" s="101"/>
+      <c r="Z39" s="100"/>
+      <c r="AA39" s="101"/>
+      <c r="AB39" s="100"/>
+      <c r="AC39" s="101"/>
     </row>
     <row r="40" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B40" s="202"/>
-      <c r="C40" s="203"/>
-      <c r="D40" s="88"/>
-      <c r="E40" s="89"/>
-      <c r="F40" s="89"/>
-      <c r="G40" s="89"/>
-      <c r="H40" s="89"/>
-      <c r="I40" s="90"/>
-      <c r="J40" s="151"/>
-      <c r="K40" s="152"/>
+      <c r="B40" s="150"/>
+      <c r="C40" s="151"/>
+      <c r="D40" s="77"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="78"/>
+      <c r="H40" s="78"/>
+      <c r="I40" s="79"/>
+      <c r="J40" s="82"/>
+      <c r="K40" s="83"/>
       <c r="L40" s="41"/>
       <c r="M40" s="42"/>
       <c r="N40" s="41"/>
@@ -7093,444 +7093,444 @@
       <c r="U40" s="8"/>
       <c r="V40" s="8"/>
       <c r="W40" s="9"/>
-      <c r="X40" s="107"/>
-      <c r="Y40" s="108"/>
-      <c r="Z40" s="107"/>
-      <c r="AA40" s="108"/>
-      <c r="AB40" s="107"/>
-      <c r="AC40" s="108"/>
+      <c r="X40" s="102"/>
+      <c r="Y40" s="103"/>
+      <c r="Z40" s="102"/>
+      <c r="AA40" s="103"/>
+      <c r="AB40" s="102"/>
+      <c r="AC40" s="103"/>
     </row>
     <row r="41" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B41" s="220" t="s">
-        <v>45</v>
+      <c r="B41" s="152" t="s">
+        <v>44</v>
       </c>
-      <c r="C41" s="221"/>
+      <c r="C41" s="153"/>
       <c r="D41" s="75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E41" s="75"/>
       <c r="F41" s="75"/>
       <c r="G41" s="75"/>
       <c r="H41" s="75"/>
       <c r="I41" s="76"/>
-      <c r="J41" s="149" t="s">
+      <c r="J41" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="K41" s="150"/>
+      <c r="K41" s="81"/>
       <c r="L41" s="39"/>
       <c r="M41" s="40"/>
       <c r="N41" s="39"/>
       <c r="O41" s="40"/>
-      <c r="P41" s="187" t="s">
-        <v>30</v>
+      <c r="P41" s="88" t="s">
+        <v>29</v>
       </c>
-      <c r="Q41" s="188"/>
-      <c r="R41" s="188"/>
-      <c r="S41" s="189"/>
+      <c r="Q41" s="89"/>
+      <c r="R41" s="89"/>
+      <c r="S41" s="90"/>
       <c r="T41" s="43"/>
       <c r="U41" s="6"/>
       <c r="V41" s="6"/>
       <c r="W41" s="7"/>
-      <c r="X41" s="105"/>
-      <c r="Y41" s="106"/>
-      <c r="Z41" s="105"/>
-      <c r="AA41" s="106"/>
-      <c r="AB41" s="105"/>
-      <c r="AC41" s="106"/>
+      <c r="X41" s="100"/>
+      <c r="Y41" s="101"/>
+      <c r="Z41" s="100"/>
+      <c r="AA41" s="101"/>
+      <c r="AB41" s="100"/>
+      <c r="AC41" s="101"/>
     </row>
     <row r="42" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B42" s="222"/>
-      <c r="C42" s="223"/>
-      <c r="D42" s="89"/>
-      <c r="E42" s="89"/>
-      <c r="F42" s="89"/>
-      <c r="G42" s="89"/>
-      <c r="H42" s="89"/>
-      <c r="I42" s="90"/>
-      <c r="J42" s="151"/>
-      <c r="K42" s="152"/>
+      <c r="B42" s="154"/>
+      <c r="C42" s="155"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="78"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="78"/>
+      <c r="H42" s="78"/>
+      <c r="I42" s="79"/>
+      <c r="J42" s="82"/>
+      <c r="K42" s="83"/>
       <c r="L42" s="41"/>
       <c r="M42" s="42"/>
       <c r="N42" s="41"/>
       <c r="O42" s="42"/>
-      <c r="P42" s="190"/>
-      <c r="Q42" s="191"/>
-      <c r="R42" s="191"/>
-      <c r="S42" s="192"/>
+      <c r="P42" s="91"/>
+      <c r="Q42" s="92"/>
+      <c r="R42" s="92"/>
+      <c r="S42" s="93"/>
       <c r="T42" s="44"/>
       <c r="U42" s="8"/>
       <c r="V42" s="8"/>
       <c r="W42" s="9"/>
-      <c r="X42" s="107"/>
-      <c r="Y42" s="108"/>
-      <c r="Z42" s="107"/>
-      <c r="AA42" s="108"/>
-      <c r="AB42" s="107"/>
-      <c r="AC42" s="108"/>
+      <c r="X42" s="102"/>
+      <c r="Y42" s="103"/>
+      <c r="Z42" s="102"/>
+      <c r="AA42" s="103"/>
+      <c r="AB42" s="102"/>
+      <c r="AC42" s="103"/>
     </row>
     <row r="43" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B43" s="222"/>
-      <c r="C43" s="223"/>
+      <c r="B43" s="154"/>
+      <c r="C43" s="155"/>
       <c r="D43" s="75" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E43" s="75"/>
       <c r="F43" s="75"/>
       <c r="G43" s="75"/>
       <c r="H43" s="75"/>
       <c r="I43" s="76"/>
-      <c r="J43" s="149" t="s">
+      <c r="J43" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="K43" s="150"/>
-      <c r="L43" s="146"/>
-      <c r="M43" s="83"/>
+      <c r="K43" s="81"/>
+      <c r="L43" s="158"/>
+      <c r="M43" s="85"/>
       <c r="N43" s="39"/>
       <c r="O43" s="40"/>
-      <c r="P43" s="93" t="s">
-        <v>31</v>
+      <c r="P43" s="130" t="s">
+        <v>30</v>
       </c>
-      <c r="Q43" s="94"/>
-      <c r="R43" s="94"/>
-      <c r="S43" s="95"/>
-      <c r="T43" s="99"/>
-      <c r="U43" s="100"/>
-      <c r="V43" s="100"/>
-      <c r="W43" s="101"/>
-      <c r="X43" s="105"/>
-      <c r="Y43" s="106"/>
-      <c r="Z43" s="105"/>
-      <c r="AA43" s="106"/>
-      <c r="AB43" s="105"/>
-      <c r="AC43" s="106"/>
+      <c r="Q43" s="131"/>
+      <c r="R43" s="131"/>
+      <c r="S43" s="132"/>
+      <c r="T43" s="94"/>
+      <c r="U43" s="95"/>
+      <c r="V43" s="95"/>
+      <c r="W43" s="96"/>
+      <c r="X43" s="100"/>
+      <c r="Y43" s="101"/>
+      <c r="Z43" s="100"/>
+      <c r="AA43" s="101"/>
+      <c r="AB43" s="100"/>
+      <c r="AC43" s="101"/>
     </row>
     <row r="44" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B44" s="222"/>
-      <c r="C44" s="223"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="79"/>
-      <c r="J44" s="173"/>
-      <c r="K44" s="174"/>
-      <c r="L44" s="84"/>
-      <c r="M44" s="85"/>
+      <c r="B44" s="154"/>
+      <c r="C44" s="155"/>
+      <c r="D44" s="106"/>
+      <c r="E44" s="106"/>
+      <c r="F44" s="106"/>
+      <c r="G44" s="106"/>
+      <c r="H44" s="106"/>
+      <c r="I44" s="107"/>
+      <c r="J44" s="128"/>
+      <c r="K44" s="129"/>
+      <c r="L44" s="136"/>
+      <c r="M44" s="137"/>
       <c r="N44" s="24"/>
       <c r="O44" s="25"/>
-      <c r="P44" s="193"/>
-      <c r="Q44" s="194"/>
-      <c r="R44" s="194"/>
-      <c r="S44" s="195"/>
-      <c r="T44" s="135"/>
-      <c r="U44" s="136"/>
-      <c r="V44" s="136"/>
-      <c r="W44" s="137"/>
-      <c r="X44" s="109"/>
-      <c r="Y44" s="110"/>
-      <c r="Z44" s="109"/>
-      <c r="AA44" s="110"/>
-      <c r="AB44" s="109"/>
-      <c r="AC44" s="110"/>
+      <c r="P44" s="224"/>
+      <c r="Q44" s="225"/>
+      <c r="R44" s="225"/>
+      <c r="S44" s="226"/>
+      <c r="T44" s="123"/>
+      <c r="U44" s="124"/>
+      <c r="V44" s="124"/>
+      <c r="W44" s="125"/>
+      <c r="X44" s="126"/>
+      <c r="Y44" s="127"/>
+      <c r="Z44" s="126"/>
+      <c r="AA44" s="127"/>
+      <c r="AB44" s="126"/>
+      <c r="AC44" s="127"/>
     </row>
     <row r="45" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B45" s="222"/>
-      <c r="C45" s="223"/>
-      <c r="D45" s="78"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="78"/>
-      <c r="G45" s="78"/>
-      <c r="H45" s="78"/>
-      <c r="I45" s="79"/>
-      <c r="J45" s="173"/>
-      <c r="K45" s="174"/>
-      <c r="L45" s="84"/>
-      <c r="M45" s="85"/>
+      <c r="B45" s="154"/>
+      <c r="C45" s="155"/>
+      <c r="D45" s="106"/>
+      <c r="E45" s="106"/>
+      <c r="F45" s="106"/>
+      <c r="G45" s="106"/>
+      <c r="H45" s="106"/>
+      <c r="I45" s="107"/>
+      <c r="J45" s="128"/>
+      <c r="K45" s="129"/>
+      <c r="L45" s="136"/>
+      <c r="M45" s="137"/>
       <c r="N45" s="24"/>
       <c r="O45" s="25"/>
-      <c r="P45" s="193"/>
-      <c r="Q45" s="194"/>
-      <c r="R45" s="194"/>
-      <c r="S45" s="195"/>
-      <c r="T45" s="135"/>
-      <c r="U45" s="136"/>
-      <c r="V45" s="136"/>
-      <c r="W45" s="137"/>
-      <c r="X45" s="109"/>
-      <c r="Y45" s="110"/>
-      <c r="Z45" s="109"/>
-      <c r="AA45" s="110"/>
-      <c r="AB45" s="109"/>
-      <c r="AC45" s="110"/>
+      <c r="P45" s="224"/>
+      <c r="Q45" s="225"/>
+      <c r="R45" s="225"/>
+      <c r="S45" s="226"/>
+      <c r="T45" s="123"/>
+      <c r="U45" s="124"/>
+      <c r="V45" s="124"/>
+      <c r="W45" s="125"/>
+      <c r="X45" s="126"/>
+      <c r="Y45" s="127"/>
+      <c r="Z45" s="126"/>
+      <c r="AA45" s="127"/>
+      <c r="AB45" s="126"/>
+      <c r="AC45" s="127"/>
     </row>
     <row r="46" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B46" s="222"/>
-      <c r="C46" s="223"/>
-      <c r="D46" s="89"/>
-      <c r="E46" s="89"/>
-      <c r="F46" s="89"/>
-      <c r="G46" s="89"/>
-      <c r="H46" s="89"/>
-      <c r="I46" s="90"/>
-      <c r="J46" s="151"/>
-      <c r="K46" s="152"/>
+      <c r="B46" s="154"/>
+      <c r="C46" s="155"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="78"/>
+      <c r="F46" s="78"/>
+      <c r="G46" s="78"/>
+      <c r="H46" s="78"/>
+      <c r="I46" s="79"/>
+      <c r="J46" s="82"/>
+      <c r="K46" s="83"/>
       <c r="L46" s="86"/>
       <c r="M46" s="87"/>
       <c r="N46" s="41"/>
       <c r="O46" s="42"/>
-      <c r="P46" s="96"/>
-      <c r="Q46" s="97"/>
-      <c r="R46" s="97"/>
-      <c r="S46" s="98"/>
-      <c r="T46" s="102"/>
-      <c r="U46" s="103"/>
-      <c r="V46" s="103"/>
-      <c r="W46" s="104"/>
-      <c r="X46" s="107"/>
-      <c r="Y46" s="108"/>
-      <c r="Z46" s="107"/>
-      <c r="AA46" s="108"/>
-      <c r="AB46" s="107"/>
-      <c r="AC46" s="108"/>
+      <c r="P46" s="133"/>
+      <c r="Q46" s="134"/>
+      <c r="R46" s="134"/>
+      <c r="S46" s="135"/>
+      <c r="T46" s="97"/>
+      <c r="U46" s="98"/>
+      <c r="V46" s="98"/>
+      <c r="W46" s="99"/>
+      <c r="X46" s="102"/>
+      <c r="Y46" s="103"/>
+      <c r="Z46" s="102"/>
+      <c r="AA46" s="103"/>
+      <c r="AB46" s="102"/>
+      <c r="AC46" s="103"/>
     </row>
     <row r="47" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="222"/>
-      <c r="C47" s="223"/>
+      <c r="B47" s="154"/>
+      <c r="C47" s="155"/>
       <c r="D47" s="75" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E47" s="75"/>
       <c r="F47" s="75"/>
       <c r="G47" s="75"/>
       <c r="H47" s="75"/>
       <c r="I47" s="76"/>
-      <c r="J47" s="80" t="s">
-        <v>17</v>
+      <c r="J47" s="227" t="s">
+        <v>54</v>
       </c>
-      <c r="K47" s="81"/>
-      <c r="L47" s="82">
+      <c r="K47" s="228"/>
+      <c r="L47" s="84">
         <v>43982</v>
       </c>
-      <c r="M47" s="83"/>
-      <c r="N47" s="82">
+      <c r="M47" s="85"/>
+      <c r="N47" s="84">
         <v>43983</v>
       </c>
-      <c r="O47" s="83"/>
-      <c r="P47" s="93" t="s">
-        <v>42</v>
+      <c r="O47" s="85"/>
+      <c r="P47" s="130" t="s">
+        <v>41</v>
       </c>
-      <c r="Q47" s="94"/>
-      <c r="R47" s="94"/>
-      <c r="S47" s="95"/>
-      <c r="T47" s="99"/>
-      <c r="U47" s="100"/>
-      <c r="V47" s="100"/>
-      <c r="W47" s="101"/>
-      <c r="X47" s="105"/>
-      <c r="Y47" s="106"/>
-      <c r="Z47" s="105"/>
-      <c r="AA47" s="106"/>
-      <c r="AB47" s="105"/>
-      <c r="AC47" s="106"/>
+      <c r="Q47" s="131"/>
+      <c r="R47" s="131"/>
+      <c r="S47" s="132"/>
+      <c r="T47" s="94"/>
+      <c r="U47" s="95"/>
+      <c r="V47" s="95"/>
+      <c r="W47" s="96"/>
+      <c r="X47" s="100"/>
+      <c r="Y47" s="101"/>
+      <c r="Z47" s="100"/>
+      <c r="AA47" s="101"/>
+      <c r="AB47" s="100"/>
+      <c r="AC47" s="101"/>
     </row>
     <row r="48" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B48" s="222"/>
-      <c r="C48" s="223"/>
-      <c r="D48" s="89"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="89"/>
-      <c r="G48" s="89"/>
-      <c r="H48" s="89"/>
-      <c r="I48" s="90"/>
-      <c r="J48" s="91"/>
-      <c r="K48" s="92"/>
+      <c r="B48" s="154"/>
+      <c r="C48" s="155"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="79"/>
+      <c r="J48" s="229"/>
+      <c r="K48" s="230"/>
       <c r="L48" s="86"/>
       <c r="M48" s="87"/>
       <c r="N48" s="86"/>
       <c r="O48" s="87"/>
-      <c r="P48" s="96"/>
-      <c r="Q48" s="97"/>
-      <c r="R48" s="97"/>
-      <c r="S48" s="98"/>
-      <c r="T48" s="102"/>
-      <c r="U48" s="103"/>
-      <c r="V48" s="103"/>
-      <c r="W48" s="104"/>
-      <c r="X48" s="107"/>
-      <c r="Y48" s="108"/>
-      <c r="Z48" s="107"/>
-      <c r="AA48" s="108"/>
-      <c r="AB48" s="107"/>
-      <c r="AC48" s="108"/>
+      <c r="P48" s="133"/>
+      <c r="Q48" s="134"/>
+      <c r="R48" s="134"/>
+      <c r="S48" s="135"/>
+      <c r="T48" s="97"/>
+      <c r="U48" s="98"/>
+      <c r="V48" s="98"/>
+      <c r="W48" s="99"/>
+      <c r="X48" s="102"/>
+      <c r="Y48" s="103"/>
+      <c r="Z48" s="102"/>
+      <c r="AA48" s="103"/>
+      <c r="AB48" s="102"/>
+      <c r="AC48" s="103"/>
     </row>
     <row r="49" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B49" s="222"/>
-      <c r="C49" s="223"/>
-      <c r="D49" s="164" t="s">
-        <v>52</v>
+      <c r="B49" s="154"/>
+      <c r="C49" s="155"/>
+      <c r="D49" s="104" t="s">
+        <v>51</v>
       </c>
       <c r="E49" s="75"/>
       <c r="F49" s="75"/>
       <c r="G49" s="75"/>
       <c r="H49" s="75"/>
       <c r="I49" s="76"/>
-      <c r="J49" s="196" t="s">
-        <v>17</v>
+      <c r="J49" s="108" t="s">
+        <v>54</v>
       </c>
-      <c r="K49" s="197"/>
-      <c r="L49" s="216">
+      <c r="K49" s="109"/>
+      <c r="L49" s="114">
         <v>43984</v>
       </c>
-      <c r="M49" s="226"/>
-      <c r="N49" s="216">
+      <c r="M49" s="115"/>
+      <c r="N49" s="114">
         <v>43986</v>
       </c>
-      <c r="O49" s="226"/>
-      <c r="P49" s="187" t="s">
-        <v>46</v>
+      <c r="O49" s="115"/>
+      <c r="P49" s="88" t="s">
+        <v>45</v>
       </c>
-      <c r="Q49" s="188"/>
-      <c r="R49" s="188"/>
-      <c r="S49" s="189"/>
-      <c r="T49" s="99"/>
-      <c r="U49" s="100"/>
-      <c r="V49" s="100"/>
-      <c r="W49" s="101"/>
-      <c r="X49" s="105"/>
-      <c r="Y49" s="106"/>
-      <c r="Z49" s="105"/>
-      <c r="AA49" s="106"/>
-      <c r="AB49" s="105"/>
-      <c r="AC49" s="106"/>
+      <c r="Q49" s="89"/>
+      <c r="R49" s="89"/>
+      <c r="S49" s="90"/>
+      <c r="T49" s="94"/>
+      <c r="U49" s="95"/>
+      <c r="V49" s="95"/>
+      <c r="W49" s="96"/>
+      <c r="X49" s="100"/>
+      <c r="Y49" s="101"/>
+      <c r="Z49" s="100"/>
+      <c r="AA49" s="101"/>
+      <c r="AB49" s="100"/>
+      <c r="AC49" s="101"/>
     </row>
     <row r="50" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B50" s="222"/>
-      <c r="C50" s="223"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="78"/>
-      <c r="F50" s="78"/>
-      <c r="G50" s="78"/>
-      <c r="H50" s="78"/>
-      <c r="I50" s="79"/>
-      <c r="J50" s="207"/>
-      <c r="K50" s="208"/>
-      <c r="L50" s="227"/>
-      <c r="M50" s="228"/>
-      <c r="N50" s="227"/>
-      <c r="O50" s="228"/>
-      <c r="P50" s="204"/>
-      <c r="Q50" s="205"/>
-      <c r="R50" s="205"/>
-      <c r="S50" s="206"/>
-      <c r="T50" s="135"/>
-      <c r="U50" s="136"/>
-      <c r="V50" s="136"/>
-      <c r="W50" s="137"/>
-      <c r="X50" s="109"/>
-      <c r="Y50" s="110"/>
-      <c r="Z50" s="109"/>
-      <c r="AA50" s="110"/>
-      <c r="AB50" s="109"/>
-      <c r="AC50" s="110"/>
+      <c r="B50" s="154"/>
+      <c r="C50" s="155"/>
+      <c r="D50" s="105"/>
+      <c r="E50" s="106"/>
+      <c r="F50" s="106"/>
+      <c r="G50" s="106"/>
+      <c r="H50" s="106"/>
+      <c r="I50" s="107"/>
+      <c r="J50" s="110"/>
+      <c r="K50" s="111"/>
+      <c r="L50" s="116"/>
+      <c r="M50" s="117"/>
+      <c r="N50" s="116"/>
+      <c r="O50" s="117"/>
+      <c r="P50" s="120"/>
+      <c r="Q50" s="121"/>
+      <c r="R50" s="121"/>
+      <c r="S50" s="122"/>
+      <c r="T50" s="123"/>
+      <c r="U50" s="124"/>
+      <c r="V50" s="124"/>
+      <c r="W50" s="125"/>
+      <c r="X50" s="126"/>
+      <c r="Y50" s="127"/>
+      <c r="Z50" s="126"/>
+      <c r="AA50" s="127"/>
+      <c r="AB50" s="126"/>
+      <c r="AC50" s="127"/>
     </row>
     <row r="51" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="222"/>
-      <c r="C51" s="223"/>
-      <c r="D51" s="88"/>
-      <c r="E51" s="89"/>
-      <c r="F51" s="89"/>
-      <c r="G51" s="89"/>
-      <c r="H51" s="89"/>
-      <c r="I51" s="90"/>
-      <c r="J51" s="198"/>
-      <c r="K51" s="199"/>
-      <c r="L51" s="229"/>
-      <c r="M51" s="230"/>
-      <c r="N51" s="229"/>
-      <c r="O51" s="230"/>
-      <c r="P51" s="190"/>
-      <c r="Q51" s="191"/>
-      <c r="R51" s="191"/>
-      <c r="S51" s="192"/>
-      <c r="T51" s="102"/>
-      <c r="U51" s="103"/>
-      <c r="V51" s="103"/>
-      <c r="W51" s="104"/>
-      <c r="X51" s="107"/>
-      <c r="Y51" s="108"/>
-      <c r="Z51" s="107"/>
-      <c r="AA51" s="108"/>
-      <c r="AB51" s="107"/>
-      <c r="AC51" s="108"/>
+      <c r="B51" s="154"/>
+      <c r="C51" s="155"/>
+      <c r="D51" s="77"/>
+      <c r="E51" s="78"/>
+      <c r="F51" s="78"/>
+      <c r="G51" s="78"/>
+      <c r="H51" s="78"/>
+      <c r="I51" s="79"/>
+      <c r="J51" s="112"/>
+      <c r="K51" s="113"/>
+      <c r="L51" s="118"/>
+      <c r="M51" s="119"/>
+      <c r="N51" s="118"/>
+      <c r="O51" s="119"/>
+      <c r="P51" s="91"/>
+      <c r="Q51" s="92"/>
+      <c r="R51" s="92"/>
+      <c r="S51" s="93"/>
+      <c r="T51" s="97"/>
+      <c r="U51" s="98"/>
+      <c r="V51" s="98"/>
+      <c r="W51" s="99"/>
+      <c r="X51" s="102"/>
+      <c r="Y51" s="103"/>
+      <c r="Z51" s="102"/>
+      <c r="AA51" s="103"/>
+      <c r="AB51" s="102"/>
+      <c r="AC51" s="103"/>
     </row>
     <row r="52" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B52" s="224"/>
-      <c r="C52" s="225"/>
+      <c r="B52" s="156"/>
+      <c r="C52" s="157"/>
       <c r="D52" s="74" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E52" s="75"/>
       <c r="F52" s="75"/>
       <c r="G52" s="75"/>
       <c r="H52" s="75"/>
       <c r="I52" s="76"/>
-      <c r="J52" s="149" t="s">
-        <v>50</v>
+      <c r="J52" s="80" t="s">
+        <v>49</v>
       </c>
-      <c r="K52" s="150"/>
-      <c r="L52" s="82">
+      <c r="K52" s="81"/>
+      <c r="L52" s="84">
         <v>43986</v>
       </c>
-      <c r="M52" s="83"/>
-      <c r="N52" s="82">
+      <c r="M52" s="85"/>
+      <c r="N52" s="84">
         <v>43986</v>
       </c>
-      <c r="O52" s="83"/>
-      <c r="P52" s="187" t="s">
-        <v>54</v>
+      <c r="O52" s="85"/>
+      <c r="P52" s="88" t="s">
+        <v>53</v>
       </c>
-      <c r="Q52" s="188"/>
-      <c r="R52" s="188"/>
-      <c r="S52" s="189"/>
-      <c r="T52" s="99"/>
-      <c r="U52" s="100"/>
-      <c r="V52" s="100"/>
-      <c r="W52" s="101"/>
-      <c r="X52" s="105"/>
-      <c r="Y52" s="106"/>
-      <c r="Z52" s="105"/>
-      <c r="AA52" s="106"/>
-      <c r="AB52" s="105"/>
-      <c r="AC52" s="106"/>
+      <c r="Q52" s="89"/>
+      <c r="R52" s="89"/>
+      <c r="S52" s="90"/>
+      <c r="T52" s="94"/>
+      <c r="U52" s="95"/>
+      <c r="V52" s="95"/>
+      <c r="W52" s="96"/>
+      <c r="X52" s="100"/>
+      <c r="Y52" s="101"/>
+      <c r="Z52" s="100"/>
+      <c r="AA52" s="101"/>
+      <c r="AB52" s="100"/>
+      <c r="AC52" s="101"/>
     </row>
     <row r="53" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="D53" s="88"/>
-      <c r="E53" s="89"/>
-      <c r="F53" s="89"/>
-      <c r="G53" s="89"/>
-      <c r="H53" s="89"/>
-      <c r="I53" s="90"/>
-      <c r="J53" s="151"/>
-      <c r="K53" s="152"/>
+      <c r="D53" s="77"/>
+      <c r="E53" s="78"/>
+      <c r="F53" s="78"/>
+      <c r="G53" s="78"/>
+      <c r="H53" s="78"/>
+      <c r="I53" s="79"/>
+      <c r="J53" s="82"/>
+      <c r="K53" s="83"/>
       <c r="L53" s="86"/>
       <c r="M53" s="87"/>
       <c r="N53" s="86"/>
       <c r="O53" s="87"/>
-      <c r="P53" s="190"/>
-      <c r="Q53" s="191"/>
-      <c r="R53" s="191"/>
-      <c r="S53" s="192"/>
-      <c r="T53" s="102"/>
-      <c r="U53" s="103"/>
-      <c r="V53" s="103"/>
-      <c r="W53" s="104"/>
-      <c r="X53" s="107"/>
-      <c r="Y53" s="108"/>
-      <c r="Z53" s="107"/>
-      <c r="AA53" s="108"/>
-      <c r="AB53" s="107"/>
-      <c r="AC53" s="108"/>
+      <c r="P53" s="91"/>
+      <c r="Q53" s="92"/>
+      <c r="R53" s="92"/>
+      <c r="S53" s="93"/>
+      <c r="T53" s="97"/>
+      <c r="U53" s="98"/>
+      <c r="V53" s="98"/>
+      <c r="W53" s="99"/>
+      <c r="X53" s="102"/>
+      <c r="Y53" s="103"/>
+      <c r="Z53" s="102"/>
+      <c r="AA53" s="103"/>
+      <c r="AB53" s="102"/>
+      <c r="AC53" s="103"/>
     </row>
     <row r="54" spans="2:29" x14ac:dyDescent="0.3">
       <c r="D54" s="51"/>
@@ -7618,134 +7618,19 @@
     </row>
   </sheetData>
   <mergeCells count="165">
-    <mergeCell ref="D52:I53"/>
-    <mergeCell ref="J52:K53"/>
-    <mergeCell ref="L52:M53"/>
-    <mergeCell ref="N52:O53"/>
-    <mergeCell ref="P52:S53"/>
-    <mergeCell ref="T52:W53"/>
-    <mergeCell ref="X52:Y53"/>
-    <mergeCell ref="Z52:AA53"/>
-    <mergeCell ref="AB52:AC53"/>
-    <mergeCell ref="D49:I51"/>
-    <mergeCell ref="J49:K51"/>
-    <mergeCell ref="L49:M51"/>
-    <mergeCell ref="N49:O51"/>
-    <mergeCell ref="P49:S51"/>
-    <mergeCell ref="T49:W51"/>
-    <mergeCell ref="X49:Y51"/>
-    <mergeCell ref="Z49:AA51"/>
-    <mergeCell ref="J34:K35"/>
-    <mergeCell ref="P34:S35"/>
-    <mergeCell ref="D36:I38"/>
-    <mergeCell ref="J36:K38"/>
-    <mergeCell ref="P36:S38"/>
-    <mergeCell ref="J39:K40"/>
-    <mergeCell ref="J13:K15"/>
-    <mergeCell ref="L13:M15"/>
-    <mergeCell ref="N13:O15"/>
-    <mergeCell ref="B6:C25"/>
-    <mergeCell ref="J22:K23"/>
-    <mergeCell ref="J24:K25"/>
-    <mergeCell ref="L26:M27"/>
-    <mergeCell ref="N26:O27"/>
-    <mergeCell ref="B26:C40"/>
-    <mergeCell ref="B41:C52"/>
-    <mergeCell ref="N28:O29"/>
-    <mergeCell ref="P28:S29"/>
-    <mergeCell ref="L32:M33"/>
-    <mergeCell ref="J26:K27"/>
-    <mergeCell ref="P26:S27"/>
-    <mergeCell ref="D39:I40"/>
-    <mergeCell ref="J41:K42"/>
-    <mergeCell ref="D20:I21"/>
-    <mergeCell ref="D22:I23"/>
-    <mergeCell ref="J28:K29"/>
-    <mergeCell ref="J30:K31"/>
-    <mergeCell ref="J32:K33"/>
-    <mergeCell ref="J20:K21"/>
-    <mergeCell ref="N32:O33"/>
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="N20:O21"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D18:I19"/>
-    <mergeCell ref="J16:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L7:M8"/>
-    <mergeCell ref="N7:O8"/>
-    <mergeCell ref="P13:S15"/>
-    <mergeCell ref="D9:I12"/>
-    <mergeCell ref="J9:K12"/>
-    <mergeCell ref="P9:S12"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I8"/>
-    <mergeCell ref="J6:K8"/>
-    <mergeCell ref="D13:I15"/>
-    <mergeCell ref="D16:I17"/>
-    <mergeCell ref="P16:S17"/>
-    <mergeCell ref="P18:S19"/>
-    <mergeCell ref="D24:I25"/>
-    <mergeCell ref="D28:I29"/>
-    <mergeCell ref="D30:I31"/>
-    <mergeCell ref="D32:I33"/>
-    <mergeCell ref="D34:I35"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="X7:Y8"/>
-    <mergeCell ref="Z7:AA8"/>
-    <mergeCell ref="X16:Y17"/>
-    <mergeCell ref="Z16:AA17"/>
-    <mergeCell ref="T9:W12"/>
-    <mergeCell ref="X26:Y27"/>
-    <mergeCell ref="Z26:AA27"/>
-    <mergeCell ref="X32:Y33"/>
-    <mergeCell ref="Z32:AA33"/>
-    <mergeCell ref="L9:M12"/>
-    <mergeCell ref="N9:O12"/>
-    <mergeCell ref="L16:M17"/>
-    <mergeCell ref="N16:O17"/>
-    <mergeCell ref="P30:S31"/>
-    <mergeCell ref="P20:S21"/>
-    <mergeCell ref="D26:I27"/>
-    <mergeCell ref="H2:U2"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="T6:W8"/>
-    <mergeCell ref="H4:U4"/>
-    <mergeCell ref="AB16:AC17"/>
-    <mergeCell ref="X18:Y19"/>
-    <mergeCell ref="Z18:AA19"/>
-    <mergeCell ref="AB18:AC19"/>
-    <mergeCell ref="AB20:AC21"/>
-    <mergeCell ref="Z20:AA21"/>
-    <mergeCell ref="AB7:AC8"/>
-    <mergeCell ref="X9:Y12"/>
-    <mergeCell ref="Z9:AA12"/>
-    <mergeCell ref="AB9:AC12"/>
-    <mergeCell ref="X13:Y15"/>
-    <mergeCell ref="Z13:AA15"/>
-    <mergeCell ref="AB13:AC15"/>
-    <mergeCell ref="X20:Y21"/>
-    <mergeCell ref="AB26:AC27"/>
-    <mergeCell ref="AB28:AC29"/>
-    <mergeCell ref="Z28:AA29"/>
-    <mergeCell ref="X28:Y29"/>
-    <mergeCell ref="X22:Y23"/>
-    <mergeCell ref="Z22:AA23"/>
-    <mergeCell ref="AB22:AC23"/>
-    <mergeCell ref="AB24:AC25"/>
-    <mergeCell ref="Z24:AA25"/>
-    <mergeCell ref="X24:Y25"/>
+    <mergeCell ref="AB43:AC46"/>
+    <mergeCell ref="T43:W46"/>
+    <mergeCell ref="P41:S42"/>
+    <mergeCell ref="P43:S46"/>
+    <mergeCell ref="L28:M29"/>
+    <mergeCell ref="D47:I48"/>
+    <mergeCell ref="J47:K48"/>
+    <mergeCell ref="L47:M48"/>
+    <mergeCell ref="N47:O48"/>
+    <mergeCell ref="D41:I42"/>
+    <mergeCell ref="J43:K46"/>
+    <mergeCell ref="L43:M46"/>
+    <mergeCell ref="D43:I46"/>
     <mergeCell ref="AB32:AC33"/>
     <mergeCell ref="AB34:AC35"/>
     <mergeCell ref="Z34:AA35"/>
@@ -7770,19 +7655,134 @@
     <mergeCell ref="X39:Y40"/>
     <mergeCell ref="X41:Y42"/>
     <mergeCell ref="Z41:AA42"/>
-    <mergeCell ref="AB43:AC46"/>
-    <mergeCell ref="T43:W46"/>
-    <mergeCell ref="P41:S42"/>
-    <mergeCell ref="P43:S46"/>
-    <mergeCell ref="L28:M29"/>
-    <mergeCell ref="D47:I48"/>
-    <mergeCell ref="J47:K48"/>
-    <mergeCell ref="L47:M48"/>
-    <mergeCell ref="N47:O48"/>
-    <mergeCell ref="D41:I42"/>
-    <mergeCell ref="J43:K46"/>
-    <mergeCell ref="L43:M46"/>
-    <mergeCell ref="D43:I46"/>
+    <mergeCell ref="AB26:AC27"/>
+    <mergeCell ref="AB28:AC29"/>
+    <mergeCell ref="Z28:AA29"/>
+    <mergeCell ref="X28:Y29"/>
+    <mergeCell ref="X22:Y23"/>
+    <mergeCell ref="Z22:AA23"/>
+    <mergeCell ref="AB22:AC23"/>
+    <mergeCell ref="AB24:AC25"/>
+    <mergeCell ref="Z24:AA25"/>
+    <mergeCell ref="X24:Y25"/>
+    <mergeCell ref="AB16:AC17"/>
+    <mergeCell ref="X18:Y19"/>
+    <mergeCell ref="Z18:AA19"/>
+    <mergeCell ref="AB18:AC19"/>
+    <mergeCell ref="AB20:AC21"/>
+    <mergeCell ref="Z20:AA21"/>
+    <mergeCell ref="AB7:AC8"/>
+    <mergeCell ref="X9:Y12"/>
+    <mergeCell ref="Z9:AA12"/>
+    <mergeCell ref="AB9:AC12"/>
+    <mergeCell ref="X13:Y15"/>
+    <mergeCell ref="Z13:AA15"/>
+    <mergeCell ref="AB13:AC15"/>
+    <mergeCell ref="X20:Y21"/>
+    <mergeCell ref="H2:U2"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="T6:W8"/>
+    <mergeCell ref="H4:U4"/>
+    <mergeCell ref="X32:Y33"/>
+    <mergeCell ref="Z32:AA33"/>
+    <mergeCell ref="L9:M12"/>
+    <mergeCell ref="N9:O12"/>
+    <mergeCell ref="L16:M17"/>
+    <mergeCell ref="N16:O17"/>
+    <mergeCell ref="P30:S31"/>
+    <mergeCell ref="P20:S21"/>
+    <mergeCell ref="D26:I27"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="X7:Y8"/>
+    <mergeCell ref="Z7:AA8"/>
+    <mergeCell ref="X16:Y17"/>
+    <mergeCell ref="Z16:AA17"/>
+    <mergeCell ref="T9:W12"/>
+    <mergeCell ref="X26:Y27"/>
+    <mergeCell ref="Z26:AA27"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D18:I19"/>
+    <mergeCell ref="J16:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L7:M8"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="P13:S15"/>
+    <mergeCell ref="D9:I12"/>
+    <mergeCell ref="J9:K12"/>
+    <mergeCell ref="P9:S12"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I8"/>
+    <mergeCell ref="J6:K8"/>
+    <mergeCell ref="D13:I15"/>
+    <mergeCell ref="D16:I17"/>
+    <mergeCell ref="P16:S17"/>
+    <mergeCell ref="P18:S19"/>
+    <mergeCell ref="B41:C52"/>
+    <mergeCell ref="N28:O29"/>
+    <mergeCell ref="P28:S29"/>
+    <mergeCell ref="L32:M33"/>
+    <mergeCell ref="J26:K27"/>
+    <mergeCell ref="P26:S27"/>
+    <mergeCell ref="D39:I40"/>
+    <mergeCell ref="J41:K42"/>
+    <mergeCell ref="D20:I21"/>
+    <mergeCell ref="D22:I23"/>
+    <mergeCell ref="J28:K29"/>
+    <mergeCell ref="J30:K31"/>
+    <mergeCell ref="J32:K33"/>
+    <mergeCell ref="J20:K21"/>
+    <mergeCell ref="N32:O33"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="N20:O21"/>
+    <mergeCell ref="D24:I25"/>
+    <mergeCell ref="D28:I29"/>
+    <mergeCell ref="D30:I31"/>
+    <mergeCell ref="D32:I33"/>
+    <mergeCell ref="D34:I35"/>
+    <mergeCell ref="J13:K15"/>
+    <mergeCell ref="L13:M15"/>
+    <mergeCell ref="N13:O15"/>
+    <mergeCell ref="B6:C25"/>
+    <mergeCell ref="J22:K23"/>
+    <mergeCell ref="J24:K25"/>
+    <mergeCell ref="L26:M27"/>
+    <mergeCell ref="N26:O27"/>
+    <mergeCell ref="B26:C40"/>
+    <mergeCell ref="D49:I51"/>
+    <mergeCell ref="J49:K51"/>
+    <mergeCell ref="L49:M51"/>
+    <mergeCell ref="N49:O51"/>
+    <mergeCell ref="P49:S51"/>
+    <mergeCell ref="T49:W51"/>
+    <mergeCell ref="X49:Y51"/>
+    <mergeCell ref="Z49:AA51"/>
+    <mergeCell ref="J34:K35"/>
+    <mergeCell ref="P34:S35"/>
+    <mergeCell ref="D36:I38"/>
+    <mergeCell ref="J36:K38"/>
+    <mergeCell ref="P36:S38"/>
+    <mergeCell ref="J39:K40"/>
+    <mergeCell ref="D52:I53"/>
+    <mergeCell ref="J52:K53"/>
+    <mergeCell ref="L52:M53"/>
+    <mergeCell ref="N52:O53"/>
+    <mergeCell ref="P52:S53"/>
+    <mergeCell ref="T52:W53"/>
+    <mergeCell ref="X52:Y53"/>
+    <mergeCell ref="Z52:AA53"/>
+    <mergeCell ref="AB52:AC53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>